<commit_message>
csv from first sandbox
</commit_message>
<xml_diff>
--- a/Writeups/Notes/Exp.1_Master.xlsx
+++ b/Writeups/Notes/Exp.1_Master.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\Documents\SI.SP\Writeups\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\Documents\SI.SP\writeups\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D970A416-986D-45F0-938A-901130FC6210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2570283B-114A-4D3C-8EEC-32AC3FC3D8F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{6F4FE53E-24C5-4985-9E6F-6A265A63BA90}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{6F4FE53E-24C5-4985-9E6F-6A265A63BA90}"/>
   </bookViews>
   <sheets>
     <sheet name="Exposure Phase" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,10 @@
     <sheet name="Filler Trials" sheetId="2" r:id="rId3"/>
     <sheet name="Test Phase" sheetId="3" r:id="rId4"/>
     <sheet name="Design Diagram" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="227">
   <si>
     <t>Critical Items</t>
   </si>
@@ -965,9 +966,6 @@
     </r>
   </si>
   <si>
-    <t>1 Block with 80 Randomized Trials</t>
-  </si>
-  <si>
     <t>12 Blocks with 72 Total Trials</t>
   </si>
   <si>
@@ -1177,12 +1175,93 @@
   <si>
     <t>Attend: Male, Left</t>
   </si>
+  <si>
+    <t>10 Blocks with 80 Total Trials</t>
+  </si>
+  <si>
+    <t>Block</t>
+  </si>
+  <si>
+    <t>Exposure</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>6 trials per block:</t>
+  </si>
+  <si>
+    <t>2 critical</t>
+  </si>
+  <si>
+    <t>1 Shifted</t>
+  </si>
+  <si>
+    <t>8 trials per block:</t>
+  </si>
+  <si>
+    <t>6 Filler</t>
+  </si>
+  <si>
+    <t>2 Set C</t>
+  </si>
+  <si>
+    <t>2 Set B</t>
+  </si>
+  <si>
+    <t>2 Set A</t>
+  </si>
+  <si>
+    <t>word</t>
+  </si>
+  <si>
+    <t>nonword</t>
+  </si>
+  <si>
+    <t>[Ear A]</t>
+  </si>
+  <si>
+    <t>[Ear B]</t>
+  </si>
+  <si>
+    <t>1 Ushifted</t>
+  </si>
+  <si>
+    <t>80 total trials</t>
+  </si>
+  <si>
+    <t>72 total trials</t>
+  </si>
+  <si>
+    <t>6 unique asi-ashi tokens</t>
+  </si>
+  <si>
+    <t>one talker per block</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">talker switches </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Sylfaen"/>
+        <family val="1"/>
+      </rPr>
+      <t>every two blocks</t>
+    </r>
+  </si>
+  <si>
+    <t>asi-ashi</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1277,6 +1356,19 @@
     </font>
     <font>
       <sz val="20"/>
+      <color theme="1"/>
+      <name val="Sylfaen"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Sylfaen"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Sylfaen"/>
       <family val="1"/>
@@ -2279,7 +2371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="310">
+  <cellXfs count="321">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2917,117 +3009,168 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="180"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="44" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3037,75 +3180,49 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="44" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="44" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3114,16 +3231,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFB5CC76"/>
+      <color rgb="FFB2E3FC"/>
       <color rgb="FF77CEF9"/>
       <color rgb="FFFFBE5F"/>
-      <color rgb="FFB5CC76"/>
       <color rgb="FFD1DFA9"/>
       <color rgb="FFECFFCD"/>
       <color rgb="FFEDF2F9"/>
       <color rgb="FFE9EEF7"/>
       <color rgb="FFE3E9F5"/>
       <color rgb="FFFFDAA3"/>
-      <color rgb="FFB2E3FC"/>
     </mruColors>
   </colors>
   <extLst>
@@ -4424,7 +4541,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -4771,7 +4888,7 @@
   </sheetPr>
   <dimension ref="B1:AM718"/>
   <sheetViews>
-    <sheetView zoomScale="65" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A21" zoomScale="65" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AK18" sqref="AK18"/>
     </sheetView>
   </sheetViews>
@@ -4822,7 +4939,7 @@
       <c r="G2" s="237"/>
       <c r="H2" s="4"/>
       <c r="I2" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="6" t="s">
@@ -4901,7 +5018,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="242"/>
       <c r="M4" s="242" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N4" s="124"/>
       <c r="O4" s="244" t="s">
@@ -4925,7 +5042,7 @@
       <c r="AA4" s="244"/>
       <c r="AB4" s="244"/>
       <c r="AI4" s="234" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AJ4" s="234"/>
       <c r="AK4" s="234"/>
@@ -12317,8 +12434,8 @@
   </sheetPr>
   <dimension ref="B2:AO41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="73" zoomScaleNormal="144" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView showGridLines="0" zoomScale="73" zoomScaleNormal="144" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6328125" defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -12340,11 +12457,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="V2" s="307" t="s">
+      <c r="V2" s="249" t="s">
         <v>75</v>
       </c>
-      <c r="W2" s="307"/>
-      <c r="X2" s="307"/>
+      <c r="W2" s="249"/>
+      <c r="X2" s="249"/>
     </row>
     <row r="3" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="161" t="s">
@@ -12353,11 +12470,11 @@
       <c r="C3" s="162" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="261" t="s">
+      <c r="D3" s="247" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="247"/>
-      <c r="F3" s="247"/>
+      <c r="E3" s="248"/>
+      <c r="F3" s="248"/>
       <c r="G3" s="64"/>
       <c r="H3" s="161" t="s">
         <v>71</v>
@@ -12365,40 +12482,40 @@
       <c r="I3" s="162" t="s">
         <v>72</v>
       </c>
-      <c r="J3" s="261" t="s">
+      <c r="J3" s="247" t="s">
         <v>74</v>
       </c>
-      <c r="K3" s="247"/>
-      <c r="L3" s="247"/>
-      <c r="N3" s="276" t="s">
+      <c r="K3" s="248"/>
+      <c r="L3" s="248"/>
+      <c r="N3" s="249" t="s">
         <v>75</v>
       </c>
-      <c r="O3" s="276"/>
+      <c r="O3" s="249"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="276" t="s">
+      <c r="Q3" s="249" t="s">
         <v>76</v>
       </c>
-      <c r="R3" s="276"/>
+      <c r="R3" s="249"/>
       <c r="S3" s="1"/>
-      <c r="V3" s="308"/>
-      <c r="W3" s="308"/>
-      <c r="X3" s="308"/>
-      <c r="AB3" s="293" t="s">
+      <c r="V3" s="271"/>
+      <c r="W3" s="271"/>
+      <c r="X3" s="271"/>
+      <c r="AB3" s="269" t="s">
         <v>151</v>
       </c>
-      <c r="AC3" s="293"/>
-      <c r="AD3" s="293"/>
-      <c r="AE3" s="293"/>
-      <c r="AF3" s="293"/>
-      <c r="AG3" s="293"/>
-      <c r="AH3" s="293"/>
-      <c r="AI3" s="293"/>
-      <c r="AJ3" s="293"/>
-      <c r="AL3" s="293" t="s">
+      <c r="AC3" s="269"/>
+      <c r="AD3" s="269"/>
+      <c r="AE3" s="269"/>
+      <c r="AF3" s="269"/>
+      <c r="AG3" s="269"/>
+      <c r="AH3" s="269"/>
+      <c r="AI3" s="269"/>
+      <c r="AJ3" s="269"/>
+      <c r="AL3" s="269" t="s">
         <v>32</v>
       </c>
-      <c r="AM3" s="293"/>
-      <c r="AN3" s="293"/>
+      <c r="AM3" s="269"/>
+      <c r="AN3" s="269"/>
     </row>
     <row r="4" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="81" t="s">
@@ -12407,9 +12524,9 @@
       <c r="C4" s="77" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="261"/>
-      <c r="E4" s="247"/>
-      <c r="F4" s="247"/>
+      <c r="D4" s="247"/>
+      <c r="E4" s="248"/>
+      <c r="F4" s="248"/>
       <c r="G4" s="64"/>
       <c r="H4" s="81" t="s">
         <v>77</v>
@@ -12417,9 +12534,9 @@
       <c r="I4" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="J4" s="261"/>
-      <c r="K4" s="247"/>
-      <c r="L4" s="247"/>
+      <c r="J4" s="247"/>
+      <c r="K4" s="248"/>
+      <c r="L4" s="248"/>
       <c r="N4" s="71" t="s">
         <v>71</v>
       </c>
@@ -12437,22 +12554,22 @@
       <c r="V4" s="98"/>
       <c r="W4" s="99"/>
       <c r="X4" s="100"/>
-      <c r="AB4" s="301" t="s">
-        <v>195</v>
-      </c>
-      <c r="AC4" s="301"/>
-      <c r="AD4" s="301"/>
-      <c r="AE4" s="301"/>
-      <c r="AF4" s="301"/>
-      <c r="AG4" s="301"/>
-      <c r="AH4" s="301"/>
-      <c r="AI4" s="301"/>
-      <c r="AJ4" s="301"/>
+      <c r="AB4" s="251" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC4" s="251"/>
+      <c r="AD4" s="251"/>
+      <c r="AE4" s="251"/>
+      <c r="AF4" s="251"/>
+      <c r="AG4" s="251"/>
+      <c r="AH4" s="251"/>
+      <c r="AI4" s="251"/>
+      <c r="AJ4" s="251"/>
       <c r="AL4" s="234" t="s">
-        <v>199</v>
-      </c>
-      <c r="AM4" s="251"/>
-      <c r="AN4" s="251"/>
+        <v>198</v>
+      </c>
+      <c r="AM4" s="264"/>
+      <c r="AN4" s="264"/>
     </row>
     <row r="5" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="78" t="s">
@@ -12461,11 +12578,11 @@
       <c r="C5" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="D5" s="261" t="s">
+      <c r="D5" s="247" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="247"/>
-      <c r="F5" s="247"/>
+      <c r="E5" s="248"/>
+      <c r="F5" s="248"/>
       <c r="G5" s="64"/>
       <c r="H5" s="78" t="s">
         <v>82</v>
@@ -12473,9 +12590,9 @@
       <c r="I5" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="J5" s="261"/>
-      <c r="K5" s="247"/>
-      <c r="L5" s="247"/>
+      <c r="J5" s="247"/>
+      <c r="K5" s="248"/>
+      <c r="L5" s="248"/>
       <c r="N5" s="135" t="s">
         <v>143</v>
       </c>
@@ -12490,7 +12607,7 @@
         <v>143</v>
       </c>
       <c r="S5" s="1"/>
-      <c r="T5" s="303" t="s">
+      <c r="T5" s="265" t="s">
         <v>143</v>
       </c>
       <c r="U5" s="101"/>
@@ -12502,21 +12619,21 @@
         <v>79</v>
       </c>
       <c r="Y5" s="104"/>
-      <c r="Z5" s="305" t="s">
+      <c r="Z5" s="267" t="s">
         <v>144</v>
       </c>
-      <c r="AB5" s="301"/>
-      <c r="AC5" s="301"/>
-      <c r="AD5" s="301"/>
-      <c r="AE5" s="301"/>
-      <c r="AF5" s="301"/>
-      <c r="AG5" s="301"/>
-      <c r="AH5" s="301"/>
-      <c r="AI5" s="301"/>
-      <c r="AJ5" s="301"/>
-      <c r="AL5" s="251"/>
-      <c r="AM5" s="251"/>
-      <c r="AN5" s="251"/>
+      <c r="AB5" s="251"/>
+      <c r="AC5" s="251"/>
+      <c r="AD5" s="251"/>
+      <c r="AE5" s="251"/>
+      <c r="AF5" s="251"/>
+      <c r="AG5" s="251"/>
+      <c r="AH5" s="251"/>
+      <c r="AI5" s="251"/>
+      <c r="AJ5" s="251"/>
+      <c r="AL5" s="264"/>
+      <c r="AM5" s="264"/>
+      <c r="AN5" s="264"/>
       <c r="AO5" s="1"/>
     </row>
     <row r="6" spans="2:41" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -12536,9 +12653,9 @@
       <c r="I6" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="J6" s="261"/>
-      <c r="K6" s="247"/>
-      <c r="L6" s="247"/>
+      <c r="J6" s="247"/>
+      <c r="K6" s="248"/>
+      <c r="L6" s="248"/>
       <c r="N6" s="102" t="s">
         <v>77</v>
       </c>
@@ -12552,7 +12669,7 @@
         <v>80</v>
       </c>
       <c r="S6" s="1"/>
-      <c r="T6" s="304"/>
+      <c r="T6" s="266"/>
       <c r="U6" s="105"/>
       <c r="V6" s="65" t="s">
         <v>86</v>
@@ -12562,7 +12679,7 @@
         <v>96</v>
       </c>
       <c r="Y6" s="107"/>
-      <c r="Z6" s="305"/>
+      <c r="Z6" s="267"/>
       <c r="AB6" s="152" t="s">
         <v>81</v>
       </c>
@@ -12588,9 +12705,9 @@
       <c r="AJ6" s="150" t="s">
         <v>98</v>
       </c>
-      <c r="AL6" s="251"/>
-      <c r="AM6" s="251"/>
-      <c r="AN6" s="251"/>
+      <c r="AL6" s="264"/>
+      <c r="AM6" s="264"/>
+      <c r="AN6" s="264"/>
       <c r="AO6" s="1"/>
     </row>
     <row r="7" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -12600,11 +12717,11 @@
       <c r="C7" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="261" t="s">
+      <c r="D7" s="247" t="s">
         <v>94</v>
       </c>
-      <c r="E7" s="247"/>
-      <c r="F7" s="247"/>
+      <c r="E7" s="248"/>
+      <c r="F7" s="248"/>
       <c r="G7" s="64"/>
       <c r="H7" s="78" t="s">
         <v>93</v>
@@ -12612,9 +12729,9 @@
       <c r="I7" s="82" t="s">
         <v>95</v>
       </c>
-      <c r="J7" s="261"/>
-      <c r="K7" s="247"/>
-      <c r="L7" s="247"/>
+      <c r="J7" s="247"/>
+      <c r="K7" s="248"/>
+      <c r="L7" s="248"/>
       <c r="N7" s="65" t="s">
         <v>86</v>
       </c>
@@ -12628,7 +12745,7 @@
         <v>85</v>
       </c>
       <c r="S7" s="1"/>
-      <c r="T7" s="304"/>
+      <c r="T7" s="266"/>
       <c r="U7" s="105"/>
       <c r="V7" s="88" t="s">
         <v>88</v>
@@ -12638,10 +12755,10 @@
         <v>90</v>
       </c>
       <c r="Y7" s="107"/>
-      <c r="Z7" s="305"/>
+      <c r="Z7" s="267"/>
       <c r="AA7" s="123"/>
       <c r="AB7" s="214" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AC7" s="106" t="s">
         <v>87</v>
@@ -12650,11 +12767,11 @@
         <v>87</v>
       </c>
       <c r="AE7" s="151" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AF7" s="1"/>
       <c r="AG7" s="153" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AH7" s="145" t="s">
         <v>87</v>
@@ -12663,11 +12780,11 @@
         <v>87</v>
       </c>
       <c r="AJ7" s="215" t="s">
-        <v>194</v>
-      </c>
-      <c r="AL7" s="251"/>
-      <c r="AM7" s="251"/>
-      <c r="AN7" s="251"/>
+        <v>193</v>
+      </c>
+      <c r="AL7" s="264"/>
+      <c r="AM7" s="264"/>
+      <c r="AN7" s="264"/>
       <c r="AO7" s="1"/>
     </row>
     <row r="8" spans="2:41" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -12677,9 +12794,9 @@
       <c r="C8" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="D8" s="261"/>
-      <c r="E8" s="247"/>
-      <c r="F8" s="247"/>
+      <c r="D8" s="247"/>
+      <c r="E8" s="248"/>
+      <c r="F8" s="248"/>
       <c r="G8" s="27"/>
       <c r="H8" s="83" t="s">
         <v>99</v>
@@ -12690,8 +12807,8 @@
       <c r="J8" s="262" t="s">
         <v>102</v>
       </c>
-      <c r="K8" s="249"/>
-      <c r="L8" s="249"/>
+      <c r="K8" s="263"/>
+      <c r="L8" s="263"/>
       <c r="N8" s="88" t="s">
         <v>88</v>
       </c>
@@ -12705,7 +12822,7 @@
         <v>92</v>
       </c>
       <c r="S8" s="1"/>
-      <c r="T8" s="304"/>
+      <c r="T8" s="266"/>
       <c r="U8" s="105"/>
       <c r="V8" s="65" t="s">
         <v>97</v>
@@ -12715,28 +12832,28 @@
         <v>107</v>
       </c>
       <c r="Y8" s="107"/>
-      <c r="Z8" s="305"/>
+      <c r="Z8" s="267"/>
       <c r="AA8" s="123"/>
       <c r="AB8" s="147" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AC8" s="144"/>
       <c r="AD8" s="117"/>
       <c r="AE8" s="217" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AF8" s="1"/>
       <c r="AG8" s="218" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AH8" s="106"/>
       <c r="AI8" s="142"/>
       <c r="AJ8" s="146" t="s">
-        <v>194</v>
-      </c>
-      <c r="AL8" s="251"/>
-      <c r="AM8" s="251"/>
-      <c r="AN8" s="251"/>
+        <v>193</v>
+      </c>
+      <c r="AL8" s="264"/>
+      <c r="AM8" s="264"/>
+      <c r="AN8" s="264"/>
       <c r="AO8" s="1"/>
     </row>
     <row r="9" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -12746,9 +12863,9 @@
       <c r="C9" s="82" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="261"/>
-      <c r="E9" s="247"/>
-      <c r="F9" s="247"/>
+      <c r="D9" s="247"/>
+      <c r="E9" s="248"/>
+      <c r="F9" s="248"/>
       <c r="G9" s="64"/>
       <c r="H9" s="78" t="s">
         <v>105</v>
@@ -12769,17 +12886,17 @@
         <v>95</v>
       </c>
       <c r="S9" s="1"/>
-      <c r="T9" s="304"/>
+      <c r="T9" s="266"/>
       <c r="U9" s="105"/>
       <c r="V9" s="88" t="s">
         <v>99</v>
       </c>
       <c r="W9" s="106"/>
       <c r="X9" s="90" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="Y9" s="107"/>
-      <c r="Z9" s="305"/>
+      <c r="Z9" s="267"/>
       <c r="AA9" s="123"/>
       <c r="AB9" s="148" t="s">
         <v>98</v>
@@ -12806,9 +12923,9 @@
       <c r="AJ9" s="149" t="s">
         <v>81</v>
       </c>
-      <c r="AL9" s="251"/>
-      <c r="AM9" s="251"/>
-      <c r="AN9" s="251"/>
+      <c r="AL9" s="264"/>
+      <c r="AM9" s="264"/>
+      <c r="AN9" s="264"/>
       <c r="AO9" s="1"/>
     </row>
     <row r="10" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -12818,9 +12935,9 @@
       <c r="C10" s="79" t="s">
         <v>110</v>
       </c>
-      <c r="D10" s="261"/>
-      <c r="E10" s="247"/>
-      <c r="F10" s="247"/>
+      <c r="D10" s="247"/>
+      <c r="E10" s="248"/>
+      <c r="F10" s="248"/>
       <c r="G10" s="64"/>
       <c r="H10" s="83" t="s">
         <v>109</v>
@@ -12828,16 +12945,16 @@
       <c r="I10" s="79" t="s">
         <v>78</v>
       </c>
-      <c r="J10" s="261" t="s">
+      <c r="J10" s="247" t="s">
         <v>111</v>
       </c>
-      <c r="K10" s="247"/>
-      <c r="L10" s="247"/>
+      <c r="K10" s="248"/>
+      <c r="L10" s="248"/>
       <c r="N10" s="88" t="s">
         <v>99</v>
       </c>
       <c r="O10" s="130" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="Q10" s="86" t="s">
         <v>112</v>
@@ -12846,7 +12963,7 @@
         <v>104</v>
       </c>
       <c r="S10" s="1"/>
-      <c r="T10" s="304"/>
+      <c r="T10" s="266"/>
       <c r="U10" s="105"/>
       <c r="V10" s="65" t="s">
         <v>108</v>
@@ -12856,7 +12973,7 @@
         <v>115</v>
       </c>
       <c r="Y10" s="107"/>
-      <c r="Z10" s="305"/>
+      <c r="Z10" s="267"/>
       <c r="AA10" s="123"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
@@ -12867,9 +12984,9 @@
       <c r="AH10" s="1"/>
       <c r="AI10" s="1"/>
       <c r="AJ10" s="1"/>
-      <c r="AL10" s="251"/>
-      <c r="AM10" s="251"/>
-      <c r="AN10" s="251"/>
+      <c r="AL10" s="264"/>
+      <c r="AM10" s="264"/>
+      <c r="AN10" s="264"/>
       <c r="AO10" s="1"/>
     </row>
     <row r="11" spans="2:41" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -12879,9 +12996,9 @@
       <c r="C11" s="82" t="s">
         <v>113</v>
       </c>
-      <c r="D11" s="261"/>
-      <c r="E11" s="247"/>
-      <c r="F11" s="247"/>
+      <c r="D11" s="247"/>
+      <c r="E11" s="248"/>
+      <c r="F11" s="248"/>
       <c r="G11" s="64"/>
       <c r="H11" s="78" t="s">
         <v>114</v>
@@ -12889,9 +13006,9 @@
       <c r="I11" s="82" t="s">
         <v>110</v>
       </c>
-      <c r="J11" s="261"/>
-      <c r="K11" s="247"/>
-      <c r="L11" s="247"/>
+      <c r="J11" s="247"/>
+      <c r="K11" s="248"/>
+      <c r="L11" s="248"/>
       <c r="N11" s="65" t="s">
         <v>108</v>
       </c>
@@ -12905,7 +13022,7 @@
         <v>106</v>
       </c>
       <c r="S11" s="1"/>
-      <c r="T11" s="304"/>
+      <c r="T11" s="266"/>
       <c r="U11" s="105"/>
       <c r="V11" s="88" t="s">
         <v>109</v>
@@ -12915,7 +13032,7 @@
         <v>78</v>
       </c>
       <c r="Y11" s="107"/>
-      <c r="Z11" s="305"/>
+      <c r="Z11" s="267"/>
       <c r="AA11" s="123"/>
       <c r="AB11" s="152" t="s">
         <v>81</v>
@@ -12942,9 +13059,9 @@
       <c r="AJ11" s="150" t="s">
         <v>98</v>
       </c>
-      <c r="AL11" s="251"/>
-      <c r="AM11" s="251"/>
-      <c r="AN11" s="251"/>
+      <c r="AL11" s="264"/>
+      <c r="AM11" s="264"/>
+      <c r="AN11" s="264"/>
       <c r="AO11" s="1"/>
     </row>
     <row r="12" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -12954,9 +13071,9 @@
       <c r="C12" s="79" t="s">
         <v>115</v>
       </c>
-      <c r="D12" s="261"/>
-      <c r="E12" s="247"/>
-      <c r="F12" s="247"/>
+      <c r="D12" s="247"/>
+      <c r="E12" s="248"/>
+      <c r="F12" s="248"/>
       <c r="G12" s="64"/>
       <c r="H12" s="83" t="s">
         <v>117</v>
@@ -12964,9 +13081,9 @@
       <c r="I12" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="J12" s="261"/>
-      <c r="K12" s="247"/>
-      <c r="L12" s="247"/>
+      <c r="J12" s="247"/>
+      <c r="K12" s="248"/>
+      <c r="L12" s="248"/>
       <c r="N12" s="88" t="s">
         <v>109</v>
       </c>
@@ -12980,7 +13097,7 @@
         <v>113</v>
       </c>
       <c r="S12" s="1"/>
-      <c r="T12" s="304"/>
+      <c r="T12" s="266"/>
       <c r="U12" s="105"/>
       <c r="V12" s="65" t="s">
         <v>116</v>
@@ -12990,28 +13107,28 @@
         <v>89</v>
       </c>
       <c r="Y12" s="107"/>
-      <c r="Z12" s="305"/>
+      <c r="Z12" s="267"/>
       <c r="AA12" s="123"/>
       <c r="AB12" s="214" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AC12" s="106"/>
       <c r="AD12" s="143"/>
       <c r="AE12" s="151" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AF12" s="1"/>
       <c r="AG12" s="153" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AH12" s="145"/>
       <c r="AI12" s="117"/>
       <c r="AJ12" s="215" t="s">
-        <v>194</v>
-      </c>
-      <c r="AL12" s="251"/>
-      <c r="AM12" s="251"/>
-      <c r="AN12" s="251"/>
+        <v>193</v>
+      </c>
+      <c r="AL12" s="264"/>
+      <c r="AM12" s="264"/>
+      <c r="AN12" s="264"/>
       <c r="AO12" s="1"/>
     </row>
     <row r="13" spans="2:41" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -13021,9 +13138,9 @@
       <c r="C13" s="82" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="261"/>
-      <c r="E13" s="247"/>
-      <c r="F13" s="247"/>
+      <c r="D13" s="247"/>
+      <c r="E13" s="248"/>
+      <c r="F13" s="248"/>
       <c r="G13" s="64"/>
       <c r="H13" s="78" t="s">
         <v>120</v>
@@ -13031,9 +13148,9 @@
       <c r="I13" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="J13" s="261"/>
-      <c r="K13" s="247"/>
-      <c r="L13" s="247"/>
+      <c r="J13" s="247"/>
+      <c r="K13" s="248"/>
+      <c r="L13" s="248"/>
       <c r="N13" s="65" t="s">
         <v>116</v>
       </c>
@@ -13047,7 +13164,7 @@
         <v>110</v>
       </c>
       <c r="S13" s="1"/>
-      <c r="T13" s="304"/>
+      <c r="T13" s="266"/>
       <c r="U13" s="105"/>
       <c r="V13" s="88" t="s">
         <v>117</v>
@@ -13057,10 +13174,10 @@
         <v>100</v>
       </c>
       <c r="Y13" s="107"/>
-      <c r="Z13" s="305"/>
+      <c r="Z13" s="267"/>
       <c r="AA13" s="123"/>
       <c r="AB13" s="147" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AC13" s="144" t="s">
         <v>87</v>
@@ -13069,11 +13186,11 @@
         <v>87</v>
       </c>
       <c r="AE13" s="217" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AF13" s="1"/>
       <c r="AG13" s="218" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AH13" s="106" t="s">
         <v>87</v>
@@ -13082,7 +13199,7 @@
         <v>87</v>
       </c>
       <c r="AJ13" s="146" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AL13" s="21"/>
       <c r="AM13" s="21"/>
@@ -13096,9 +13213,9 @@
       <c r="C14" s="79" t="s">
         <v>119</v>
       </c>
-      <c r="D14" s="261"/>
-      <c r="E14" s="247"/>
-      <c r="F14" s="247"/>
+      <c r="D14" s="247"/>
+      <c r="E14" s="248"/>
+      <c r="F14" s="248"/>
       <c r="G14" s="64"/>
       <c r="H14" s="83" t="s">
         <v>91</v>
@@ -13106,9 +13223,9 @@
       <c r="I14" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="J14" s="261"/>
-      <c r="K14" s="247"/>
-      <c r="L14" s="247"/>
+      <c r="J14" s="247"/>
+      <c r="K14" s="248"/>
+      <c r="L14" s="248"/>
       <c r="N14" s="88" t="s">
         <v>117</v>
       </c>
@@ -13122,7 +13239,7 @@
         <v>119</v>
       </c>
       <c r="S14" s="1"/>
-      <c r="T14" s="304"/>
+      <c r="T14" s="266"/>
       <c r="U14" s="105"/>
       <c r="V14" s="69" t="s">
         <v>121</v>
@@ -13132,7 +13249,7 @@
         <v>123</v>
       </c>
       <c r="Y14" s="107"/>
-      <c r="Z14" s="305"/>
+      <c r="Z14" s="267"/>
       <c r="AA14" s="123"/>
       <c r="AB14" s="148" t="s">
         <v>98</v>
@@ -13167,9 +13284,9 @@
       <c r="C15" s="82" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="261"/>
-      <c r="E15" s="247"/>
-      <c r="F15" s="247"/>
+      <c r="D15" s="247"/>
+      <c r="E15" s="248"/>
+      <c r="F15" s="248"/>
       <c r="G15" s="64"/>
       <c r="H15" s="78" t="s">
         <v>86</v>
@@ -13177,9 +13294,9 @@
       <c r="I15" s="82" t="s">
         <v>96</v>
       </c>
-      <c r="J15" s="261"/>
-      <c r="K15" s="247"/>
-      <c r="L15" s="247"/>
+      <c r="J15" s="247"/>
+      <c r="K15" s="248"/>
+      <c r="L15" s="248"/>
       <c r="N15" s="69" t="s">
         <v>121</v>
       </c>
@@ -13193,13 +13310,13 @@
         <v>83</v>
       </c>
       <c r="S15" s="1"/>
-      <c r="T15" s="304"/>
+      <c r="T15" s="266"/>
       <c r="U15" s="108"/>
       <c r="V15" s="109"/>
       <c r="W15" s="110"/>
       <c r="X15" s="111"/>
       <c r="Y15" s="112"/>
-      <c r="Z15" s="305"/>
+      <c r="Z15" s="267"/>
       <c r="AL15" s="234" t="s">
         <v>126</v>
       </c>
@@ -13214,9 +13331,9 @@
       <c r="C16" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="D16" s="261"/>
-      <c r="E16" s="247"/>
-      <c r="F16" s="247"/>
+      <c r="D16" s="247"/>
+      <c r="E16" s="248"/>
+      <c r="F16" s="248"/>
       <c r="G16" s="64"/>
       <c r="H16" s="83" t="s">
         <v>103</v>
@@ -13224,27 +13341,27 @@
       <c r="I16" s="79" t="s">
         <v>92</v>
       </c>
-      <c r="J16" s="261"/>
-      <c r="K16" s="247"/>
-      <c r="L16" s="247"/>
-      <c r="T16" s="304"/>
+      <c r="J16" s="247"/>
+      <c r="K16" s="248"/>
+      <c r="L16" s="248"/>
+      <c r="T16" s="266"/>
       <c r="U16" s="105"/>
       <c r="V16" s="113"/>
       <c r="W16" s="114"/>
       <c r="X16" s="115"/>
       <c r="Y16" s="107"/>
-      <c r="Z16" s="305"/>
-      <c r="AB16" s="301" t="s">
-        <v>196</v>
-      </c>
-      <c r="AC16" s="301"/>
-      <c r="AD16" s="301"/>
-      <c r="AE16" s="301"/>
-      <c r="AF16" s="301"/>
-      <c r="AG16" s="301"/>
-      <c r="AH16" s="301"/>
-      <c r="AI16" s="301"/>
-      <c r="AJ16" s="301"/>
+      <c r="Z16" s="267"/>
+      <c r="AB16" s="251" t="s">
+        <v>195</v>
+      </c>
+      <c r="AC16" s="251"/>
+      <c r="AD16" s="251"/>
+      <c r="AE16" s="251"/>
+      <c r="AF16" s="251"/>
+      <c r="AG16" s="251"/>
+      <c r="AH16" s="251"/>
+      <c r="AI16" s="251"/>
+      <c r="AJ16" s="251"/>
       <c r="AL16" s="21"/>
       <c r="AM16" s="21"/>
       <c r="AN16" s="21"/>
@@ -13257,9 +13374,9 @@
       <c r="C17" s="82" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="261"/>
-      <c r="E17" s="247"/>
-      <c r="F17" s="247"/>
+      <c r="D17" s="247"/>
+      <c r="E17" s="248"/>
+      <c r="F17" s="248"/>
       <c r="G17" s="64"/>
       <c r="H17" s="78" t="s">
         <v>97</v>
@@ -13267,11 +13384,11 @@
       <c r="I17" s="82" t="s">
         <v>107</v>
       </c>
-      <c r="J17" s="261"/>
-      <c r="K17" s="247"/>
-      <c r="L17" s="247"/>
+      <c r="J17" s="247"/>
+      <c r="K17" s="248"/>
+      <c r="L17" s="248"/>
       <c r="S17" s="125"/>
-      <c r="T17" s="304"/>
+      <c r="T17" s="266"/>
       <c r="U17" s="105"/>
       <c r="V17" s="72" t="s">
         <v>80</v>
@@ -13281,17 +13398,17 @@
         <v>91</v>
       </c>
       <c r="Y17" s="107"/>
-      <c r="Z17" s="305"/>
+      <c r="Z17" s="267"/>
       <c r="AA17" s="123"/>
-      <c r="AB17" s="301"/>
-      <c r="AC17" s="301"/>
-      <c r="AD17" s="301"/>
-      <c r="AE17" s="301"/>
-      <c r="AF17" s="301"/>
-      <c r="AG17" s="301"/>
-      <c r="AH17" s="301"/>
-      <c r="AI17" s="301"/>
-      <c r="AJ17" s="301"/>
+      <c r="AB17" s="251"/>
+      <c r="AC17" s="251"/>
+      <c r="AD17" s="251"/>
+      <c r="AE17" s="251"/>
+      <c r="AF17" s="251"/>
+      <c r="AG17" s="251"/>
+      <c r="AH17" s="251"/>
+      <c r="AI17" s="251"/>
+      <c r="AJ17" s="251"/>
       <c r="AL17" s="234" t="s">
         <v>128</v>
       </c>
@@ -13306,9 +13423,9 @@
       <c r="C18" s="79" t="s">
         <v>125</v>
       </c>
-      <c r="D18" s="261"/>
-      <c r="E18" s="247"/>
-      <c r="F18" s="247"/>
+      <c r="D18" s="247"/>
+      <c r="E18" s="248"/>
+      <c r="F18" s="248"/>
       <c r="G18" s="64"/>
       <c r="H18" s="83" t="s">
         <v>112</v>
@@ -13316,21 +13433,21 @@
       <c r="I18" s="79" t="s">
         <v>104</v>
       </c>
-      <c r="J18" s="261"/>
-      <c r="K18" s="247"/>
-      <c r="L18" s="247"/>
+      <c r="J18" s="247"/>
+      <c r="K18" s="248"/>
+      <c r="L18" s="248"/>
       <c r="M18" s="73"/>
-      <c r="N18" s="301" t="s">
+      <c r="N18" s="251" t="s">
         <v>143</v>
       </c>
-      <c r="O18" s="301"/>
+      <c r="O18" s="251"/>
       <c r="P18" s="73"/>
-      <c r="Q18" s="302" t="s">
+      <c r="Q18" s="252" t="s">
         <v>144</v>
       </c>
-      <c r="R18" s="302"/>
+      <c r="R18" s="252"/>
       <c r="S18" s="125"/>
-      <c r="T18" s="304"/>
+      <c r="T18" s="266"/>
       <c r="U18" s="105"/>
       <c r="V18" s="88" t="s">
         <v>85</v>
@@ -13340,7 +13457,7 @@
         <v>82</v>
       </c>
       <c r="Y18" s="107"/>
-      <c r="Z18" s="305"/>
+      <c r="Z18" s="267"/>
       <c r="AA18" s="123"/>
       <c r="AB18" s="152" t="s">
         <v>98</v>
@@ -13381,9 +13498,9 @@
       <c r="C19" s="82" t="s">
         <v>106</v>
       </c>
-      <c r="D19" s="261"/>
-      <c r="E19" s="247"/>
-      <c r="F19" s="247"/>
+      <c r="D19" s="247"/>
+      <c r="E19" s="248"/>
+      <c r="F19" s="248"/>
       <c r="G19" s="64"/>
       <c r="H19" s="78" t="s">
         <v>108</v>
@@ -13391,9 +13508,9 @@
       <c r="I19" s="82" t="s">
         <v>115</v>
       </c>
-      <c r="J19" s="261"/>
-      <c r="K19" s="247"/>
-      <c r="L19" s="247"/>
+      <c r="J19" s="247"/>
+      <c r="K19" s="248"/>
+      <c r="L19" s="248"/>
       <c r="M19" s="21"/>
       <c r="N19" s="157" t="s">
         <v>71</v>
@@ -13409,7 +13526,7 @@
         <v>72</v>
       </c>
       <c r="S19" s="125"/>
-      <c r="T19" s="304"/>
+      <c r="T19" s="266"/>
       <c r="U19" s="105"/>
       <c r="V19" s="65" t="s">
         <v>92</v>
@@ -13419,10 +13536,10 @@
         <v>103</v>
       </c>
       <c r="Y19" s="107"/>
-      <c r="Z19" s="305"/>
+      <c r="Z19" s="267"/>
       <c r="AA19" s="123"/>
       <c r="AB19" s="214" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AC19" s="106" t="s">
         <v>87</v>
@@ -13431,11 +13548,11 @@
         <v>87</v>
       </c>
       <c r="AE19" s="151" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AF19" s="1"/>
       <c r="AG19" s="148" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AH19" s="145" t="s">
         <v>87</v>
@@ -13444,7 +13561,7 @@
         <v>87</v>
       </c>
       <c r="AJ19" s="217" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AL19" s="234" t="s">
         <v>133</v>
@@ -13460,9 +13577,9 @@
       <c r="C20" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="D20" s="261"/>
-      <c r="E20" s="247"/>
-      <c r="F20" s="247"/>
+      <c r="D20" s="247"/>
+      <c r="E20" s="248"/>
+      <c r="F20" s="248"/>
       <c r="G20" s="64"/>
       <c r="H20" s="83" t="s">
         <v>118</v>
@@ -13470,9 +13587,9 @@
       <c r="I20" s="79" t="s">
         <v>113</v>
       </c>
-      <c r="J20" s="261"/>
-      <c r="K20" s="247"/>
-      <c r="L20" s="247"/>
+      <c r="J20" s="247"/>
+      <c r="K20" s="248"/>
+      <c r="L20" s="248"/>
       <c r="M20" s="21"/>
       <c r="N20" s="95" t="s">
         <v>77</v>
@@ -13488,7 +13605,7 @@
         <v>79</v>
       </c>
       <c r="S20" s="125"/>
-      <c r="T20" s="304"/>
+      <c r="T20" s="266"/>
       <c r="U20" s="105"/>
       <c r="V20" s="88" t="s">
         <v>95</v>
@@ -13498,24 +13615,24 @@
         <v>93</v>
       </c>
       <c r="Y20" s="107"/>
-      <c r="Z20" s="305"/>
+      <c r="Z20" s="267"/>
       <c r="AA20" s="123"/>
       <c r="AB20" s="147" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AC20" s="144"/>
       <c r="AD20" s="117"/>
       <c r="AE20" s="217" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AF20" s="1"/>
       <c r="AG20" s="214" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AH20" s="106"/>
       <c r="AI20" s="142"/>
       <c r="AJ20" s="150" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AL20" s="21"/>
       <c r="AM20" s="21"/>
@@ -13529,9 +13646,9 @@
       <c r="C21" s="82" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="261"/>
-      <c r="E21" s="247"/>
-      <c r="F21" s="247"/>
+      <c r="D21" s="247"/>
+      <c r="E21" s="248"/>
+      <c r="F21" s="248"/>
       <c r="G21" s="64"/>
       <c r="H21" s="78" t="s">
         <v>116</v>
@@ -13539,9 +13656,9 @@
       <c r="I21" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="J21" s="261"/>
-      <c r="K21" s="247"/>
-      <c r="L21" s="247"/>
+      <c r="J21" s="247"/>
+      <c r="K21" s="248"/>
+      <c r="L21" s="248"/>
       <c r="N21" s="68" t="s">
         <v>86</v>
       </c>
@@ -13555,7 +13672,7 @@
         <v>96</v>
       </c>
       <c r="S21" s="125"/>
-      <c r="T21" s="304"/>
+      <c r="T21" s="266"/>
       <c r="U21" s="105"/>
       <c r="V21" s="65" t="s">
         <v>104</v>
@@ -13565,7 +13682,7 @@
         <v>112</v>
       </c>
       <c r="Y21" s="107"/>
-      <c r="Z21" s="305"/>
+      <c r="Z21" s="267"/>
       <c r="AA21" s="123"/>
       <c r="AB21" s="148" t="s">
         <v>81</v>
@@ -13604,9 +13721,9 @@
       <c r="C22" s="79" t="s">
         <v>127</v>
       </c>
-      <c r="D22" s="261"/>
-      <c r="E22" s="247"/>
-      <c r="F22" s="247"/>
+      <c r="D22" s="247"/>
+      <c r="E22" s="248"/>
+      <c r="F22" s="248"/>
       <c r="G22" s="64"/>
       <c r="H22" s="83" t="s">
         <v>122</v>
@@ -13614,9 +13731,9 @@
       <c r="I22" s="79" t="s">
         <v>119</v>
       </c>
-      <c r="J22" s="261"/>
-      <c r="K22" s="247"/>
-      <c r="L22" s="247"/>
+      <c r="J22" s="247"/>
+      <c r="K22" s="248"/>
+      <c r="L22" s="248"/>
       <c r="N22" s="89" t="s">
         <v>88</v>
       </c>
@@ -13630,7 +13747,7 @@
         <v>90</v>
       </c>
       <c r="S22" s="60"/>
-      <c r="T22" s="304"/>
+      <c r="T22" s="266"/>
       <c r="U22" s="105"/>
       <c r="V22" s="88" t="s">
         <v>106</v>
@@ -13640,7 +13757,7 @@
         <v>105</v>
       </c>
       <c r="Y22" s="107"/>
-      <c r="Z22" s="305"/>
+      <c r="Z22" s="267"/>
       <c r="AA22" s="123"/>
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
@@ -13663,9 +13780,9 @@
       <c r="C23" s="84" t="s">
         <v>107</v>
       </c>
-      <c r="D23" s="261"/>
-      <c r="E23" s="247"/>
-      <c r="F23" s="247"/>
+      <c r="D23" s="247"/>
+      <c r="E23" s="248"/>
+      <c r="F23" s="248"/>
       <c r="G23" s="64"/>
       <c r="H23" s="80" t="s">
         <v>121</v>
@@ -13673,9 +13790,9 @@
       <c r="I23" s="84" t="s">
         <v>123</v>
       </c>
-      <c r="J23" s="261"/>
-      <c r="K23" s="247"/>
-      <c r="L23" s="247"/>
+      <c r="J23" s="247"/>
+      <c r="K23" s="248"/>
+      <c r="L23" s="248"/>
       <c r="N23" s="68" t="s">
         <v>97</v>
       </c>
@@ -13688,7 +13805,7 @@
       <c r="R23" s="86" t="s">
         <v>107</v>
       </c>
-      <c r="T23" s="304"/>
+      <c r="T23" s="266"/>
       <c r="U23" s="105"/>
       <c r="V23" s="65" t="s">
         <v>113</v>
@@ -13698,7 +13815,7 @@
         <v>118</v>
       </c>
       <c r="Y23" s="107"/>
-      <c r="Z23" s="305"/>
+      <c r="Z23" s="267"/>
       <c r="AA23" s="123"/>
       <c r="AB23" s="152" t="s">
         <v>98</v>
@@ -13741,10 +13858,10 @@
         <v>112</v>
       </c>
       <c r="R24" s="90" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="S24" s="1"/>
-      <c r="T24" s="304"/>
+      <c r="T24" s="266"/>
       <c r="U24" s="105"/>
       <c r="V24" s="88" t="s">
         <v>110</v>
@@ -13754,24 +13871,24 @@
         <v>114</v>
       </c>
       <c r="Y24" s="107"/>
-      <c r="Z24" s="305"/>
+      <c r="Z24" s="267"/>
       <c r="AA24" s="123"/>
       <c r="AB24" s="214" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AC24" s="106"/>
       <c r="AD24" s="143"/>
       <c r="AE24" s="151" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AF24" s="1"/>
       <c r="AG24" s="148" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AH24" s="145"/>
       <c r="AI24" s="117"/>
       <c r="AJ24" s="217" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -13780,13 +13897,13 @@
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
-      <c r="H25" s="251" t="s">
+      <c r="H25" s="264" t="s">
         <v>152</v>
       </c>
-      <c r="I25" s="251"/>
-      <c r="J25" s="251"/>
-      <c r="K25" s="251"/>
-      <c r="L25" s="251"/>
+      <c r="I25" s="264"/>
+      <c r="J25" s="264"/>
+      <c r="K25" s="264"/>
+      <c r="L25" s="264"/>
       <c r="N25" s="68" t="s">
         <v>108</v>
       </c>
@@ -13800,7 +13917,7 @@
         <v>115</v>
       </c>
       <c r="S25" s="1"/>
-      <c r="T25" s="304"/>
+      <c r="T25" s="266"/>
       <c r="U25" s="105"/>
       <c r="V25" s="65" t="s">
         <v>119</v>
@@ -13810,10 +13927,10 @@
         <v>122</v>
       </c>
       <c r="Y25" s="107"/>
-      <c r="Z25" s="305"/>
+      <c r="Z25" s="267"/>
       <c r="AA25" s="123"/>
       <c r="AB25" s="147" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AC25" s="144" t="s">
         <v>87</v>
@@ -13822,11 +13939,11 @@
         <v>87</v>
       </c>
       <c r="AE25" s="217" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AF25" s="1"/>
       <c r="AG25" s="214" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AH25" s="106" t="s">
         <v>87</v>
@@ -13835,26 +13952,26 @@
         <v>87</v>
       </c>
       <c r="AJ25" s="150" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="26" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="74" t="s">
         <v>130</v>
       </c>
-      <c r="C26" s="252" t="s">
+      <c r="C26" s="253" t="s">
         <v>131</v>
       </c>
-      <c r="D26" s="253"/>
-      <c r="E26" s="252" t="s">
+      <c r="D26" s="254"/>
+      <c r="E26" s="253" t="s">
         <v>132</v>
       </c>
-      <c r="F26" s="254"/>
-      <c r="H26" s="251"/>
-      <c r="I26" s="251"/>
-      <c r="J26" s="251"/>
-      <c r="K26" s="251"/>
-      <c r="L26" s="251"/>
+      <c r="F26" s="255"/>
+      <c r="H26" s="264"/>
+      <c r="I26" s="264"/>
+      <c r="J26" s="264"/>
+      <c r="K26" s="264"/>
+      <c r="L26" s="264"/>
       <c r="N26" s="89" t="s">
         <v>109</v>
       </c>
@@ -13868,7 +13985,7 @@
         <v>78</v>
       </c>
       <c r="S26" s="1"/>
-      <c r="T26" s="304"/>
+      <c r="T26" s="266"/>
       <c r="U26" s="118"/>
       <c r="V26" s="94" t="s">
         <v>83</v>
@@ -13878,7 +13995,7 @@
         <v>120</v>
       </c>
       <c r="Y26" s="112"/>
-      <c r="Z26" s="305"/>
+      <c r="Z26" s="267"/>
       <c r="AA26" s="123"/>
       <c r="AB26" s="148" t="s">
         <v>81</v>
@@ -13910,19 +14027,19 @@
       <c r="B27" s="75" t="s">
         <v>134</v>
       </c>
-      <c r="C27" s="255">
+      <c r="C27" s="256">
         <v>0.8</v>
       </c>
-      <c r="D27" s="256"/>
-      <c r="E27" s="255">
+      <c r="D27" s="257"/>
+      <c r="E27" s="256">
         <v>100</v>
       </c>
-      <c r="F27" s="257"/>
-      <c r="H27" s="251"/>
-      <c r="I27" s="251"/>
-      <c r="J27" s="251"/>
-      <c r="K27" s="251"/>
-      <c r="L27" s="251"/>
+      <c r="F27" s="258"/>
+      <c r="H27" s="264"/>
+      <c r="I27" s="264"/>
+      <c r="J27" s="264"/>
+      <c r="K27" s="264"/>
+      <c r="L27" s="264"/>
       <c r="N27" s="68" t="s">
         <v>116</v>
       </c>
@@ -13946,19 +14063,19 @@
       <c r="B28" s="76" t="s">
         <v>135</v>
       </c>
-      <c r="C28" s="258">
+      <c r="C28" s="259">
         <v>1</v>
       </c>
-      <c r="D28" s="259"/>
-      <c r="E28" s="258">
+      <c r="D28" s="260"/>
+      <c r="E28" s="259">
         <v>180</v>
       </c>
-      <c r="F28" s="260"/>
-      <c r="H28" s="251"/>
-      <c r="I28" s="251"/>
-      <c r="J28" s="251"/>
-      <c r="K28" s="251"/>
-      <c r="L28" s="251"/>
+      <c r="F28" s="261"/>
+      <c r="H28" s="264"/>
+      <c r="I28" s="264"/>
+      <c r="J28" s="264"/>
+      <c r="K28" s="264"/>
+      <c r="L28" s="264"/>
       <c r="N28" s="89" t="s">
         <v>117</v>
       </c>
@@ -13971,36 +14088,36 @@
       <c r="R28" s="90" t="s">
         <v>100</v>
       </c>
-      <c r="V28" s="306" t="s">
+      <c r="V28" s="270" t="s">
         <v>76</v>
       </c>
-      <c r="W28" s="306"/>
-      <c r="X28" s="306"/>
-      <c r="AB28" s="248" t="s">
-        <v>198</v>
-      </c>
-      <c r="AC28" s="248"/>
-      <c r="AD28" s="248"/>
-      <c r="AE28" s="248"/>
-      <c r="AF28" s="248"/>
-      <c r="AG28" s="248"/>
-      <c r="AH28" s="248"/>
-      <c r="AI28" s="248"/>
-      <c r="AJ28" s="248"/>
+      <c r="W28" s="270"/>
+      <c r="X28" s="270"/>
+      <c r="AB28" s="268" t="s">
+        <v>197</v>
+      </c>
+      <c r="AC28" s="268"/>
+      <c r="AD28" s="268"/>
+      <c r="AE28" s="268"/>
+      <c r="AF28" s="268"/>
+      <c r="AG28" s="268"/>
+      <c r="AH28" s="268"/>
+      <c r="AI28" s="268"/>
+      <c r="AJ28" s="268"/>
     </row>
     <row r="29" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="309" t="s">
+      <c r="B29" s="250" t="s">
         <v>136</v>
       </c>
-      <c r="C29" s="309"/>
-      <c r="D29" s="309"/>
-      <c r="E29" s="309"/>
-      <c r="F29" s="309"/>
-      <c r="H29" s="251"/>
-      <c r="I29" s="251"/>
-      <c r="J29" s="251"/>
-      <c r="K29" s="251"/>
-      <c r="L29" s="251"/>
+      <c r="C29" s="250"/>
+      <c r="D29" s="250"/>
+      <c r="E29" s="250"/>
+      <c r="F29" s="250"/>
+      <c r="H29" s="264"/>
+      <c r="I29" s="264"/>
+      <c r="J29" s="264"/>
+      <c r="K29" s="264"/>
+      <c r="L29" s="264"/>
       <c r="N29" s="70" t="s">
         <v>121</v>
       </c>
@@ -14014,20 +14131,20 @@
         <v>123</v>
       </c>
       <c r="S29" s="60"/>
-      <c r="V29" s="307"/>
-      <c r="W29" s="307"/>
-      <c r="X29" s="307"/>
-      <c r="AB29" s="248" t="s">
-        <v>197</v>
-      </c>
-      <c r="AC29" s="248"/>
-      <c r="AD29" s="248"/>
-      <c r="AE29" s="248"/>
-      <c r="AF29" s="248"/>
-      <c r="AG29" s="248"/>
-      <c r="AH29" s="248"/>
-      <c r="AI29" s="248"/>
-      <c r="AJ29" s="248"/>
+      <c r="V29" s="249"/>
+      <c r="W29" s="249"/>
+      <c r="X29" s="249"/>
+      <c r="AB29" s="268" t="s">
+        <v>196</v>
+      </c>
+      <c r="AC29" s="268"/>
+      <c r="AD29" s="268"/>
+      <c r="AE29" s="268"/>
+      <c r="AF29" s="268"/>
+      <c r="AG29" s="268"/>
+      <c r="AH29" s="268"/>
+      <c r="AI29" s="268"/>
+      <c r="AJ29" s="268"/>
     </row>
     <row r="30" spans="2:41" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="S30" s="1"/>
@@ -14065,11 +14182,21 @@
     <row r="41" spans="19:19" ht="14" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="D3:F4"/>
-    <mergeCell ref="J3:L7"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="AB28:AJ28"/>
+    <mergeCell ref="AB29:AJ29"/>
+    <mergeCell ref="AL3:AN3"/>
+    <mergeCell ref="AB3:AJ3"/>
+    <mergeCell ref="V28:X29"/>
+    <mergeCell ref="V2:X3"/>
+    <mergeCell ref="T5:T26"/>
+    <mergeCell ref="Z5:Z26"/>
+    <mergeCell ref="AL15:AN15"/>
+    <mergeCell ref="AL4:AN12"/>
+    <mergeCell ref="AL17:AN17"/>
+    <mergeCell ref="AL18:AN18"/>
+    <mergeCell ref="AB4:AJ5"/>
+    <mergeCell ref="AB16:AJ17"/>
+    <mergeCell ref="AL19:AN19"/>
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="N18:O18"/>
     <mergeCell ref="Q18:R18"/>
@@ -14083,21 +14210,11 @@
     <mergeCell ref="J8:L8"/>
     <mergeCell ref="J10:L23"/>
     <mergeCell ref="H25:L29"/>
-    <mergeCell ref="T5:T26"/>
-    <mergeCell ref="Z5:Z26"/>
-    <mergeCell ref="AL15:AN15"/>
-    <mergeCell ref="AL4:AN12"/>
-    <mergeCell ref="AL17:AN17"/>
-    <mergeCell ref="AL18:AN18"/>
-    <mergeCell ref="AB4:AJ5"/>
-    <mergeCell ref="AB16:AJ17"/>
-    <mergeCell ref="AL19:AN19"/>
-    <mergeCell ref="AB28:AJ28"/>
-    <mergeCell ref="AB29:AJ29"/>
-    <mergeCell ref="AL3:AN3"/>
-    <mergeCell ref="AB3:AJ3"/>
-    <mergeCell ref="V28:X29"/>
-    <mergeCell ref="V2:X3"/>
+    <mergeCell ref="D3:F4"/>
+    <mergeCell ref="J3:L7"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="D5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="44" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -14111,7 +14228,7 @@
   </sheetPr>
   <dimension ref="A2:AC43"/>
   <sheetViews>
-    <sheetView zoomScale="84" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="G1" zoomScale="84" workbookViewId="0">
       <selection activeCell="O45" sqref="O45"/>
     </sheetView>
   </sheetViews>
@@ -14128,27 +14245,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:29" ht="16" x14ac:dyDescent="0.35">
-      <c r="B2" s="275" t="s">
+      <c r="B2" s="276" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="275"/>
-      <c r="D2" s="275"/>
-      <c r="E2" s="275"/>
-      <c r="F2" s="275"/>
-      <c r="N2" s="276" t="s">
-        <v>174</v>
-      </c>
-      <c r="O2" s="276"/>
-      <c r="P2" s="276"/>
-      <c r="Q2" s="276"/>
-      <c r="R2" s="276"/>
-      <c r="T2" s="276" t="s">
+      <c r="C2" s="276"/>
+      <c r="D2" s="276"/>
+      <c r="E2" s="276"/>
+      <c r="F2" s="276"/>
+      <c r="N2" s="249" t="s">
         <v>173</v>
       </c>
-      <c r="U2" s="276"/>
-      <c r="V2" s="276"/>
-      <c r="W2" s="276"/>
-      <c r="X2" s="276"/>
+      <c r="O2" s="249"/>
+      <c r="P2" s="249"/>
+      <c r="Q2" s="249"/>
+      <c r="R2" s="249"/>
+      <c r="T2" s="249" t="s">
+        <v>172</v>
+      </c>
+      <c r="U2" s="249"/>
+      <c r="V2" s="249"/>
+      <c r="W2" s="249"/>
+      <c r="X2" s="249"/>
     </row>
     <row r="3" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="H3" s="24" t="s">
@@ -14158,33 +14275,33 @@
         <v>20</v>
       </c>
       <c r="N3" s="278" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="O3" s="278"/>
       <c r="P3" s="278"/>
       <c r="Q3" s="278"/>
       <c r="R3" s="278"/>
       <c r="T3" s="278" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="U3" s="278"/>
       <c r="V3" s="278"/>
       <c r="W3" s="278"/>
       <c r="X3" s="278"/>
-      <c r="Z3" s="247" t="s">
+      <c r="Z3" s="248" t="s">
         <v>34</v>
       </c>
-      <c r="AA3" s="247"/>
-      <c r="AB3" s="247"/>
+      <c r="AA3" s="248"/>
+      <c r="AB3" s="248"/>
     </row>
     <row r="4" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="26"/>
       <c r="C4" s="277" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="263"/>
-      <c r="E4" s="263"/>
-      <c r="F4" s="263"/>
+      <c r="D4" s="275"/>
+      <c r="E4" s="275"/>
+      <c r="F4" s="275"/>
       <c r="H4" s="1" t="s">
         <v>4</v>
       </c>
@@ -14201,9 +14318,9 @@
       <c r="V4" s="20"/>
       <c r="W4" s="20"/>
       <c r="X4" s="22"/>
-      <c r="Z4" s="247"/>
-      <c r="AA4" s="247"/>
-      <c r="AB4" s="247"/>
+      <c r="Z4" s="248"/>
+      <c r="AA4" s="248"/>
+      <c r="AB4" s="248"/>
     </row>
     <row r="5" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="H5" s="1" t="s">
@@ -14212,44 +14329,44 @@
       <c r="I5" s="1">
         <v>20</v>
       </c>
-      <c r="Z5" s="247"/>
-      <c r="AA5" s="247"/>
-      <c r="AB5" s="247"/>
+      <c r="Z5" s="248"/>
+      <c r="AA5" s="248"/>
+      <c r="AB5" s="248"/>
       <c r="AC5" s="21"/>
     </row>
     <row r="6" spans="1:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="263" t="s">
+      <c r="C6" s="275" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="263"/>
-      <c r="E6" s="263"/>
-      <c r="F6" s="263"/>
+      <c r="D6" s="275"/>
+      <c r="E6" s="275"/>
+      <c r="F6" s="275"/>
       <c r="H6" s="1" t="s">
         <v>37</v>
       </c>
       <c r="I6" s="1">
         <v>20</v>
       </c>
-      <c r="N6" s="272" t="s">
-        <v>200</v>
-      </c>
-      <c r="O6" s="273"/>
-      <c r="Q6" s="272" t="s">
-        <v>200</v>
-      </c>
-      <c r="R6" s="273"/>
-      <c r="T6" s="272" t="s">
-        <v>204</v>
-      </c>
-      <c r="U6" s="273"/>
+      <c r="N6" s="273" t="s">
+        <v>199</v>
+      </c>
+      <c r="O6" s="274"/>
+      <c r="Q6" s="273" t="s">
+        <v>199</v>
+      </c>
+      <c r="R6" s="274"/>
+      <c r="T6" s="273" t="s">
+        <v>203</v>
+      </c>
+      <c r="U6" s="274"/>
       <c r="V6" s="27"/>
-      <c r="W6" s="272" t="s">
-        <v>204</v>
-      </c>
-      <c r="X6" s="273"/>
+      <c r="W6" s="273" t="s">
+        <v>203</v>
+      </c>
+      <c r="X6" s="274"/>
       <c r="Z6" s="21"/>
       <c r="AA6" s="21"/>
       <c r="AB6" s="21"/>
@@ -14257,22 +14374,22 @@
     </row>
     <row r="7" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="M7" s="29"/>
-      <c r="Z7" s="247" t="s">
+      <c r="Z7" s="248" t="s">
         <v>42</v>
       </c>
-      <c r="AA7" s="247"/>
-      <c r="AB7" s="247"/>
+      <c r="AA7" s="248"/>
+      <c r="AB7" s="248"/>
     </row>
     <row r="8" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="263" t="s">
+      <c r="C8" s="275" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="263"/>
-      <c r="E8" s="263"/>
-      <c r="F8" s="263"/>
+      <c r="D8" s="275"/>
+      <c r="E8" s="275"/>
+      <c r="F8" s="275"/>
       <c r="N8" s="30" t="s">
         <v>41</v>
       </c>
@@ -14297,25 +14414,25 @@
       <c r="X8" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="Z8" s="247"/>
-      <c r="AA8" s="247"/>
-      <c r="AB8" s="247"/>
+      <c r="Z8" s="248"/>
+      <c r="AA8" s="248"/>
+      <c r="AB8" s="248"/>
     </row>
     <row r="9" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="Z9" s="247"/>
-      <c r="AA9" s="247"/>
-      <c r="AB9" s="247"/>
+      <c r="Z9" s="248"/>
+      <c r="AA9" s="248"/>
+      <c r="AB9" s="248"/>
     </row>
     <row r="10" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="263" t="s">
+      <c r="C10" s="275" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="263"/>
-      <c r="E10" s="263"/>
-      <c r="F10" s="263"/>
+      <c r="D10" s="275"/>
+      <c r="E10" s="275"/>
+      <c r="F10" s="275"/>
       <c r="N10" s="34" t="s">
         <v>44</v>
       </c>
@@ -14345,47 +14462,47 @@
       <c r="AB10" s="38"/>
     </row>
     <row r="11" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N11" s="263" t="s">
+      <c r="N11" s="275" t="s">
         <v>58</v>
       </c>
-      <c r="O11" s="263"/>
-      <c r="Q11" s="263" t="s">
+      <c r="O11" s="275"/>
+      <c r="Q11" s="275" t="s">
         <v>58</v>
       </c>
-      <c r="R11" s="263"/>
-      <c r="T11" s="279" t="s">
+      <c r="R11" s="275"/>
+      <c r="T11" s="272" t="s">
         <v>59</v>
       </c>
-      <c r="U11" s="279"/>
-      <c r="W11" s="279" t="s">
+      <c r="U11" s="272"/>
+      <c r="W11" s="272" t="s">
         <v>59</v>
       </c>
-      <c r="X11" s="279"/>
-      <c r="Z11" s="247" t="s">
+      <c r="X11" s="272"/>
+      <c r="Z11" s="248" t="s">
         <v>49</v>
       </c>
-      <c r="AA11" s="247"/>
-      <c r="AB11" s="247"/>
+      <c r="AA11" s="248"/>
+      <c r="AB11" s="248"/>
     </row>
     <row r="12" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="274" t="s">
+      <c r="B12" s="279" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="274"/>
-      <c r="D12" s="274"/>
-      <c r="E12" s="274"/>
-      <c r="F12" s="274"/>
+      <c r="C12" s="279"/>
+      <c r="D12" s="279"/>
+      <c r="E12" s="279"/>
+      <c r="F12" s="279"/>
       <c r="N12" s="40" t="s">
         <v>45</v>
       </c>
       <c r="O12" s="41" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q12" s="40" t="s">
         <v>45</v>
       </c>
       <c r="R12" s="41" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="T12" s="40" t="s">
         <v>44</v>
@@ -14399,54 +14516,54 @@
       <c r="X12" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="Z12" s="247"/>
-      <c r="AA12" s="247"/>
-      <c r="AB12" s="247"/>
+      <c r="Z12" s="248"/>
+      <c r="AA12" s="248"/>
+      <c r="AB12" s="248"/>
     </row>
     <row r="13" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N13" s="263" t="s">
+      <c r="N13" s="275" t="s">
         <v>61</v>
       </c>
-      <c r="O13" s="263"/>
-      <c r="Q13" s="263" t="s">
+      <c r="O13" s="275"/>
+      <c r="Q13" s="275" t="s">
         <v>61</v>
       </c>
-      <c r="R13" s="263"/>
-      <c r="T13" s="263" t="s">
+      <c r="R13" s="275"/>
+      <c r="T13" s="275" t="s">
         <v>62</v>
       </c>
-      <c r="U13" s="263"/>
-      <c r="W13" s="263" t="s">
+      <c r="U13" s="275"/>
+      <c r="W13" s="275" t="s">
         <v>62</v>
       </c>
-      <c r="X13" s="263"/>
-      <c r="Z13" s="247"/>
-      <c r="AA13" s="247"/>
-      <c r="AB13" s="247"/>
+      <c r="X13" s="275"/>
+      <c r="Z13" s="248"/>
+      <c r="AA13" s="248"/>
+      <c r="AB13" s="248"/>
     </row>
     <row r="14" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="270" t="s">
+      <c r="B14" s="280" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="270"/>
-      <c r="D14" s="270"/>
-      <c r="E14" s="270"/>
-      <c r="F14" s="270"/>
-      <c r="H14" s="271" t="s">
+      <c r="C14" s="280"/>
+      <c r="D14" s="280"/>
+      <c r="E14" s="280"/>
+      <c r="F14" s="280"/>
+      <c r="H14" s="281" t="s">
         <v>5</v>
       </c>
-      <c r="I14" s="271"/>
-      <c r="J14" s="271"/>
-      <c r="K14" s="271"/>
-      <c r="L14" s="271"/>
+      <c r="I14" s="281"/>
+      <c r="J14" s="281"/>
+      <c r="K14" s="281"/>
+      <c r="L14" s="281"/>
       <c r="N14" s="44" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="O14" s="42" t="s">
         <v>45</v>
       </c>
       <c r="Q14" s="44" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="R14" s="42" t="s">
         <v>45</v>
@@ -14465,30 +14582,30 @@
       </c>
     </row>
     <row r="15" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N15" s="263" t="s">
+      <c r="N15" s="275" t="s">
         <v>65</v>
       </c>
-      <c r="O15" s="263"/>
-      <c r="Q15" s="263" t="s">
+      <c r="O15" s="275"/>
+      <c r="Q15" s="275" t="s">
         <v>65</v>
       </c>
-      <c r="R15" s="263"/>
-      <c r="T15" s="263" t="s">
+      <c r="R15" s="275"/>
+      <c r="T15" s="275" t="s">
         <v>64</v>
       </c>
-      <c r="U15" s="263"/>
-      <c r="W15" s="263" t="s">
+      <c r="U15" s="275"/>
+      <c r="W15" s="275" t="s">
         <v>64</v>
       </c>
-      <c r="X15" s="263"/>
-      <c r="Z15" s="247" t="s">
+      <c r="X15" s="275"/>
+      <c r="Z15" s="248" t="s">
         <v>55</v>
       </c>
-      <c r="AA15" s="247"/>
-      <c r="AB15" s="247"/>
+      <c r="AA15" s="248"/>
+      <c r="AB15" s="248"/>
     </row>
     <row r="16" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="264">
+      <c r="A16" s="282">
         <v>1</v>
       </c>
       <c r="B16" s="45" t="s">
@@ -14497,7 +14614,7 @@
       <c r="C16" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="265">
+      <c r="D16" s="283">
         <v>3</v>
       </c>
       <c r="E16" s="45" t="s">
@@ -14506,7 +14623,7 @@
       <c r="F16" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="264">
+      <c r="G16" s="282">
         <v>1</v>
       </c>
       <c r="H16" s="47" t="s">
@@ -14515,7 +14632,7 @@
       <c r="I16" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="J16" s="265">
+      <c r="J16" s="283">
         <v>3</v>
       </c>
       <c r="K16" s="47" t="s">
@@ -14524,63 +14641,63 @@
       <c r="L16" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="Z16" s="247"/>
-      <c r="AA16" s="247"/>
-      <c r="AB16" s="247"/>
+      <c r="Z16" s="248"/>
+      <c r="AA16" s="248"/>
+      <c r="AB16" s="248"/>
     </row>
     <row r="17" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="264"/>
+      <c r="A17" s="282"/>
       <c r="B17" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="265"/>
+      <c r="D17" s="283"/>
       <c r="E17" s="49" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="264"/>
+      <c r="G17" s="282"/>
       <c r="H17" s="51" t="s">
         <v>16</v>
       </c>
       <c r="I17" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="265"/>
+      <c r="J17" s="283"/>
       <c r="K17" s="51" t="s">
         <v>15</v>
       </c>
       <c r="L17" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="N17" s="272" t="s">
+      <c r="N17" s="273" t="s">
+        <v>200</v>
+      </c>
+      <c r="O17" s="274"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="273" t="s">
+        <v>200</v>
+      </c>
+      <c r="R17" s="274"/>
+      <c r="T17" s="273" t="s">
         <v>201</v>
       </c>
-      <c r="O17" s="273"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="272" t="s">
-        <v>201</v>
-      </c>
-      <c r="R17" s="273"/>
-      <c r="T17" s="272" t="s">
+      <c r="U17" s="274"/>
+      <c r="W17" s="273" t="s">
         <v>202</v>
       </c>
-      <c r="U17" s="273"/>
-      <c r="W17" s="272" t="s">
-        <v>203</v>
-      </c>
-      <c r="X17" s="273"/>
-      <c r="Z17" s="247"/>
-      <c r="AA17" s="247"/>
-      <c r="AB17" s="247"/>
+      <c r="X17" s="274"/>
+      <c r="Z17" s="248"/>
+      <c r="AA17" s="248"/>
+      <c r="AB17" s="248"/>
     </row>
     <row r="18" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="19" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="264">
+      <c r="A19" s="282">
         <v>2</v>
       </c>
       <c r="B19" s="45" t="s">
@@ -14589,7 +14706,7 @@
       <c r="C19" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="265">
+      <c r="D19" s="283">
         <v>4</v>
       </c>
       <c r="E19" s="45" t="s">
@@ -14598,7 +14715,7 @@
       <c r="F19" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="264">
+      <c r="G19" s="282">
         <v>2</v>
       </c>
       <c r="H19" s="47" t="s">
@@ -14607,7 +14724,7 @@
       <c r="I19" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="J19" s="265">
+      <c r="J19" s="283">
         <v>4</v>
       </c>
       <c r="K19" s="47" t="s">
@@ -14640,44 +14757,44 @@
       <c r="X19" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="Z19" s="247" t="s">
+      <c r="Z19" s="248" t="s">
         <v>57</v>
       </c>
-      <c r="AA19" s="247"/>
-      <c r="AB19" s="247"/>
+      <c r="AA19" s="248"/>
+      <c r="AB19" s="248"/>
     </row>
     <row r="20" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="264"/>
+      <c r="A20" s="282"/>
       <c r="B20" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="265"/>
+      <c r="D20" s="283"/>
       <c r="E20" s="49" t="s">
         <v>15</v>
       </c>
       <c r="F20" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="264"/>
+      <c r="G20" s="282"/>
       <c r="H20" s="51" t="s">
         <v>16</v>
       </c>
       <c r="I20" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="J20" s="265"/>
+      <c r="J20" s="283"/>
       <c r="K20" s="51" t="s">
         <v>15</v>
       </c>
       <c r="L20" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="Z20" s="247"/>
-      <c r="AA20" s="247"/>
-      <c r="AB20" s="247"/>
+      <c r="Z20" s="248"/>
+      <c r="AA20" s="248"/>
+      <c r="AB20" s="248"/>
     </row>
     <row r="21" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="N21" s="35" t="s">
@@ -14704,43 +14821,43 @@
       <c r="X21" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="Z21" s="247"/>
-      <c r="AA21" s="247"/>
-      <c r="AB21" s="247"/>
+      <c r="Z21" s="248"/>
+      <c r="AA21" s="248"/>
+      <c r="AB21" s="248"/>
     </row>
     <row r="22" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N22" s="279" t="s">
+      <c r="N22" s="272" t="s">
         <v>47</v>
       </c>
-      <c r="O22" s="279"/>
-      <c r="Q22" s="279" t="s">
+      <c r="O22" s="272"/>
+      <c r="Q22" s="272" t="s">
         <v>47</v>
       </c>
-      <c r="R22" s="279"/>
-      <c r="T22" s="263" t="s">
+      <c r="R22" s="272"/>
+      <c r="T22" s="275" t="s">
         <v>48</v>
       </c>
-      <c r="U22" s="263"/>
-      <c r="W22" s="263" t="s">
+      <c r="U22" s="275"/>
+      <c r="W22" s="275" t="s">
         <v>48</v>
       </c>
-      <c r="X22" s="263"/>
+      <c r="X22" s="275"/>
     </row>
     <row r="23" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="267" t="s">
+      <c r="B23" s="285" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="267"/>
-      <c r="D23" s="267"/>
-      <c r="E23" s="267"/>
-      <c r="F23" s="267"/>
-      <c r="H23" s="247" t="s">
+      <c r="C23" s="285"/>
+      <c r="D23" s="285"/>
+      <c r="E23" s="285"/>
+      <c r="F23" s="285"/>
+      <c r="H23" s="248" t="s">
         <v>60</v>
       </c>
-      <c r="I23" s="247"/>
-      <c r="J23" s="247"/>
-      <c r="K23" s="247"/>
-      <c r="L23" s="247"/>
+      <c r="I23" s="248"/>
+      <c r="J23" s="248"/>
+      <c r="K23" s="248"/>
+      <c r="L23" s="248"/>
       <c r="N23" s="39" t="s">
         <v>46</v>
       </c>
@@ -14754,51 +14871,51 @@
         <v>45</v>
       </c>
       <c r="T23" s="39" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="U23" s="40" t="s">
         <v>44</v>
       </c>
       <c r="W23" s="39" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="X23" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="Z23" s="247" t="s">
+      <c r="Z23" s="248" t="s">
         <v>63</v>
       </c>
-      <c r="AA23" s="247"/>
-      <c r="AB23" s="247"/>
+      <c r="AA23" s="248"/>
+      <c r="AB23" s="248"/>
     </row>
     <row r="24" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H24" s="247"/>
-      <c r="I24" s="247"/>
-      <c r="J24" s="247"/>
-      <c r="K24" s="247"/>
-      <c r="L24" s="247"/>
-      <c r="N24" s="263" t="s">
+      <c r="H24" s="248"/>
+      <c r="I24" s="248"/>
+      <c r="J24" s="248"/>
+      <c r="K24" s="248"/>
+      <c r="L24" s="248"/>
+      <c r="N24" s="275" t="s">
         <v>51</v>
       </c>
-      <c r="O24" s="263"/>
-      <c r="Q24" s="263" t="s">
+      <c r="O24" s="275"/>
+      <c r="Q24" s="275" t="s">
         <v>51</v>
       </c>
-      <c r="R24" s="263"/>
-      <c r="T24" s="263" t="s">
+      <c r="R24" s="275"/>
+      <c r="T24" s="275" t="s">
         <v>52</v>
       </c>
-      <c r="U24" s="263"/>
-      <c r="W24" s="263" t="s">
+      <c r="U24" s="275"/>
+      <c r="W24" s="275" t="s">
         <v>52</v>
       </c>
-      <c r="X24" s="263"/>
-      <c r="Z24" s="247"/>
-      <c r="AA24" s="247"/>
-      <c r="AB24" s="247"/>
+      <c r="X24" s="275"/>
+      <c r="Z24" s="248"/>
+      <c r="AA24" s="248"/>
+      <c r="AB24" s="248"/>
     </row>
     <row r="25" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="264">
+      <c r="A25" s="282">
         <v>1</v>
       </c>
       <c r="B25" s="53" t="s">
@@ -14807,7 +14924,7 @@
       <c r="C25" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="265">
+      <c r="D25" s="283">
         <v>3</v>
       </c>
       <c r="E25" s="53" t="s">
@@ -14816,11 +14933,11 @@
       <c r="F25" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="247"/>
-      <c r="I25" s="247"/>
-      <c r="J25" s="247"/>
-      <c r="K25" s="247"/>
-      <c r="L25" s="247"/>
+      <c r="H25" s="248"/>
+      <c r="I25" s="248"/>
+      <c r="J25" s="248"/>
+      <c r="K25" s="248"/>
+      <c r="L25" s="248"/>
       <c r="N25" s="42" t="s">
         <v>45</v>
       </c>
@@ -14845,53 +14962,53 @@
       <c r="X25" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="Z25" s="247"/>
-      <c r="AA25" s="247"/>
-      <c r="AB25" s="247"/>
+      <c r="Z25" s="248"/>
+      <c r="AA25" s="248"/>
+      <c r="AB25" s="248"/>
     </row>
     <row r="26" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="264"/>
+      <c r="A26" s="282"/>
       <c r="B26" s="55" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="265"/>
+      <c r="D26" s="283"/>
       <c r="E26" s="55" t="s">
         <v>15</v>
       </c>
       <c r="F26" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="H26" s="247"/>
-      <c r="I26" s="247"/>
-      <c r="J26" s="247"/>
-      <c r="K26" s="247"/>
-      <c r="L26" s="247"/>
-      <c r="N26" s="263" t="s">
+      <c r="H26" s="248"/>
+      <c r="I26" s="248"/>
+      <c r="J26" s="248"/>
+      <c r="K26" s="248"/>
+      <c r="L26" s="248"/>
+      <c r="N26" s="275" t="s">
         <v>54</v>
       </c>
-      <c r="O26" s="263"/>
-      <c r="Q26" s="263" t="s">
+      <c r="O26" s="275"/>
+      <c r="Q26" s="275" t="s">
         <v>54</v>
       </c>
-      <c r="R26" s="263"/>
-      <c r="T26" s="263" t="s">
+      <c r="R26" s="275"/>
+      <c r="T26" s="275" t="s">
         <v>53</v>
       </c>
-      <c r="U26" s="263"/>
-      <c r="W26" s="263" t="s">
+      <c r="U26" s="275"/>
+      <c r="W26" s="275" t="s">
         <v>53</v>
       </c>
-      <c r="X26" s="263"/>
+      <c r="X26" s="275"/>
     </row>
     <row r="27" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H27" s="247"/>
-      <c r="I27" s="247"/>
-      <c r="J27" s="247"/>
-      <c r="K27" s="247"/>
-      <c r="L27" s="247"/>
+      <c r="H27" s="248"/>
+      <c r="I27" s="248"/>
+      <c r="J27" s="248"/>
+      <c r="K27" s="248"/>
+      <c r="L27" s="248"/>
       <c r="N27" s="57"/>
       <c r="O27" s="210"/>
       <c r="P27" s="210"/>
@@ -14904,7 +15021,7 @@
       <c r="X27" s="23"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A28" s="264">
+      <c r="A28" s="282">
         <v>2</v>
       </c>
       <c r="B28" s="53" t="s">
@@ -14913,7 +15030,7 @@
       <c r="C28" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="D28" s="265">
+      <c r="D28" s="283">
         <v>4</v>
       </c>
       <c r="E28" s="53" t="s">
@@ -14922,49 +15039,49 @@
       <c r="F28" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="H28" s="247"/>
-      <c r="I28" s="247"/>
-      <c r="J28" s="247"/>
-      <c r="K28" s="247"/>
-      <c r="L28" s="247"/>
-      <c r="N28" s="268" t="s">
-        <v>180</v>
-      </c>
-      <c r="O28" s="268"/>
-      <c r="P28" s="268"/>
-      <c r="Q28" s="268"/>
-      <c r="R28" s="268"/>
+      <c r="H28" s="248"/>
+      <c r="I28" s="248"/>
+      <c r="J28" s="248"/>
+      <c r="K28" s="248"/>
+      <c r="L28" s="248"/>
+      <c r="N28" s="286" t="s">
+        <v>179</v>
+      </c>
+      <c r="O28" s="286"/>
+      <c r="P28" s="286"/>
+      <c r="Q28" s="286"/>
+      <c r="R28" s="286"/>
       <c r="S28" s="58"/>
-      <c r="T28" s="269" t="s">
-        <v>179</v>
-      </c>
-      <c r="U28" s="269"/>
-      <c r="V28" s="269"/>
-      <c r="W28" s="269"/>
-      <c r="X28" s="269"/>
+      <c r="T28" s="287" t="s">
+        <v>178</v>
+      </c>
+      <c r="U28" s="287"/>
+      <c r="V28" s="287"/>
+      <c r="W28" s="287"/>
+      <c r="X28" s="287"/>
     </row>
     <row r="29" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="264"/>
+      <c r="A29" s="282"/>
       <c r="B29" s="55" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="265"/>
+      <c r="D29" s="283"/>
       <c r="E29" s="55" t="s">
         <v>15</v>
       </c>
       <c r="F29" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="266" t="s">
+      <c r="H29" s="284" t="s">
         <v>66</v>
       </c>
-      <c r="I29" s="266"/>
-      <c r="J29" s="266"/>
-      <c r="K29" s="266"/>
-      <c r="L29" s="266"/>
+      <c r="I29" s="284"/>
+      <c r="J29" s="284"/>
+      <c r="K29" s="284"/>
+      <c r="L29" s="284"/>
       <c r="N29" s="59"/>
       <c r="O29" s="59"/>
       <c r="P29" s="58"/>
@@ -15009,7 +15126,7 @@
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B33" s="232" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>6</v>
@@ -15024,7 +15141,7 @@
         <v>12</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I33" s="220" t="s">
         <v>15</v>
@@ -15054,7 +15171,7 @@
         <v>13</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I35" s="220" t="s">
         <v>15</v>
@@ -15062,7 +15179,7 @@
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B36" s="227" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>6</v>
@@ -15092,7 +15209,7 @@
         <v>14</v>
       </c>
       <c r="H37" s="221" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I37" s="222" t="s">
         <v>16</v>
@@ -15106,10 +15223,10 @@
     </row>
     <row r="39" spans="2:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" s="227" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>16</v>
@@ -15117,11 +15234,11 @@
       <c r="E39" s="220" t="s">
         <v>9</v>
       </c>
-      <c r="G39" s="247" t="s">
-        <v>190</v>
-      </c>
-      <c r="H39" s="247"/>
-      <c r="I39" s="247"/>
+      <c r="G39" s="248" t="s">
+        <v>189</v>
+      </c>
+      <c r="H39" s="248"/>
+      <c r="I39" s="248"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B40" s="223"/>
@@ -15134,9 +15251,9 @@
       <c r="E40" s="220" t="s">
         <v>8</v>
       </c>
-      <c r="G40" s="247"/>
-      <c r="H40" s="247"/>
-      <c r="I40" s="247"/>
+      <c r="G40" s="248"/>
+      <c r="H40" s="248"/>
+      <c r="I40" s="248"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B41" s="225"/>
@@ -15149,7 +15266,7 @@
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B42" s="227" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>6</v>
@@ -15170,7 +15287,7 @@
         <v>7</v>
       </c>
       <c r="D43" s="221" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E43" s="222" t="s">
         <v>8</v>
@@ -15181,28 +15298,36 @@
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="W11:X11"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="T26:U26"/>
-    <mergeCell ref="W22:X22"/>
-    <mergeCell ref="W24:X24"/>
-    <mergeCell ref="W26:X26"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="T2:X2"/>
-    <mergeCell ref="Z3:AB5"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="N3:R3"/>
-    <mergeCell ref="T3:X3"/>
+    <mergeCell ref="G39:I40"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="Z23:AB25"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="H23:L28"/>
+    <mergeCell ref="N28:R28"/>
+    <mergeCell ref="T28:X28"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="Z19:AB21"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="H14:L14"/>
+    <mergeCell ref="W13:X13"/>
+    <mergeCell ref="Z15:AB17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="W15:X15"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="W17:X17"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="T15:U15"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="Z7:AB9"/>
     <mergeCell ref="C8:F8"/>
@@ -15219,36 +15344,28 @@
     <mergeCell ref="Q11:R11"/>
     <mergeCell ref="T11:U11"/>
     <mergeCell ref="T13:U13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="H14:L14"/>
-    <mergeCell ref="W13:X13"/>
-    <mergeCell ref="Z15:AB17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="W15:X15"/>
-    <mergeCell ref="T17:U17"/>
-    <mergeCell ref="W17:X17"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="T15:U15"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="Z19:AB21"/>
-    <mergeCell ref="G39:I40"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="H29:L29"/>
-    <mergeCell ref="Z23:AB25"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="H23:L28"/>
-    <mergeCell ref="N28:R28"/>
-    <mergeCell ref="T28:X28"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="T2:X2"/>
+    <mergeCell ref="Z3:AB5"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="N3:R3"/>
+    <mergeCell ref="T3:X3"/>
+    <mergeCell ref="W11:X11"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="T26:U26"/>
+    <mergeCell ref="W22:X22"/>
+    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="W26:X26"/>
   </mergeCells>
   <pageMargins left="2.56" right="2.15" top="0.75" bottom="0.75" header="0.61" footer="0.3"/>
   <pageSetup scale="32" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -15263,7 +15380,7 @@
   </sheetPr>
   <dimension ref="B2:S38"/>
   <sheetViews>
-    <sheetView zoomScale="77" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="D2" zoomScale="77" workbookViewId="0">
       <selection activeCell="B7" sqref="B7:M11"/>
     </sheetView>
   </sheetViews>
@@ -15277,10 +15394,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B2" s="281" t="s">
+      <c r="B2" s="289" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="281"/>
+      <c r="C2" s="289"/>
       <c r="D2" s="60"/>
       <c r="E2" s="60"/>
       <c r="F2" s="60"/>
@@ -15294,28 +15411,28 @@
       <c r="N2" s="60"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B3" s="249" t="s">
+      <c r="B3" s="263" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="249"/>
-      <c r="D3" s="249"/>
-      <c r="E3" s="249"/>
-      <c r="F3" s="249"/>
-      <c r="G3" s="249"/>
-      <c r="H3" s="249"/>
-      <c r="I3" s="249"/>
-      <c r="J3" s="249"/>
-      <c r="K3" s="249"/>
-      <c r="L3" s="249"/>
-      <c r="M3" s="249"/>
+      <c r="C3" s="263"/>
+      <c r="D3" s="263"/>
+      <c r="E3" s="263"/>
+      <c r="F3" s="263"/>
+      <c r="G3" s="263"/>
+      <c r="H3" s="263"/>
+      <c r="I3" s="263"/>
+      <c r="J3" s="263"/>
+      <c r="K3" s="263"/>
+      <c r="L3" s="263"/>
+      <c r="M3" s="263"/>
       <c r="N3" s="60"/>
-      <c r="O3" s="248" t="s">
+      <c r="O3" s="268" t="s">
         <v>147</v>
       </c>
-      <c r="P3" s="248"/>
-      <c r="Q3" s="248"/>
-      <c r="R3" s="248"/>
-      <c r="S3" s="249"/>
+      <c r="P3" s="268"/>
+      <c r="Q3" s="268"/>
+      <c r="R3" s="268"/>
+      <c r="S3" s="263"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B4" s="62">
@@ -15355,164 +15472,164 @@
         <v>12</v>
       </c>
       <c r="N4" s="127"/>
-      <c r="O4" s="248"/>
-      <c r="P4" s="248"/>
-      <c r="Q4" s="248"/>
-      <c r="R4" s="248"/>
-      <c r="S4" s="249"/>
+      <c r="O4" s="268"/>
+      <c r="P4" s="268"/>
+      <c r="Q4" s="268"/>
+      <c r="R4" s="268"/>
+      <c r="S4" s="263"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B5" s="282" t="s">
+      <c r="B5" s="290" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="250"/>
-      <c r="D5" s="282" t="s">
+      <c r="C5" s="291"/>
+      <c r="D5" s="290" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="250"/>
-      <c r="F5" s="282" t="s">
+      <c r="E5" s="291"/>
+      <c r="F5" s="290" t="s">
         <v>69</v>
       </c>
-      <c r="G5" s="250"/>
-      <c r="H5" s="282" t="s">
+      <c r="G5" s="291"/>
+      <c r="H5" s="290" t="s">
         <v>70</v>
       </c>
-      <c r="I5" s="250"/>
-      <c r="J5" s="282" t="s">
+      <c r="I5" s="291"/>
+      <c r="J5" s="290" t="s">
         <v>69</v>
       </c>
-      <c r="K5" s="283"/>
-      <c r="L5" s="282" t="s">
+      <c r="K5" s="292"/>
+      <c r="L5" s="290" t="s">
         <v>70</v>
       </c>
-      <c r="M5" s="283"/>
+      <c r="M5" s="292"/>
       <c r="N5" s="60"/>
-      <c r="S5" s="249"/>
+      <c r="S5" s="263"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B6" s="63"/>
-      <c r="O6" s="247" t="s">
+      <c r="O6" s="248" t="s">
         <v>149</v>
       </c>
-      <c r="P6" s="247"/>
-      <c r="Q6" s="247"/>
-      <c r="R6" s="247"/>
-      <c r="S6" s="249"/>
+      <c r="P6" s="248"/>
+      <c r="Q6" s="248"/>
+      <c r="R6" s="248"/>
+      <c r="S6" s="263"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B7" s="247" t="s">
-        <v>191</v>
-      </c>
-      <c r="C7" s="247"/>
-      <c r="D7" s="247"/>
-      <c r="E7" s="247"/>
-      <c r="F7" s="247"/>
-      <c r="G7" s="247"/>
-      <c r="H7" s="247"/>
-      <c r="I7" s="247"/>
-      <c r="J7" s="247"/>
-      <c r="K7" s="247"/>
-      <c r="L7" s="247"/>
-      <c r="M7" s="247"/>
+      <c r="B7" s="248" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7" s="248"/>
+      <c r="D7" s="248"/>
+      <c r="E7" s="248"/>
+      <c r="F7" s="248"/>
+      <c r="G7" s="248"/>
+      <c r="H7" s="248"/>
+      <c r="I7" s="248"/>
+      <c r="J7" s="248"/>
+      <c r="K7" s="248"/>
+      <c r="L7" s="248"/>
+      <c r="M7" s="248"/>
       <c r="N7" s="141"/>
-      <c r="O7" s="247"/>
-      <c r="P7" s="247"/>
-      <c r="Q7" s="247"/>
-      <c r="R7" s="247"/>
-      <c r="S7" s="249"/>
+      <c r="O7" s="248"/>
+      <c r="P7" s="248"/>
+      <c r="Q7" s="248"/>
+      <c r="R7" s="248"/>
+      <c r="S7" s="263"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B8" s="247"/>
-      <c r="C8" s="247"/>
-      <c r="D8" s="247"/>
-      <c r="E8" s="247"/>
-      <c r="F8" s="247"/>
-      <c r="G8" s="247"/>
-      <c r="H8" s="247"/>
-      <c r="I8" s="247"/>
-      <c r="J8" s="247"/>
-      <c r="K8" s="247"/>
-      <c r="L8" s="247"/>
-      <c r="M8" s="247"/>
+      <c r="B8" s="248"/>
+      <c r="C8" s="248"/>
+      <c r="D8" s="248"/>
+      <c r="E8" s="248"/>
+      <c r="F8" s="248"/>
+      <c r="G8" s="248"/>
+      <c r="H8" s="248"/>
+      <c r="I8" s="248"/>
+      <c r="J8" s="248"/>
+      <c r="K8" s="248"/>
+      <c r="L8" s="248"/>
+      <c r="M8" s="248"/>
       <c r="N8" s="141"/>
-      <c r="O8" s="247"/>
-      <c r="P8" s="247"/>
-      <c r="Q8" s="247"/>
-      <c r="R8" s="247"/>
-      <c r="S8" s="249"/>
+      <c r="O8" s="248"/>
+      <c r="P8" s="248"/>
+      <c r="Q8" s="248"/>
+      <c r="R8" s="248"/>
+      <c r="S8" s="263"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B9" s="247"/>
-      <c r="C9" s="247"/>
-      <c r="D9" s="247"/>
-      <c r="E9" s="247"/>
-      <c r="F9" s="247"/>
-      <c r="G9" s="247"/>
-      <c r="H9" s="247"/>
-      <c r="I9" s="247"/>
-      <c r="J9" s="247"/>
-      <c r="K9" s="247"/>
-      <c r="L9" s="247"/>
-      <c r="M9" s="247"/>
+      <c r="B9" s="248"/>
+      <c r="C9" s="248"/>
+      <c r="D9" s="248"/>
+      <c r="E9" s="248"/>
+      <c r="F9" s="248"/>
+      <c r="G9" s="248"/>
+      <c r="H9" s="248"/>
+      <c r="I9" s="248"/>
+      <c r="J9" s="248"/>
+      <c r="K9" s="248"/>
+      <c r="L9" s="248"/>
+      <c r="M9" s="248"/>
       <c r="N9" s="141"/>
-      <c r="O9" s="247"/>
-      <c r="P9" s="247"/>
-      <c r="Q9" s="247"/>
-      <c r="R9" s="247"/>
-      <c r="S9" s="249"/>
+      <c r="O9" s="248"/>
+      <c r="P9" s="248"/>
+      <c r="Q9" s="248"/>
+      <c r="R9" s="248"/>
+      <c r="S9" s="263"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B10" s="247"/>
-      <c r="C10" s="247"/>
-      <c r="D10" s="247"/>
-      <c r="E10" s="247"/>
-      <c r="F10" s="247"/>
-      <c r="G10" s="247"/>
-      <c r="H10" s="247"/>
-      <c r="I10" s="247"/>
-      <c r="J10" s="247"/>
-      <c r="K10" s="247"/>
-      <c r="L10" s="247"/>
-      <c r="M10" s="247"/>
+      <c r="B10" s="248"/>
+      <c r="C10" s="248"/>
+      <c r="D10" s="248"/>
+      <c r="E10" s="248"/>
+      <c r="F10" s="248"/>
+      <c r="G10" s="248"/>
+      <c r="H10" s="248"/>
+      <c r="I10" s="248"/>
+      <c r="J10" s="248"/>
+      <c r="K10" s="248"/>
+      <c r="L10" s="248"/>
+      <c r="M10" s="248"/>
       <c r="N10" s="141"/>
-      <c r="O10" s="247"/>
-      <c r="P10" s="247"/>
-      <c r="Q10" s="247"/>
-      <c r="R10" s="247"/>
-      <c r="S10" s="249"/>
+      <c r="O10" s="248"/>
+      <c r="P10" s="248"/>
+      <c r="Q10" s="248"/>
+      <c r="R10" s="248"/>
+      <c r="S10" s="263"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B11" s="247"/>
-      <c r="C11" s="247"/>
-      <c r="D11" s="247"/>
-      <c r="E11" s="247"/>
-      <c r="F11" s="247"/>
-      <c r="G11" s="247"/>
-      <c r="H11" s="247"/>
-      <c r="I11" s="247"/>
-      <c r="J11" s="247"/>
-      <c r="K11" s="247"/>
-      <c r="L11" s="247"/>
-      <c r="M11" s="247"/>
+      <c r="B11" s="248"/>
+      <c r="C11" s="248"/>
+      <c r="D11" s="248"/>
+      <c r="E11" s="248"/>
+      <c r="F11" s="248"/>
+      <c r="G11" s="248"/>
+      <c r="H11" s="248"/>
+      <c r="I11" s="248"/>
+      <c r="J11" s="248"/>
+      <c r="K11" s="248"/>
+      <c r="L11" s="248"/>
+      <c r="M11" s="248"/>
       <c r="N11" s="141"/>
-      <c r="O11" s="247"/>
-      <c r="P11" s="247"/>
-      <c r="Q11" s="247"/>
-      <c r="R11" s="247"/>
-      <c r="S11" s="249"/>
+      <c r="O11" s="248"/>
+      <c r="P11" s="248"/>
+      <c r="Q11" s="248"/>
+      <c r="R11" s="248"/>
+      <c r="S11" s="263"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="O12" s="247"/>
-      <c r="P12" s="247"/>
-      <c r="Q12" s="247"/>
-      <c r="R12" s="247"/>
-      <c r="S12" s="249"/>
+      <c r="O12" s="248"/>
+      <c r="P12" s="248"/>
+      <c r="Q12" s="248"/>
+      <c r="R12" s="248"/>
+      <c r="S12" s="263"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B13" s="280" t="s">
+      <c r="B13" s="288" t="s">
         <v>153</v>
       </c>
-      <c r="C13" s="280"/>
+      <c r="C13" s="288"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B14" s="60">
@@ -15529,12 +15646,12 @@
       <c r="C15" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="O15" s="247" t="s">
+      <c r="O15" s="248" t="s">
         <v>148</v>
       </c>
-      <c r="P15" s="247"/>
-      <c r="Q15" s="247"/>
-      <c r="R15" s="247"/>
+      <c r="P15" s="248"/>
+      <c r="Q15" s="248"/>
+      <c r="R15" s="248"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B16" s="60">
@@ -15543,10 +15660,10 @@
       <c r="C16" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="O16" s="247"/>
-      <c r="P16" s="247"/>
-      <c r="Q16" s="247"/>
-      <c r="R16" s="247"/>
+      <c r="O16" s="248"/>
+      <c r="P16" s="248"/>
+      <c r="Q16" s="248"/>
+      <c r="R16" s="248"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B17" s="60">
@@ -15563,12 +15680,12 @@
       <c r="C18" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="O18" s="247" t="s">
+      <c r="O18" s="248" t="s">
         <v>150</v>
       </c>
-      <c r="P18" s="247"/>
-      <c r="Q18" s="247"/>
-      <c r="R18" s="247"/>
+      <c r="P18" s="248"/>
+      <c r="Q18" s="248"/>
+      <c r="R18" s="248"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B19" s="60">
@@ -15577,97 +15694,97 @@
       <c r="C19" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="O19" s="247"/>
-      <c r="P19" s="247"/>
-      <c r="Q19" s="247"/>
-      <c r="R19" s="247"/>
+      <c r="O19" s="248"/>
+      <c r="P19" s="248"/>
+      <c r="Q19" s="248"/>
+      <c r="R19" s="248"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O20" s="247"/>
-      <c r="P20" s="247"/>
-      <c r="Q20" s="247"/>
-      <c r="R20" s="247"/>
+      <c r="O20" s="248"/>
+      <c r="P20" s="248"/>
+      <c r="Q20" s="248"/>
+      <c r="R20" s="248"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O21" s="247"/>
-      <c r="P21" s="247"/>
-      <c r="Q21" s="247"/>
-      <c r="R21" s="247"/>
+      <c r="O21" s="248"/>
+      <c r="P21" s="248"/>
+      <c r="Q21" s="248"/>
+      <c r="R21" s="248"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O22" s="247"/>
-      <c r="P22" s="247"/>
-      <c r="Q22" s="247"/>
-      <c r="R22" s="247"/>
+      <c r="O22" s="248"/>
+      <c r="P22" s="248"/>
+      <c r="Q22" s="248"/>
+      <c r="R22" s="248"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O23" s="247"/>
-      <c r="P23" s="247"/>
-      <c r="Q23" s="247"/>
-      <c r="R23" s="247"/>
+      <c r="O23" s="248"/>
+      <c r="P23" s="248"/>
+      <c r="Q23" s="248"/>
+      <c r="R23" s="248"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O27" s="248" t="s">
+      <c r="O27" s="268" t="s">
         <v>146</v>
       </c>
-      <c r="P27" s="248"/>
-      <c r="Q27" s="248"/>
-      <c r="R27" s="248"/>
+      <c r="P27" s="268"/>
+      <c r="Q27" s="268"/>
+      <c r="R27" s="268"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O28" s="248"/>
-      <c r="P28" s="248"/>
-      <c r="Q28" s="248"/>
-      <c r="R28" s="248"/>
+      <c r="O28" s="268"/>
+      <c r="P28" s="268"/>
+      <c r="Q28" s="268"/>
+      <c r="R28" s="268"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O30" s="247" t="s">
+      <c r="O30" s="248" t="s">
         <v>145</v>
       </c>
-      <c r="P30" s="247"/>
-      <c r="Q30" s="247"/>
-      <c r="R30" s="247"/>
+      <c r="P30" s="248"/>
+      <c r="Q30" s="248"/>
+      <c r="R30" s="248"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O31" s="247"/>
-      <c r="P31" s="247"/>
-      <c r="Q31" s="247"/>
-      <c r="R31" s="247"/>
+      <c r="O31" s="248"/>
+      <c r="P31" s="248"/>
+      <c r="Q31" s="248"/>
+      <c r="R31" s="248"/>
     </row>
     <row r="32" spans="2:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M32" s="73"/>
       <c r="N32" s="73"/>
-      <c r="O32" s="247"/>
-      <c r="P32" s="247"/>
-      <c r="Q32" s="247"/>
-      <c r="R32" s="247"/>
+      <c r="O32" s="248"/>
+      <c r="P32" s="248"/>
+      <c r="Q32" s="248"/>
+      <c r="R32" s="248"/>
     </row>
     <row r="33" spans="12:18" x14ac:dyDescent="0.35">
       <c r="L33" s="73"/>
       <c r="M33" s="73"/>
       <c r="N33" s="73"/>
-      <c r="O33" s="247"/>
-      <c r="P33" s="247"/>
-      <c r="Q33" s="247"/>
-      <c r="R33" s="247"/>
+      <c r="O33" s="248"/>
+      <c r="P33" s="248"/>
+      <c r="Q33" s="248"/>
+      <c r="R33" s="248"/>
     </row>
     <row r="34" spans="12:18" x14ac:dyDescent="0.35">
       <c r="L34" s="73"/>
       <c r="M34" s="73"/>
       <c r="N34" s="73"/>
-      <c r="O34" s="247"/>
-      <c r="P34" s="247"/>
-      <c r="Q34" s="247"/>
-      <c r="R34" s="247"/>
+      <c r="O34" s="248"/>
+      <c r="P34" s="248"/>
+      <c r="Q34" s="248"/>
+      <c r="R34" s="248"/>
     </row>
     <row r="35" spans="12:18" x14ac:dyDescent="0.35">
       <c r="L35" s="73"/>
       <c r="M35" s="73"/>
       <c r="N35" s="73"/>
-      <c r="O35" s="247"/>
-      <c r="P35" s="247"/>
-      <c r="Q35" s="247"/>
-      <c r="R35" s="247"/>
+      <c r="O35" s="248"/>
+      <c r="P35" s="248"/>
+      <c r="Q35" s="248"/>
+      <c r="R35" s="248"/>
     </row>
     <row r="36" spans="12:18" x14ac:dyDescent="0.35">
       <c r="L36" s="73"/>
@@ -15695,6 +15812,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="O30:R35"/>
+    <mergeCell ref="O15:R16"/>
+    <mergeCell ref="O3:R4"/>
+    <mergeCell ref="O18:R23"/>
+    <mergeCell ref="O6:R12"/>
     <mergeCell ref="B7:M11"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="S3:S12"/>
@@ -15707,11 +15829,6 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="L5:M5"/>
-    <mergeCell ref="O30:R35"/>
-    <mergeCell ref="O15:R16"/>
-    <mergeCell ref="O3:R4"/>
-    <mergeCell ref="O18:R23"/>
-    <mergeCell ref="O6:R12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="55" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -15726,8 +15843,8 @@
   </sheetPr>
   <dimension ref="B3:R23"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="81" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -15739,57 +15856,57 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:18" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B3" s="289" t="s">
+      <c r="B3" s="295" t="s">
         <v>154</v>
       </c>
-      <c r="C3" s="293"/>
-      <c r="D3" s="293"/>
-      <c r="E3" s="293"/>
-      <c r="F3" s="289" t="s">
+      <c r="C3" s="269"/>
+      <c r="D3" s="269"/>
+      <c r="E3" s="269"/>
+      <c r="F3" s="295" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="289"/>
-      <c r="H3" s="289"/>
-      <c r="I3" s="289"/>
-      <c r="J3" s="289"/>
-      <c r="K3" s="289"/>
-      <c r="L3" s="289"/>
-      <c r="M3" s="289"/>
-      <c r="N3" s="289"/>
-      <c r="O3" s="289"/>
-      <c r="P3" s="289"/>
-      <c r="Q3" s="289"/>
+      <c r="G3" s="295"/>
+      <c r="H3" s="295"/>
+      <c r="I3" s="295"/>
+      <c r="J3" s="295"/>
+      <c r="K3" s="295"/>
+      <c r="L3" s="295"/>
+      <c r="M3" s="295"/>
+      <c r="N3" s="295"/>
+      <c r="O3" s="295"/>
+      <c r="P3" s="295"/>
+      <c r="Q3" s="295"/>
     </row>
     <row r="4" spans="2:18" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B4" s="297" t="s">
+      <c r="B4" s="299" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" s="299"/>
+      <c r="D4" s="299"/>
+      <c r="E4" s="299"/>
+      <c r="F4" s="299" t="s">
         <v>162</v>
       </c>
-      <c r="C4" s="297"/>
-      <c r="D4" s="297"/>
-      <c r="E4" s="297"/>
-      <c r="F4" s="297" t="s">
-        <v>163</v>
-      </c>
-      <c r="G4" s="297"/>
-      <c r="H4" s="297"/>
-      <c r="I4" s="297"/>
-      <c r="J4" s="297"/>
-      <c r="K4" s="297"/>
-      <c r="L4" s="297"/>
-      <c r="M4" s="297"/>
-      <c r="N4" s="297"/>
-      <c r="O4" s="297"/>
-      <c r="P4" s="297"/>
-      <c r="Q4" s="297"/>
+      <c r="G4" s="299"/>
+      <c r="H4" s="299"/>
+      <c r="I4" s="299"/>
+      <c r="J4" s="299"/>
+      <c r="K4" s="299"/>
+      <c r="L4" s="299"/>
+      <c r="M4" s="299"/>
+      <c r="N4" s="299"/>
+      <c r="O4" s="299"/>
+      <c r="P4" s="299"/>
+      <c r="Q4" s="299"/>
       <c r="R4" s="172"/>
     </row>
     <row r="5" spans="2:18" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="294">
+      <c r="B5" s="318">
         <v>80</v>
       </c>
-      <c r="C5" s="295"/>
-      <c r="D5" s="295"/>
-      <c r="E5" s="296"/>
+      <c r="C5" s="319"/>
+      <c r="D5" s="319"/>
+      <c r="E5" s="320"/>
       <c r="F5" s="171">
         <v>6</v>
       </c>
@@ -15867,29 +15984,29 @@
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B8" s="173"/>
-      <c r="C8" s="292" t="s">
+      <c r="C8" s="298" t="s">
         <v>157</v>
       </c>
-      <c r="D8" s="292"/>
+      <c r="D8" s="298"/>
       <c r="E8" s="163"/>
       <c r="F8" s="178"/>
       <c r="G8" s="179"/>
-      <c r="H8" s="287" t="s">
+      <c r="H8" s="293" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="288"/>
+      <c r="I8" s="294"/>
       <c r="J8" s="178"/>
       <c r="K8" s="179"/>
-      <c r="L8" s="287" t="s">
+      <c r="L8" s="293" t="s">
         <v>70</v>
       </c>
-      <c r="M8" s="288"/>
+      <c r="M8" s="294"/>
       <c r="N8" s="178"/>
       <c r="O8" s="179"/>
-      <c r="P8" s="290" t="s">
+      <c r="P8" s="296" t="s">
         <v>70</v>
       </c>
-      <c r="Q8" s="291"/>
+      <c r="Q8" s="297"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B9" s="207"/>
@@ -15900,22 +16017,22 @@
         <v>20</v>
       </c>
       <c r="E9" s="165"/>
-      <c r="F9" s="285" t="s">
+      <c r="F9" s="302" t="s">
         <v>69</v>
       </c>
-      <c r="G9" s="285"/>
+      <c r="G9" s="302"/>
       <c r="H9" s="181"/>
       <c r="I9" s="182"/>
-      <c r="J9" s="285" t="s">
+      <c r="J9" s="302" t="s">
         <v>69</v>
       </c>
-      <c r="K9" s="285"/>
+      <c r="K9" s="302"/>
       <c r="L9" s="183"/>
       <c r="M9" s="183"/>
-      <c r="N9" s="285" t="s">
+      <c r="N9" s="302" t="s">
         <v>69</v>
       </c>
-      <c r="O9" s="285"/>
+      <c r="O9" s="302"/>
       <c r="P9" s="183"/>
       <c r="Q9" s="183"/>
     </row>
@@ -15946,27 +16063,27 @@
       <c r="C11" s="167"/>
       <c r="D11" s="167"/>
       <c r="E11" s="167"/>
-      <c r="F11" s="298" t="s">
-        <v>166</v>
-      </c>
-      <c r="G11" s="298"/>
-      <c r="H11" s="298"/>
-      <c r="I11" s="298"/>
-      <c r="J11" s="298"/>
-      <c r="K11" s="298"/>
-      <c r="L11" s="298"/>
-      <c r="M11" s="298"/>
-      <c r="N11" s="298"/>
-      <c r="O11" s="298"/>
-      <c r="P11" s="298"/>
-      <c r="Q11" s="298"/>
+      <c r="F11" s="300" t="s">
+        <v>165</v>
+      </c>
+      <c r="G11" s="300"/>
+      <c r="H11" s="300"/>
+      <c r="I11" s="300"/>
+      <c r="J11" s="300"/>
+      <c r="K11" s="300"/>
+      <c r="L11" s="300"/>
+      <c r="M11" s="300"/>
+      <c r="N11" s="300"/>
+      <c r="O11" s="300"/>
+      <c r="P11" s="300"/>
+      <c r="Q11" s="300"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B12" s="168"/>
-      <c r="C12" s="292" t="s">
+      <c r="C12" s="298" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="292"/>
+      <c r="D12" s="298"/>
       <c r="E12" s="168"/>
       <c r="F12" s="191"/>
       <c r="G12" s="191"/>
@@ -15993,15 +16110,15 @@
       <c r="F13" s="191"/>
       <c r="G13" s="191"/>
       <c r="H13" s="191"/>
-      <c r="I13" s="284" t="s">
-        <v>168</v>
-      </c>
-      <c r="J13" s="284"/>
-      <c r="K13" s="284"/>
-      <c r="L13" s="284"/>
-      <c r="M13" s="284"/>
-      <c r="N13" s="284"/>
-      <c r="O13" s="284"/>
+      <c r="I13" s="301" t="s">
+        <v>167</v>
+      </c>
+      <c r="J13" s="301"/>
+      <c r="K13" s="301"/>
+      <c r="L13" s="301"/>
+      <c r="M13" s="301"/>
+      <c r="N13" s="301"/>
+      <c r="O13" s="301"/>
       <c r="P13" s="192"/>
       <c r="Q13" s="192"/>
     </row>
@@ -16019,13 +16136,13 @@
       <c r="H14" s="191"/>
       <c r="I14" s="193"/>
       <c r="J14" s="206" t="s">
+        <v>168</v>
+      </c>
+      <c r="K14" s="305"/>
+      <c r="L14" s="305"/>
+      <c r="M14" s="305"/>
+      <c r="N14" s="206" t="s">
         <v>169</v>
-      </c>
-      <c r="K14" s="300"/>
-      <c r="L14" s="300"/>
-      <c r="M14" s="300"/>
-      <c r="N14" s="206" t="s">
-        <v>170</v>
       </c>
       <c r="O14" s="194"/>
       <c r="P14" s="191"/>
@@ -16044,7 +16161,7 @@
       <c r="G15" s="191"/>
       <c r="H15" s="192"/>
       <c r="I15" s="195" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J15" s="205"/>
       <c r="K15" s="202"/>
@@ -16052,7 +16169,7 @@
       <c r="M15" s="203"/>
       <c r="N15" s="204"/>
       <c r="O15" s="195" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P15" s="191"/>
       <c r="Q15" s="191"/>
@@ -16100,13 +16217,13 @@
       <c r="G17" s="191"/>
       <c r="H17" s="191"/>
       <c r="I17" s="199"/>
-      <c r="J17" s="299" t="s">
-        <v>167</v>
-      </c>
-      <c r="K17" s="299"/>
-      <c r="L17" s="299"/>
-      <c r="M17" s="299"/>
-      <c r="N17" s="299"/>
+      <c r="J17" s="304" t="s">
+        <v>166</v>
+      </c>
+      <c r="K17" s="304"/>
+      <c r="L17" s="304"/>
+      <c r="M17" s="304"/>
+      <c r="N17" s="304"/>
       <c r="O17" s="200"/>
       <c r="P17" s="191"/>
       <c r="Q17" s="191"/>
@@ -16144,63 +16261,70 @@
       <c r="Q19" s="191"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B21" s="286" t="s">
-        <v>181</v>
-      </c>
-      <c r="C21" s="286"/>
-      <c r="D21" s="286"/>
-      <c r="E21" s="286"/>
-      <c r="F21" s="286"/>
-      <c r="G21" s="286"/>
-      <c r="H21" s="286"/>
-      <c r="I21" s="286"/>
-      <c r="J21" s="286"/>
-      <c r="K21" s="286"/>
-      <c r="L21" s="286"/>
-      <c r="M21" s="286"/>
-      <c r="N21" s="286"/>
-      <c r="O21" s="286"/>
-      <c r="P21" s="286"/>
-      <c r="Q21" s="286"/>
+      <c r="B21" s="303" t="s">
+        <v>180</v>
+      </c>
+      <c r="C21" s="303"/>
+      <c r="D21" s="303"/>
+      <c r="E21" s="303"/>
+      <c r="F21" s="303"/>
+      <c r="G21" s="303"/>
+      <c r="H21" s="303"/>
+      <c r="I21" s="303"/>
+      <c r="J21" s="303"/>
+      <c r="K21" s="303"/>
+      <c r="L21" s="303"/>
+      <c r="M21" s="303"/>
+      <c r="N21" s="303"/>
+      <c r="O21" s="303"/>
+      <c r="P21" s="303"/>
+      <c r="Q21" s="303"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B22" s="286"/>
-      <c r="C22" s="286"/>
-      <c r="D22" s="286"/>
-      <c r="E22" s="286"/>
-      <c r="F22" s="286"/>
-      <c r="G22" s="286"/>
-      <c r="H22" s="286"/>
-      <c r="I22" s="286"/>
-      <c r="J22" s="286"/>
-      <c r="K22" s="286"/>
-      <c r="L22" s="286"/>
-      <c r="M22" s="286"/>
-      <c r="N22" s="286"/>
-      <c r="O22" s="286"/>
-      <c r="P22" s="286"/>
-      <c r="Q22" s="286"/>
+      <c r="B22" s="303"/>
+      <c r="C22" s="303"/>
+      <c r="D22" s="303"/>
+      <c r="E22" s="303"/>
+      <c r="F22" s="303"/>
+      <c r="G22" s="303"/>
+      <c r="H22" s="303"/>
+      <c r="I22" s="303"/>
+      <c r="J22" s="303"/>
+      <c r="K22" s="303"/>
+      <c r="L22" s="303"/>
+      <c r="M22" s="303"/>
+      <c r="N22" s="303"/>
+      <c r="O22" s="303"/>
+      <c r="P22" s="303"/>
+      <c r="Q22" s="303"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B23" s="286"/>
-      <c r="C23" s="286"/>
-      <c r="D23" s="286"/>
-      <c r="E23" s="286"/>
-      <c r="F23" s="286"/>
-      <c r="G23" s="286"/>
-      <c r="H23" s="286"/>
-      <c r="I23" s="286"/>
-      <c r="J23" s="286"/>
-      <c r="K23" s="286"/>
-      <c r="L23" s="286"/>
-      <c r="M23" s="286"/>
-      <c r="N23" s="286"/>
-      <c r="O23" s="286"/>
-      <c r="P23" s="286"/>
-      <c r="Q23" s="286"/>
+      <c r="B23" s="303"/>
+      <c r="C23" s="303"/>
+      <c r="D23" s="303"/>
+      <c r="E23" s="303"/>
+      <c r="F23" s="303"/>
+      <c r="G23" s="303"/>
+      <c r="H23" s="303"/>
+      <c r="I23" s="303"/>
+      <c r="J23" s="303"/>
+      <c r="K23" s="303"/>
+      <c r="L23" s="303"/>
+      <c r="M23" s="303"/>
+      <c r="N23" s="303"/>
+      <c r="O23" s="303"/>
+      <c r="P23" s="303"/>
+      <c r="Q23" s="303"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="17">
+    <mergeCell ref="I13:O13"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="B21:Q23"/>
+    <mergeCell ref="J17:N17"/>
+    <mergeCell ref="K14:M14"/>
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="F3:Q3"/>
     <mergeCell ref="H8:I8"/>
@@ -16208,19 +16332,322 @@
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B5:E5"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="F4:Q4"/>
     <mergeCell ref="F11:Q11"/>
-    <mergeCell ref="I13:O13"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="B21:Q23"/>
-    <mergeCell ref="J17:N17"/>
-    <mergeCell ref="K14:M14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8FBCA58-0396-46E3-8F1B-89C0F6C32117}">
+  <dimension ref="B2:X20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R12" sqref="R12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="8.7265625" style="313"/>
+    <col min="3" max="12" width="5.6328125" style="313" customWidth="1"/>
+    <col min="13" max="24" width="4.6328125" style="313" customWidth="1"/>
+    <col min="25" max="16384" width="8.7265625" style="313"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C2" s="315" t="s">
+        <v>206</v>
+      </c>
+      <c r="D2" s="315"/>
+      <c r="E2" s="315"/>
+      <c r="F2" s="315"/>
+      <c r="G2" s="315"/>
+      <c r="H2" s="315"/>
+      <c r="I2" s="315"/>
+      <c r="J2" s="315"/>
+      <c r="K2" s="315"/>
+      <c r="L2" s="315"/>
+      <c r="M2" s="315" t="s">
+        <v>207</v>
+      </c>
+      <c r="N2" s="315"/>
+      <c r="O2" s="315"/>
+      <c r="P2" s="315"/>
+      <c r="Q2" s="315"/>
+      <c r="R2" s="315"/>
+      <c r="S2" s="315"/>
+      <c r="T2" s="315"/>
+      <c r="U2" s="315"/>
+      <c r="V2" s="315"/>
+      <c r="W2" s="315"/>
+      <c r="X2" s="315"/>
+    </row>
+    <row r="3" spans="2:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="313" t="s">
+        <v>205</v>
+      </c>
+      <c r="C3" s="306">
+        <v>1</v>
+      </c>
+      <c r="D3" s="307">
+        <v>2</v>
+      </c>
+      <c r="E3" s="307">
+        <v>3</v>
+      </c>
+      <c r="F3" s="307">
+        <v>4</v>
+      </c>
+      <c r="G3" s="307">
+        <v>5</v>
+      </c>
+      <c r="H3" s="307">
+        <v>6</v>
+      </c>
+      <c r="I3" s="307">
+        <v>7</v>
+      </c>
+      <c r="J3" s="307">
+        <v>8</v>
+      </c>
+      <c r="K3" s="307">
+        <v>9</v>
+      </c>
+      <c r="L3" s="308">
+        <v>10</v>
+      </c>
+      <c r="M3" s="309">
+        <v>11</v>
+      </c>
+      <c r="N3" s="310">
+        <v>12</v>
+      </c>
+      <c r="O3" s="311">
+        <v>13</v>
+      </c>
+      <c r="P3" s="312">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="309">
+        <v>15</v>
+      </c>
+      <c r="R3" s="310">
+        <v>16</v>
+      </c>
+      <c r="S3" s="311">
+        <v>17</v>
+      </c>
+      <c r="T3" s="312">
+        <v>18</v>
+      </c>
+      <c r="U3" s="309">
+        <v>19</v>
+      </c>
+      <c r="V3" s="310">
+        <v>20</v>
+      </c>
+      <c r="W3" s="311">
+        <v>21</v>
+      </c>
+      <c r="X3" s="310">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="C4" s="316" t="s">
+        <v>221</v>
+      </c>
+      <c r="D4" s="316"/>
+      <c r="E4" s="316"/>
+      <c r="F4" s="316"/>
+      <c r="G4" s="316"/>
+      <c r="H4" s="316"/>
+      <c r="I4" s="316"/>
+      <c r="J4" s="316"/>
+      <c r="K4" s="316"/>
+      <c r="L4" s="316"/>
+      <c r="M4" s="317" t="s">
+        <v>222</v>
+      </c>
+      <c r="N4" s="317"/>
+      <c r="O4" s="317"/>
+      <c r="P4" s="317"/>
+      <c r="Q4" s="317"/>
+      <c r="R4" s="317"/>
+      <c r="S4" s="317"/>
+      <c r="T4" s="317"/>
+      <c r="U4" s="317"/>
+      <c r="V4" s="317"/>
+      <c r="W4" s="317"/>
+      <c r="X4" s="317"/>
+    </row>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="D5" s="313" t="s">
+        <v>211</v>
+      </c>
+      <c r="M5" s="313" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="E6" s="313" t="s">
+        <v>209</v>
+      </c>
+      <c r="N6" s="313" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="F7" s="313" t="s">
+        <v>210</v>
+      </c>
+      <c r="P7" s="313" t="s">
+        <v>226</v>
+      </c>
+      <c r="R7" s="313">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="G8" s="313" t="s">
+        <v>216</v>
+      </c>
+      <c r="I8" s="313" t="s">
+        <v>218</v>
+      </c>
+      <c r="P8" s="313" t="s">
+        <v>226</v>
+      </c>
+      <c r="R8" s="313">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="F9" s="313" t="s">
+        <v>220</v>
+      </c>
+      <c r="P9" s="313" t="s">
+        <v>226</v>
+      </c>
+      <c r="R9" s="313">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="G10" s="313" t="s">
+        <v>216</v>
+      </c>
+      <c r="I10" s="313" t="s">
+        <v>218</v>
+      </c>
+      <c r="P10" s="313" t="s">
+        <v>226</v>
+      </c>
+      <c r="R10" s="313">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="E11" s="313" t="s">
+        <v>212</v>
+      </c>
+      <c r="P11" s="313" t="s">
+        <v>226</v>
+      </c>
+      <c r="R11" s="313">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="F12" s="313" t="s">
+        <v>215</v>
+      </c>
+      <c r="P12" s="313" t="s">
+        <v>226</v>
+      </c>
+      <c r="R12" s="313">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="G13" s="314" t="s">
+        <v>216</v>
+      </c>
+      <c r="H13" s="314"/>
+      <c r="I13" s="313" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="G14" s="314" t="s">
+        <v>216</v>
+      </c>
+      <c r="H14" s="314"/>
+      <c r="I14" s="313" t="s">
+        <v>219</v>
+      </c>
+      <c r="O14" s="313" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="F15" s="313" t="s">
+        <v>214</v>
+      </c>
+      <c r="P15" s="313" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="16" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="G16" s="313" t="s">
+        <v>217</v>
+      </c>
+      <c r="I16" s="313" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="17" spans="6:9" x14ac:dyDescent="0.35">
+      <c r="G17" s="313" t="s">
+        <v>217</v>
+      </c>
+      <c r="I17" s="313" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="18" spans="6:9" x14ac:dyDescent="0.35">
+      <c r="F18" s="313" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="19" spans="6:9" x14ac:dyDescent="0.35">
+      <c r="G19" s="313" t="s">
+        <v>217</v>
+      </c>
+      <c r="I19" s="313" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="20" spans="6:9" x14ac:dyDescent="0.35">
+      <c r="G20" s="313" t="s">
+        <v>217</v>
+      </c>
+      <c r="I20" s="313" t="s">
+        <v>219</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C2:L2"/>
+    <mergeCell ref="M2:X2"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="C4:L4"/>
+    <mergeCell ref="M4:X4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Exp. B + joining data
</commit_message>
<xml_diff>
--- a/Writeups/Notes/Exp.1_Master.xlsx
+++ b/Writeups/Notes/Exp.1_Master.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel\Documents\SI.SP\writeups\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2570283B-114A-4D3C-8EEC-32AC3FC3D8F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1340D474-9A73-4EDD-9127-60F7902E0EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{6F4FE53E-24C5-4985-9E6F-6A265A63BA90}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6F4FE53E-24C5-4985-9E6F-6A265A63BA90}"/>
   </bookViews>
   <sheets>
-    <sheet name="Exposure Phase" sheetId="1" r:id="rId1"/>
-    <sheet name="Critical Trials" sheetId="4" r:id="rId2"/>
-    <sheet name="Filler Trials" sheetId="2" r:id="rId3"/>
-    <sheet name="Test Phase" sheetId="3" r:id="rId4"/>
-    <sheet name="Design Diagram" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
+    <sheet name="Cover" sheetId="7" r:id="rId1"/>
+    <sheet name="Exposure Phase" sheetId="1" r:id="rId2"/>
+    <sheet name="Critical Trials" sheetId="4" r:id="rId3"/>
+    <sheet name="Filler Trials" sheetId="2" r:id="rId4"/>
+    <sheet name="Test Phase" sheetId="3" r:id="rId5"/>
+    <sheet name="Design Diagram" sheetId="5" r:id="rId6"/>
+    <sheet name="Design Diagram 2" sheetId="6" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2970,6 +2971,31 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3009,93 +3035,120 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="180"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3103,33 +3156,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3147,6 +3173,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="44" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="44" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="44" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="36" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3171,58 +3212,18 @@
     <xf numFmtId="0" fontId="3" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="44" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="37" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="44" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="44" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4185,6 +4186,54 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>11766</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>3920</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>71783</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A35F14D-5844-6160-821A-8376857B4FAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect t="15420" b="12000"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1226549" y="0"/>
+          <a:ext cx="7888241" cy="4080566"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
@@ -4226,7 +4275,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
@@ -4399,7 +4448,7 @@
 </c:userShapes>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -4882,13 +4931,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B29CE66-92EA-4368-848D-A617A92CBC0A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACC81691-9F24-4C87-8366-AE2912EBB662}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:AM718"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="65" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AK18" sqref="AK18"/>
     </sheetView>
   </sheetViews>
@@ -4929,14 +4993,14 @@
       <c r="AB1" s="1"/>
     </row>
     <row r="2" spans="2:39" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="237" t="s">
+      <c r="B2" s="248" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="237"/>
-      <c r="D2" s="237"/>
-      <c r="E2" s="237"/>
-      <c r="F2" s="237"/>
-      <c r="G2" s="237"/>
+      <c r="C2" s="248"/>
+      <c r="D2" s="248"/>
+      <c r="E2" s="248"/>
+      <c r="F2" s="248"/>
+      <c r="G2" s="248"/>
       <c r="H2" s="4"/>
       <c r="I2" s="6" t="s">
         <v>170</v>
@@ -4946,40 +5010,40 @@
         <v>17</v>
       </c>
       <c r="L2" s="4"/>
-      <c r="M2" s="237" t="s">
+      <c r="M2" s="248" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="237"/>
-      <c r="O2" s="237"/>
-      <c r="P2" s="237"/>
-      <c r="Q2" s="237"/>
-      <c r="R2" s="237"/>
-      <c r="S2" s="237"/>
-      <c r="T2" s="237"/>
-      <c r="U2" s="237"/>
-      <c r="V2" s="237"/>
-      <c r="W2" s="237"/>
-      <c r="X2" s="237"/>
-      <c r="Y2" s="237"/>
-      <c r="Z2" s="237"/>
-      <c r="AA2" s="237"/>
-      <c r="AB2" s="237"/>
+      <c r="N2" s="248"/>
+      <c r="O2" s="248"/>
+      <c r="P2" s="248"/>
+      <c r="Q2" s="248"/>
+      <c r="R2" s="248"/>
+      <c r="S2" s="248"/>
+      <c r="T2" s="248"/>
+      <c r="U2" s="248"/>
+      <c r="V2" s="248"/>
+      <c r="W2" s="248"/>
+      <c r="X2" s="248"/>
+      <c r="Y2" s="248"/>
+      <c r="Z2" s="248"/>
+      <c r="AA2" s="248"/>
+      <c r="AB2" s="248"/>
     </row>
     <row r="3" spans="2:39" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="238" t="s">
+      <c r="B3" s="249" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="239"/>
-      <c r="D3" s="239"/>
-      <c r="E3" s="239"/>
-      <c r="F3" s="239"/>
-      <c r="G3" s="240"/>
+      <c r="C3" s="250"/>
+      <c r="D3" s="250"/>
+      <c r="E3" s="250"/>
+      <c r="F3" s="250"/>
+      <c r="G3" s="251"/>
       <c r="H3" s="17"/>
-      <c r="I3" s="241" t="s">
+      <c r="I3" s="252" t="s">
         <v>25</v>
       </c>
       <c r="J3" s="17"/>
-      <c r="K3" s="241" t="s">
+      <c r="K3" s="252" t="s">
         <v>27</v>
       </c>
       <c r="L3" s="3"/>
@@ -4987,26 +5051,26 @@
         <v>21</v>
       </c>
       <c r="N3" s="18"/>
-      <c r="O3" s="245" t="s">
+      <c r="O3" s="256" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="245"/>
-      <c r="Q3" s="245"/>
-      <c r="R3" s="245"/>
+      <c r="P3" s="256"/>
+      <c r="Q3" s="256"/>
+      <c r="R3" s="256"/>
       <c r="S3" s="20"/>
-      <c r="T3" s="245" t="s">
+      <c r="T3" s="256" t="s">
         <v>13</v>
       </c>
-      <c r="U3" s="245"/>
-      <c r="V3" s="245"/>
-      <c r="W3" s="245"/>
+      <c r="U3" s="256"/>
+      <c r="V3" s="256"/>
+      <c r="W3" s="256"/>
       <c r="X3" s="18"/>
-      <c r="Y3" s="245" t="s">
+      <c r="Y3" s="256" t="s">
         <v>14</v>
       </c>
-      <c r="Z3" s="245"/>
-      <c r="AA3" s="245"/>
-      <c r="AB3" s="246"/>
+      <c r="Z3" s="256"/>
+      <c r="AA3" s="256"/>
+      <c r="AB3" s="257"/>
     </row>
     <row r="4" spans="2:39" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D4" s="4"/>
@@ -5014,40 +5078,40 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="243"/>
+      <c r="I4" s="254"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="242"/>
-      <c r="M4" s="242" t="s">
+      <c r="K4" s="253"/>
+      <c r="M4" s="253" t="s">
         <v>171</v>
       </c>
       <c r="N4" s="124"/>
-      <c r="O4" s="244" t="s">
+      <c r="O4" s="255" t="s">
         <v>31</v>
       </c>
-      <c r="P4" s="244"/>
-      <c r="Q4" s="244"/>
-      <c r="R4" s="244"/>
+      <c r="P4" s="255"/>
+      <c r="Q4" s="255"/>
+      <c r="R4" s="255"/>
       <c r="S4" s="124"/>
-      <c r="T4" s="244" t="s">
+      <c r="T4" s="255" t="s">
         <v>29</v>
       </c>
-      <c r="U4" s="244"/>
-      <c r="V4" s="244"/>
-      <c r="W4" s="244"/>
+      <c r="U4" s="255"/>
+      <c r="V4" s="255"/>
+      <c r="W4" s="255"/>
       <c r="X4" s="124"/>
-      <c r="Y4" s="244" t="s">
+      <c r="Y4" s="255" t="s">
         <v>30</v>
       </c>
-      <c r="Z4" s="244"/>
-      <c r="AA4" s="244"/>
-      <c r="AB4" s="244"/>
-      <c r="AI4" s="234" t="s">
+      <c r="Z4" s="255"/>
+      <c r="AA4" s="255"/>
+      <c r="AB4" s="255"/>
+      <c r="AI4" s="245" t="s">
         <v>191</v>
       </c>
-      <c r="AJ4" s="234"/>
-      <c r="AK4" s="234"/>
-      <c r="AL4" s="234"/>
-      <c r="AM4" s="234"/>
+      <c r="AJ4" s="245"/>
+      <c r="AK4" s="245"/>
+      <c r="AL4" s="245"/>
+      <c r="AM4" s="245"/>
     </row>
     <row r="5" spans="2:39" x14ac:dyDescent="0.35">
       <c r="C5" s="4" t="s">
@@ -5066,10 +5130,10 @@
         <v>3</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="I5" s="243"/>
+      <c r="I5" s="254"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="242"/>
-      <c r="M5" s="242"/>
+      <c r="K5" s="253"/>
+      <c r="M5" s="253"/>
       <c r="O5" s="5" t="s">
         <v>18</v>
       </c>
@@ -5108,11 +5172,11 @@
       <c r="AB5" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="AI5" s="234"/>
-      <c r="AJ5" s="234"/>
-      <c r="AK5" s="234"/>
-      <c r="AL5" s="234"/>
-      <c r="AM5" s="234"/>
+      <c r="AI5" s="245"/>
+      <c r="AJ5" s="245"/>
+      <c r="AK5" s="245"/>
+      <c r="AL5" s="245"/>
+      <c r="AM5" s="245"/>
     </row>
     <row r="6" spans="2:39" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="6"/>
@@ -5143,16 +5207,16 @@
       <c r="AA6" s="7"/>
       <c r="AB6" s="7"/>
       <c r="AE6" s="22"/>
-      <c r="AF6" s="235" t="s">
+      <c r="AF6" s="246" t="s">
         <v>28</v>
       </c>
-      <c r="AG6" s="236"/>
+      <c r="AG6" s="247"/>
       <c r="AH6" s="21"/>
-      <c r="AI6" s="234"/>
-      <c r="AJ6" s="234"/>
-      <c r="AK6" s="234"/>
-      <c r="AL6" s="234"/>
-      <c r="AM6" s="234"/>
+      <c r="AI6" s="245"/>
+      <c r="AJ6" s="245"/>
+      <c r="AK6" s="245"/>
+      <c r="AL6" s="245"/>
+      <c r="AM6" s="245"/>
     </row>
     <row r="7" spans="2:39" x14ac:dyDescent="0.35">
       <c r="B7" s="6">
@@ -5221,14 +5285,14 @@
         <v>9</v>
       </c>
       <c r="AE7" s="2"/>
-      <c r="AF7" s="235"/>
-      <c r="AG7" s="236"/>
+      <c r="AF7" s="246"/>
+      <c r="AG7" s="247"/>
       <c r="AH7" s="21"/>
-      <c r="AI7" s="234"/>
-      <c r="AJ7" s="234"/>
-      <c r="AK7" s="234"/>
-      <c r="AL7" s="234"/>
-      <c r="AM7" s="234"/>
+      <c r="AI7" s="245"/>
+      <c r="AJ7" s="245"/>
+      <c r="AK7" s="245"/>
+      <c r="AL7" s="245"/>
+      <c r="AM7" s="245"/>
     </row>
     <row r="8" spans="2:39" x14ac:dyDescent="0.35">
       <c r="C8" s="15" t="s">
@@ -5275,14 +5339,14 @@
         <v>8</v>
       </c>
       <c r="AE8" s="2"/>
-      <c r="AF8" s="235"/>
-      <c r="AG8" s="236"/>
+      <c r="AF8" s="246"/>
+      <c r="AG8" s="247"/>
       <c r="AH8" s="21"/>
-      <c r="AI8" s="234"/>
-      <c r="AJ8" s="234"/>
-      <c r="AK8" s="234"/>
-      <c r="AL8" s="234"/>
-      <c r="AM8" s="234"/>
+      <c r="AI8" s="245"/>
+      <c r="AJ8" s="245"/>
+      <c r="AK8" s="245"/>
+      <c r="AL8" s="245"/>
+      <c r="AM8" s="245"/>
     </row>
     <row r="9" spans="2:39" x14ac:dyDescent="0.35">
       <c r="C9" s="14"/>
@@ -5311,14 +5375,14 @@
       <c r="AA9" s="8"/>
       <c r="AB9" s="9"/>
       <c r="AE9" s="2"/>
-      <c r="AF9" s="235"/>
-      <c r="AG9" s="236"/>
+      <c r="AF9" s="246"/>
+      <c r="AG9" s="247"/>
       <c r="AH9" s="21"/>
-      <c r="AI9" s="234"/>
-      <c r="AJ9" s="234"/>
-      <c r="AK9" s="234"/>
-      <c r="AL9" s="234"/>
-      <c r="AM9" s="234"/>
+      <c r="AI9" s="245"/>
+      <c r="AJ9" s="245"/>
+      <c r="AK9" s="245"/>
+      <c r="AL9" s="245"/>
+      <c r="AM9" s="245"/>
     </row>
     <row r="10" spans="2:39" x14ac:dyDescent="0.35">
       <c r="C10" s="14"/>
@@ -5374,14 +5438,14 @@
         <v>9</v>
       </c>
       <c r="AE10" s="2"/>
-      <c r="AF10" s="235"/>
-      <c r="AG10" s="236"/>
+      <c r="AF10" s="246"/>
+      <c r="AG10" s="247"/>
       <c r="AH10" s="21"/>
-      <c r="AI10" s="234"/>
-      <c r="AJ10" s="234"/>
-      <c r="AK10" s="234"/>
-      <c r="AL10" s="234"/>
-      <c r="AM10" s="234"/>
+      <c r="AI10" s="245"/>
+      <c r="AJ10" s="245"/>
+      <c r="AK10" s="245"/>
+      <c r="AL10" s="245"/>
+      <c r="AM10" s="245"/>
     </row>
     <row r="11" spans="2:39" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
@@ -5419,14 +5483,14 @@
         <v>8</v>
       </c>
       <c r="AE11" s="23"/>
-      <c r="AF11" s="235"/>
-      <c r="AG11" s="236"/>
+      <c r="AF11" s="246"/>
+      <c r="AG11" s="247"/>
       <c r="AH11" s="21"/>
-      <c r="AI11" s="234"/>
-      <c r="AJ11" s="234"/>
-      <c r="AK11" s="234"/>
-      <c r="AL11" s="234"/>
-      <c r="AM11" s="234"/>
+      <c r="AI11" s="245"/>
+      <c r="AJ11" s="245"/>
+      <c r="AK11" s="245"/>
+      <c r="AL11" s="245"/>
+      <c r="AM11" s="245"/>
     </row>
     <row r="12" spans="2:39" x14ac:dyDescent="0.35">
       <c r="B12" s="6"/>
@@ -5456,11 +5520,11 @@
       <c r="Z12" s="11"/>
       <c r="AA12" s="7"/>
       <c r="AB12" s="7"/>
-      <c r="AI12" s="234"/>
-      <c r="AJ12" s="234"/>
-      <c r="AK12" s="234"/>
-      <c r="AL12" s="234"/>
-      <c r="AM12" s="234"/>
+      <c r="AI12" s="245"/>
+      <c r="AJ12" s="245"/>
+      <c r="AK12" s="245"/>
+      <c r="AL12" s="245"/>
+      <c r="AM12" s="245"/>
     </row>
     <row r="13" spans="2:39" x14ac:dyDescent="0.35">
       <c r="B13" s="6">
@@ -5528,11 +5592,11 @@
       <c r="AB13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AI13" s="234"/>
-      <c r="AJ13" s="234"/>
-      <c r="AK13" s="234"/>
-      <c r="AL13" s="234"/>
-      <c r="AM13" s="234"/>
+      <c r="AI13" s="245"/>
+      <c r="AJ13" s="245"/>
+      <c r="AK13" s="245"/>
+      <c r="AL13" s="245"/>
+      <c r="AM13" s="245"/>
     </row>
     <row r="14" spans="2:39" x14ac:dyDescent="0.35">
       <c r="C14" s="15" t="s">
@@ -5724,10 +5788,10 @@
       <c r="AA18" s="7"/>
       <c r="AB18" s="7"/>
       <c r="AE18" s="22"/>
-      <c r="AF18" s="235" t="s">
+      <c r="AF18" s="246" t="s">
         <v>28</v>
       </c>
-      <c r="AG18" s="236"/>
+      <c r="AG18" s="247"/>
     </row>
     <row r="19" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B19" s="6">
@@ -5796,8 +5860,8 @@
         <v>9</v>
       </c>
       <c r="AE19" s="2"/>
-      <c r="AF19" s="235"/>
-      <c r="AG19" s="236"/>
+      <c r="AF19" s="246"/>
+      <c r="AG19" s="247"/>
     </row>
     <row r="20" spans="2:33" x14ac:dyDescent="0.35">
       <c r="C20" s="15" t="s">
@@ -5844,8 +5908,8 @@
         <v>8</v>
       </c>
       <c r="AE20" s="2"/>
-      <c r="AF20" s="235"/>
-      <c r="AG20" s="236"/>
+      <c r="AF20" s="246"/>
+      <c r="AG20" s="247"/>
     </row>
     <row r="21" spans="2:33" x14ac:dyDescent="0.35">
       <c r="C21" s="14"/>
@@ -5874,8 +5938,8 @@
       <c r="AA21" s="8"/>
       <c r="AB21" s="9"/>
       <c r="AE21" s="2"/>
-      <c r="AF21" s="235"/>
-      <c r="AG21" s="236"/>
+      <c r="AF21" s="246"/>
+      <c r="AG21" s="247"/>
     </row>
     <row r="22" spans="2:33" x14ac:dyDescent="0.35">
       <c r="C22" s="14"/>
@@ -5931,8 +5995,8 @@
         <v>9</v>
       </c>
       <c r="AE22" s="2"/>
-      <c r="AF22" s="235"/>
-      <c r="AG22" s="236"/>
+      <c r="AF22" s="246"/>
+      <c r="AG22" s="247"/>
     </row>
     <row r="23" spans="2:33" x14ac:dyDescent="0.35">
       <c r="C23" s="14"/>
@@ -5969,8 +6033,8 @@
         <v>8</v>
       </c>
       <c r="AE23" s="23"/>
-      <c r="AF23" s="235"/>
-      <c r="AG23" s="236"/>
+      <c r="AF23" s="246"/>
+      <c r="AG23" s="247"/>
     </row>
     <row r="24" spans="2:33" x14ac:dyDescent="0.35">
       <c r="B24" s="6"/>
@@ -12427,7 +12491,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E104CA3-F104-4BEB-8735-F7B82CCBE338}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -12457,11 +12521,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="V2" s="249" t="s">
+      <c r="V2" s="261" t="s">
         <v>75</v>
       </c>
-      <c r="W2" s="249"/>
-      <c r="X2" s="249"/>
+      <c r="W2" s="261"/>
+      <c r="X2" s="261"/>
     </row>
     <row r="3" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="161" t="s">
@@ -12470,11 +12534,11 @@
       <c r="C3" s="162" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="247" t="s">
+      <c r="D3" s="279" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="248"/>
-      <c r="F3" s="248"/>
+      <c r="E3" s="280"/>
+      <c r="F3" s="280"/>
       <c r="G3" s="64"/>
       <c r="H3" s="161" t="s">
         <v>71</v>
@@ -12482,40 +12546,40 @@
       <c r="I3" s="162" t="s">
         <v>72</v>
       </c>
-      <c r="J3" s="247" t="s">
+      <c r="J3" s="279" t="s">
         <v>74</v>
       </c>
-      <c r="K3" s="248"/>
-      <c r="L3" s="248"/>
-      <c r="N3" s="249" t="s">
+      <c r="K3" s="280"/>
+      <c r="L3" s="280"/>
+      <c r="N3" s="261" t="s">
         <v>75</v>
       </c>
-      <c r="O3" s="249"/>
+      <c r="O3" s="261"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="249" t="s">
+      <c r="Q3" s="261" t="s">
         <v>76</v>
       </c>
-      <c r="R3" s="249"/>
+      <c r="R3" s="261"/>
       <c r="S3" s="1"/>
-      <c r="V3" s="271"/>
-      <c r="W3" s="271"/>
-      <c r="X3" s="271"/>
-      <c r="AB3" s="269" t="s">
+      <c r="V3" s="262"/>
+      <c r="W3" s="262"/>
+      <c r="X3" s="262"/>
+      <c r="AB3" s="259" t="s">
         <v>151</v>
       </c>
-      <c r="AC3" s="269"/>
-      <c r="AD3" s="269"/>
-      <c r="AE3" s="269"/>
-      <c r="AF3" s="269"/>
-      <c r="AG3" s="269"/>
-      <c r="AH3" s="269"/>
-      <c r="AI3" s="269"/>
-      <c r="AJ3" s="269"/>
-      <c r="AL3" s="269" t="s">
+      <c r="AC3" s="259"/>
+      <c r="AD3" s="259"/>
+      <c r="AE3" s="259"/>
+      <c r="AF3" s="259"/>
+      <c r="AG3" s="259"/>
+      <c r="AH3" s="259"/>
+      <c r="AI3" s="259"/>
+      <c r="AJ3" s="259"/>
+      <c r="AL3" s="259" t="s">
         <v>32</v>
       </c>
-      <c r="AM3" s="269"/>
-      <c r="AN3" s="269"/>
+      <c r="AM3" s="259"/>
+      <c r="AN3" s="259"/>
     </row>
     <row r="4" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="81" t="s">
@@ -12524,9 +12588,9 @@
       <c r="C4" s="77" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="247"/>
-      <c r="E4" s="248"/>
-      <c r="F4" s="248"/>
+      <c r="D4" s="279"/>
+      <c r="E4" s="280"/>
+      <c r="F4" s="280"/>
       <c r="G4" s="64"/>
       <c r="H4" s="81" t="s">
         <v>77</v>
@@ -12534,9 +12598,9 @@
       <c r="I4" s="77" t="s">
         <v>79</v>
       </c>
-      <c r="J4" s="247"/>
-      <c r="K4" s="248"/>
-      <c r="L4" s="248"/>
+      <c r="J4" s="279"/>
+      <c r="K4" s="280"/>
+      <c r="L4" s="280"/>
       <c r="N4" s="71" t="s">
         <v>71</v>
       </c>
@@ -12554,22 +12618,22 @@
       <c r="V4" s="98"/>
       <c r="W4" s="99"/>
       <c r="X4" s="100"/>
-      <c r="AB4" s="251" t="s">
+      <c r="AB4" s="267" t="s">
         <v>194</v>
       </c>
-      <c r="AC4" s="251"/>
-      <c r="AD4" s="251"/>
-      <c r="AE4" s="251"/>
-      <c r="AF4" s="251"/>
-      <c r="AG4" s="251"/>
-      <c r="AH4" s="251"/>
-      <c r="AI4" s="251"/>
-      <c r="AJ4" s="251"/>
-      <c r="AL4" s="234" t="s">
+      <c r="AC4" s="267"/>
+      <c r="AD4" s="267"/>
+      <c r="AE4" s="267"/>
+      <c r="AF4" s="267"/>
+      <c r="AG4" s="267"/>
+      <c r="AH4" s="267"/>
+      <c r="AI4" s="267"/>
+      <c r="AJ4" s="267"/>
+      <c r="AL4" s="245" t="s">
         <v>198</v>
       </c>
-      <c r="AM4" s="264"/>
-      <c r="AN4" s="264"/>
+      <c r="AM4" s="266"/>
+      <c r="AN4" s="266"/>
     </row>
     <row r="5" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="78" t="s">
@@ -12578,11 +12642,11 @@
       <c r="C5" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="D5" s="247" t="s">
+      <c r="D5" s="279" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="248"/>
-      <c r="F5" s="248"/>
+      <c r="E5" s="280"/>
+      <c r="F5" s="280"/>
       <c r="G5" s="64"/>
       <c r="H5" s="78" t="s">
         <v>82</v>
@@ -12590,9 +12654,9 @@
       <c r="I5" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="J5" s="247"/>
-      <c r="K5" s="248"/>
-      <c r="L5" s="248"/>
+      <c r="J5" s="279"/>
+      <c r="K5" s="280"/>
+      <c r="L5" s="280"/>
       <c r="N5" s="135" t="s">
         <v>143</v>
       </c>
@@ -12607,7 +12671,7 @@
         <v>143</v>
       </c>
       <c r="S5" s="1"/>
-      <c r="T5" s="265" t="s">
+      <c r="T5" s="263" t="s">
         <v>143</v>
       </c>
       <c r="U5" s="101"/>
@@ -12619,21 +12683,21 @@
         <v>79</v>
       </c>
       <c r="Y5" s="104"/>
-      <c r="Z5" s="267" t="s">
+      <c r="Z5" s="265" t="s">
         <v>144</v>
       </c>
-      <c r="AB5" s="251"/>
-      <c r="AC5" s="251"/>
-      <c r="AD5" s="251"/>
-      <c r="AE5" s="251"/>
-      <c r="AF5" s="251"/>
-      <c r="AG5" s="251"/>
-      <c r="AH5" s="251"/>
-      <c r="AI5" s="251"/>
-      <c r="AJ5" s="251"/>
-      <c r="AL5" s="264"/>
-      <c r="AM5" s="264"/>
-      <c r="AN5" s="264"/>
+      <c r="AB5" s="267"/>
+      <c r="AC5" s="267"/>
+      <c r="AD5" s="267"/>
+      <c r="AE5" s="267"/>
+      <c r="AF5" s="267"/>
+      <c r="AG5" s="267"/>
+      <c r="AH5" s="267"/>
+      <c r="AI5" s="267"/>
+      <c r="AJ5" s="267"/>
+      <c r="AL5" s="266"/>
+      <c r="AM5" s="266"/>
+      <c r="AN5" s="266"/>
       <c r="AO5" s="1"/>
     </row>
     <row r="6" spans="2:41" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -12653,9 +12717,9 @@
       <c r="I6" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="J6" s="247"/>
-      <c r="K6" s="248"/>
-      <c r="L6" s="248"/>
+      <c r="J6" s="279"/>
+      <c r="K6" s="280"/>
+      <c r="L6" s="280"/>
       <c r="N6" s="102" t="s">
         <v>77</v>
       </c>
@@ -12669,7 +12733,7 @@
         <v>80</v>
       </c>
       <c r="S6" s="1"/>
-      <c r="T6" s="266"/>
+      <c r="T6" s="264"/>
       <c r="U6" s="105"/>
       <c r="V6" s="65" t="s">
         <v>86</v>
@@ -12679,7 +12743,7 @@
         <v>96</v>
       </c>
       <c r="Y6" s="107"/>
-      <c r="Z6" s="267"/>
+      <c r="Z6" s="265"/>
       <c r="AB6" s="152" t="s">
         <v>81</v>
       </c>
@@ -12705,9 +12769,9 @@
       <c r="AJ6" s="150" t="s">
         <v>98</v>
       </c>
-      <c r="AL6" s="264"/>
-      <c r="AM6" s="264"/>
-      <c r="AN6" s="264"/>
+      <c r="AL6" s="266"/>
+      <c r="AM6" s="266"/>
+      <c r="AN6" s="266"/>
       <c r="AO6" s="1"/>
     </row>
     <row r="7" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -12717,11 +12781,11 @@
       <c r="C7" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="247" t="s">
+      <c r="D7" s="279" t="s">
         <v>94</v>
       </c>
-      <c r="E7" s="248"/>
-      <c r="F7" s="248"/>
+      <c r="E7" s="280"/>
+      <c r="F7" s="280"/>
       <c r="G7" s="64"/>
       <c r="H7" s="78" t="s">
         <v>93</v>
@@ -12729,9 +12793,9 @@
       <c r="I7" s="82" t="s">
         <v>95</v>
       </c>
-      <c r="J7" s="247"/>
-      <c r="K7" s="248"/>
-      <c r="L7" s="248"/>
+      <c r="J7" s="279"/>
+      <c r="K7" s="280"/>
+      <c r="L7" s="280"/>
       <c r="N7" s="65" t="s">
         <v>86</v>
       </c>
@@ -12745,7 +12809,7 @@
         <v>85</v>
       </c>
       <c r="S7" s="1"/>
-      <c r="T7" s="266"/>
+      <c r="T7" s="264"/>
       <c r="U7" s="105"/>
       <c r="V7" s="88" t="s">
         <v>88</v>
@@ -12755,7 +12819,7 @@
         <v>90</v>
       </c>
       <c r="Y7" s="107"/>
-      <c r="Z7" s="267"/>
+      <c r="Z7" s="265"/>
       <c r="AA7" s="123"/>
       <c r="AB7" s="214" t="s">
         <v>192</v>
@@ -12782,9 +12846,9 @@
       <c r="AJ7" s="215" t="s">
         <v>193</v>
       </c>
-      <c r="AL7" s="264"/>
-      <c r="AM7" s="264"/>
-      <c r="AN7" s="264"/>
+      <c r="AL7" s="266"/>
+      <c r="AM7" s="266"/>
+      <c r="AN7" s="266"/>
       <c r="AO7" s="1"/>
     </row>
     <row r="8" spans="2:41" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -12794,9 +12858,9 @@
       <c r="C8" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="D8" s="247"/>
-      <c r="E8" s="248"/>
-      <c r="F8" s="248"/>
+      <c r="D8" s="279"/>
+      <c r="E8" s="280"/>
+      <c r="F8" s="280"/>
       <c r="G8" s="27"/>
       <c r="H8" s="83" t="s">
         <v>99</v>
@@ -12804,11 +12868,11 @@
       <c r="I8" s="79" t="s">
         <v>101</v>
       </c>
-      <c r="J8" s="262" t="s">
+      <c r="J8" s="281" t="s">
         <v>102</v>
       </c>
-      <c r="K8" s="263"/>
-      <c r="L8" s="263"/>
+      <c r="K8" s="282"/>
+      <c r="L8" s="282"/>
       <c r="N8" s="88" t="s">
         <v>88</v>
       </c>
@@ -12822,7 +12886,7 @@
         <v>92</v>
       </c>
       <c r="S8" s="1"/>
-      <c r="T8" s="266"/>
+      <c r="T8" s="264"/>
       <c r="U8" s="105"/>
       <c r="V8" s="65" t="s">
         <v>97</v>
@@ -12832,7 +12896,7 @@
         <v>107</v>
       </c>
       <c r="Y8" s="107"/>
-      <c r="Z8" s="267"/>
+      <c r="Z8" s="265"/>
       <c r="AA8" s="123"/>
       <c r="AB8" s="147" t="s">
         <v>192</v>
@@ -12851,9 +12915,9 @@
       <c r="AJ8" s="146" t="s">
         <v>193</v>
       </c>
-      <c r="AL8" s="264"/>
-      <c r="AM8" s="264"/>
-      <c r="AN8" s="264"/>
+      <c r="AL8" s="266"/>
+      <c r="AM8" s="266"/>
+      <c r="AN8" s="266"/>
       <c r="AO8" s="1"/>
     </row>
     <row r="9" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -12863,9 +12927,9 @@
       <c r="C9" s="82" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="247"/>
-      <c r="E9" s="248"/>
-      <c r="F9" s="248"/>
+      <c r="D9" s="279"/>
+      <c r="E9" s="280"/>
+      <c r="F9" s="280"/>
       <c r="G9" s="64"/>
       <c r="H9" s="78" t="s">
         <v>105</v>
@@ -12886,7 +12950,7 @@
         <v>95</v>
       </c>
       <c r="S9" s="1"/>
-      <c r="T9" s="266"/>
+      <c r="T9" s="264"/>
       <c r="U9" s="105"/>
       <c r="V9" s="88" t="s">
         <v>99</v>
@@ -12896,7 +12960,7 @@
         <v>125</v>
       </c>
       <c r="Y9" s="107"/>
-      <c r="Z9" s="267"/>
+      <c r="Z9" s="265"/>
       <c r="AA9" s="123"/>
       <c r="AB9" s="148" t="s">
         <v>98</v>
@@ -12923,9 +12987,9 @@
       <c r="AJ9" s="149" t="s">
         <v>81</v>
       </c>
-      <c r="AL9" s="264"/>
-      <c r="AM9" s="264"/>
-      <c r="AN9" s="264"/>
+      <c r="AL9" s="266"/>
+      <c r="AM9" s="266"/>
+      <c r="AN9" s="266"/>
       <c r="AO9" s="1"/>
     </row>
     <row r="10" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -12935,9 +12999,9 @@
       <c r="C10" s="79" t="s">
         <v>110</v>
       </c>
-      <c r="D10" s="247"/>
-      <c r="E10" s="248"/>
-      <c r="F10" s="248"/>
+      <c r="D10" s="279"/>
+      <c r="E10" s="280"/>
+      <c r="F10" s="280"/>
       <c r="G10" s="64"/>
       <c r="H10" s="83" t="s">
         <v>109</v>
@@ -12945,11 +13009,11 @@
       <c r="I10" s="79" t="s">
         <v>78</v>
       </c>
-      <c r="J10" s="247" t="s">
+      <c r="J10" s="279" t="s">
         <v>111</v>
       </c>
-      <c r="K10" s="248"/>
-      <c r="L10" s="248"/>
+      <c r="K10" s="280"/>
+      <c r="L10" s="280"/>
       <c r="N10" s="88" t="s">
         <v>99</v>
       </c>
@@ -12963,7 +13027,7 @@
         <v>104</v>
       </c>
       <c r="S10" s="1"/>
-      <c r="T10" s="266"/>
+      <c r="T10" s="264"/>
       <c r="U10" s="105"/>
       <c r="V10" s="65" t="s">
         <v>108</v>
@@ -12973,7 +13037,7 @@
         <v>115</v>
       </c>
       <c r="Y10" s="107"/>
-      <c r="Z10" s="267"/>
+      <c r="Z10" s="265"/>
       <c r="AA10" s="123"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
@@ -12984,9 +13048,9 @@
       <c r="AH10" s="1"/>
       <c r="AI10" s="1"/>
       <c r="AJ10" s="1"/>
-      <c r="AL10" s="264"/>
-      <c r="AM10" s="264"/>
-      <c r="AN10" s="264"/>
+      <c r="AL10" s="266"/>
+      <c r="AM10" s="266"/>
+      <c r="AN10" s="266"/>
       <c r="AO10" s="1"/>
     </row>
     <row r="11" spans="2:41" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -12996,9 +13060,9 @@
       <c r="C11" s="82" t="s">
         <v>113</v>
       </c>
-      <c r="D11" s="247"/>
-      <c r="E11" s="248"/>
-      <c r="F11" s="248"/>
+      <c r="D11" s="279"/>
+      <c r="E11" s="280"/>
+      <c r="F11" s="280"/>
       <c r="G11" s="64"/>
       <c r="H11" s="78" t="s">
         <v>114</v>
@@ -13006,9 +13070,9 @@
       <c r="I11" s="82" t="s">
         <v>110</v>
       </c>
-      <c r="J11" s="247"/>
-      <c r="K11" s="248"/>
-      <c r="L11" s="248"/>
+      <c r="J11" s="279"/>
+      <c r="K11" s="280"/>
+      <c r="L11" s="280"/>
       <c r="N11" s="65" t="s">
         <v>108</v>
       </c>
@@ -13022,7 +13086,7 @@
         <v>106</v>
       </c>
       <c r="S11" s="1"/>
-      <c r="T11" s="266"/>
+      <c r="T11" s="264"/>
       <c r="U11" s="105"/>
       <c r="V11" s="88" t="s">
         <v>109</v>
@@ -13032,7 +13096,7 @@
         <v>78</v>
       </c>
       <c r="Y11" s="107"/>
-      <c r="Z11" s="267"/>
+      <c r="Z11" s="265"/>
       <c r="AA11" s="123"/>
       <c r="AB11" s="152" t="s">
         <v>81</v>
@@ -13059,9 +13123,9 @@
       <c r="AJ11" s="150" t="s">
         <v>98</v>
       </c>
-      <c r="AL11" s="264"/>
-      <c r="AM11" s="264"/>
-      <c r="AN11" s="264"/>
+      <c r="AL11" s="266"/>
+      <c r="AM11" s="266"/>
+      <c r="AN11" s="266"/>
       <c r="AO11" s="1"/>
     </row>
     <row r="12" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -13071,9 +13135,9 @@
       <c r="C12" s="79" t="s">
         <v>115</v>
       </c>
-      <c r="D12" s="247"/>
-      <c r="E12" s="248"/>
-      <c r="F12" s="248"/>
+      <c r="D12" s="279"/>
+      <c r="E12" s="280"/>
+      <c r="F12" s="280"/>
       <c r="G12" s="64"/>
       <c r="H12" s="83" t="s">
         <v>117</v>
@@ -13081,9 +13145,9 @@
       <c r="I12" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="J12" s="247"/>
-      <c r="K12" s="248"/>
-      <c r="L12" s="248"/>
+      <c r="J12" s="279"/>
+      <c r="K12" s="280"/>
+      <c r="L12" s="280"/>
       <c r="N12" s="88" t="s">
         <v>109</v>
       </c>
@@ -13097,7 +13161,7 @@
         <v>113</v>
       </c>
       <c r="S12" s="1"/>
-      <c r="T12" s="266"/>
+      <c r="T12" s="264"/>
       <c r="U12" s="105"/>
       <c r="V12" s="65" t="s">
         <v>116</v>
@@ -13107,7 +13171,7 @@
         <v>89</v>
       </c>
       <c r="Y12" s="107"/>
-      <c r="Z12" s="267"/>
+      <c r="Z12" s="265"/>
       <c r="AA12" s="123"/>
       <c r="AB12" s="214" t="s">
         <v>192</v>
@@ -13126,9 +13190,9 @@
       <c r="AJ12" s="215" t="s">
         <v>193</v>
       </c>
-      <c r="AL12" s="264"/>
-      <c r="AM12" s="264"/>
-      <c r="AN12" s="264"/>
+      <c r="AL12" s="266"/>
+      <c r="AM12" s="266"/>
+      <c r="AN12" s="266"/>
       <c r="AO12" s="1"/>
     </row>
     <row r="13" spans="2:41" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -13138,9 +13202,9 @@
       <c r="C13" s="82" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="247"/>
-      <c r="E13" s="248"/>
-      <c r="F13" s="248"/>
+      <c r="D13" s="279"/>
+      <c r="E13" s="280"/>
+      <c r="F13" s="280"/>
       <c r="G13" s="64"/>
       <c r="H13" s="78" t="s">
         <v>120</v>
@@ -13148,9 +13212,9 @@
       <c r="I13" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="J13" s="247"/>
-      <c r="K13" s="248"/>
-      <c r="L13" s="248"/>
+      <c r="J13" s="279"/>
+      <c r="K13" s="280"/>
+      <c r="L13" s="280"/>
       <c r="N13" s="65" t="s">
         <v>116</v>
       </c>
@@ -13164,7 +13228,7 @@
         <v>110</v>
       </c>
       <c r="S13" s="1"/>
-      <c r="T13" s="266"/>
+      <c r="T13" s="264"/>
       <c r="U13" s="105"/>
       <c r="V13" s="88" t="s">
         <v>117</v>
@@ -13174,7 +13238,7 @@
         <v>100</v>
       </c>
       <c r="Y13" s="107"/>
-      <c r="Z13" s="267"/>
+      <c r="Z13" s="265"/>
       <c r="AA13" s="123"/>
       <c r="AB13" s="147" t="s">
         <v>192</v>
@@ -13213,9 +13277,9 @@
       <c r="C14" s="79" t="s">
         <v>119</v>
       </c>
-      <c r="D14" s="247"/>
-      <c r="E14" s="248"/>
-      <c r="F14" s="248"/>
+      <c r="D14" s="279"/>
+      <c r="E14" s="280"/>
+      <c r="F14" s="280"/>
       <c r="G14" s="64"/>
       <c r="H14" s="83" t="s">
         <v>91</v>
@@ -13223,9 +13287,9 @@
       <c r="I14" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="J14" s="247"/>
-      <c r="K14" s="248"/>
-      <c r="L14" s="248"/>
+      <c r="J14" s="279"/>
+      <c r="K14" s="280"/>
+      <c r="L14" s="280"/>
       <c r="N14" s="88" t="s">
         <v>117</v>
       </c>
@@ -13239,7 +13303,7 @@
         <v>119</v>
       </c>
       <c r="S14" s="1"/>
-      <c r="T14" s="266"/>
+      <c r="T14" s="264"/>
       <c r="U14" s="105"/>
       <c r="V14" s="69" t="s">
         <v>121</v>
@@ -13249,7 +13313,7 @@
         <v>123</v>
       </c>
       <c r="Y14" s="107"/>
-      <c r="Z14" s="267"/>
+      <c r="Z14" s="265"/>
       <c r="AA14" s="123"/>
       <c r="AB14" s="148" t="s">
         <v>98</v>
@@ -13284,9 +13348,9 @@
       <c r="C15" s="82" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="247"/>
-      <c r="E15" s="248"/>
-      <c r="F15" s="248"/>
+      <c r="D15" s="279"/>
+      <c r="E15" s="280"/>
+      <c r="F15" s="280"/>
       <c r="G15" s="64"/>
       <c r="H15" s="78" t="s">
         <v>86</v>
@@ -13294,9 +13358,9 @@
       <c r="I15" s="82" t="s">
         <v>96</v>
       </c>
-      <c r="J15" s="247"/>
-      <c r="K15" s="248"/>
-      <c r="L15" s="248"/>
+      <c r="J15" s="279"/>
+      <c r="K15" s="280"/>
+      <c r="L15" s="280"/>
       <c r="N15" s="69" t="s">
         <v>121</v>
       </c>
@@ -13310,18 +13374,18 @@
         <v>83</v>
       </c>
       <c r="S15" s="1"/>
-      <c r="T15" s="266"/>
+      <c r="T15" s="264"/>
       <c r="U15" s="108"/>
       <c r="V15" s="109"/>
       <c r="W15" s="110"/>
       <c r="X15" s="111"/>
       <c r="Y15" s="112"/>
-      <c r="Z15" s="267"/>
-      <c r="AL15" s="234" t="s">
+      <c r="Z15" s="265"/>
+      <c r="AL15" s="245" t="s">
         <v>126</v>
       </c>
-      <c r="AM15" s="234"/>
-      <c r="AN15" s="234"/>
+      <c r="AM15" s="245"/>
+      <c r="AN15" s="245"/>
       <c r="AO15" s="1"/>
     </row>
     <row r="16" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -13331,9 +13395,9 @@
       <c r="C16" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="D16" s="247"/>
-      <c r="E16" s="248"/>
-      <c r="F16" s="248"/>
+      <c r="D16" s="279"/>
+      <c r="E16" s="280"/>
+      <c r="F16" s="280"/>
       <c r="G16" s="64"/>
       <c r="H16" s="83" t="s">
         <v>103</v>
@@ -13341,27 +13405,27 @@
       <c r="I16" s="79" t="s">
         <v>92</v>
       </c>
-      <c r="J16" s="247"/>
-      <c r="K16" s="248"/>
-      <c r="L16" s="248"/>
-      <c r="T16" s="266"/>
+      <c r="J16" s="279"/>
+      <c r="K16" s="280"/>
+      <c r="L16" s="280"/>
+      <c r="T16" s="264"/>
       <c r="U16" s="105"/>
       <c r="V16" s="113"/>
       <c r="W16" s="114"/>
       <c r="X16" s="115"/>
       <c r="Y16" s="107"/>
-      <c r="Z16" s="267"/>
-      <c r="AB16" s="251" t="s">
+      <c r="Z16" s="265"/>
+      <c r="AB16" s="267" t="s">
         <v>195</v>
       </c>
-      <c r="AC16" s="251"/>
-      <c r="AD16" s="251"/>
-      <c r="AE16" s="251"/>
-      <c r="AF16" s="251"/>
-      <c r="AG16" s="251"/>
-      <c r="AH16" s="251"/>
-      <c r="AI16" s="251"/>
-      <c r="AJ16" s="251"/>
+      <c r="AC16" s="267"/>
+      <c r="AD16" s="267"/>
+      <c r="AE16" s="267"/>
+      <c r="AF16" s="267"/>
+      <c r="AG16" s="267"/>
+      <c r="AH16" s="267"/>
+      <c r="AI16" s="267"/>
+      <c r="AJ16" s="267"/>
       <c r="AL16" s="21"/>
       <c r="AM16" s="21"/>
       <c r="AN16" s="21"/>
@@ -13374,9 +13438,9 @@
       <c r="C17" s="82" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="247"/>
-      <c r="E17" s="248"/>
-      <c r="F17" s="248"/>
+      <c r="D17" s="279"/>
+      <c r="E17" s="280"/>
+      <c r="F17" s="280"/>
       <c r="G17" s="64"/>
       <c r="H17" s="78" t="s">
         <v>97</v>
@@ -13384,11 +13448,11 @@
       <c r="I17" s="82" t="s">
         <v>107</v>
       </c>
-      <c r="J17" s="247"/>
-      <c r="K17" s="248"/>
-      <c r="L17" s="248"/>
+      <c r="J17" s="279"/>
+      <c r="K17" s="280"/>
+      <c r="L17" s="280"/>
       <c r="S17" s="125"/>
-      <c r="T17" s="266"/>
+      <c r="T17" s="264"/>
       <c r="U17" s="105"/>
       <c r="V17" s="72" t="s">
         <v>80</v>
@@ -13398,22 +13462,22 @@
         <v>91</v>
       </c>
       <c r="Y17" s="107"/>
-      <c r="Z17" s="267"/>
+      <c r="Z17" s="265"/>
       <c r="AA17" s="123"/>
-      <c r="AB17" s="251"/>
-      <c r="AC17" s="251"/>
-      <c r="AD17" s="251"/>
-      <c r="AE17" s="251"/>
-      <c r="AF17" s="251"/>
-      <c r="AG17" s="251"/>
-      <c r="AH17" s="251"/>
-      <c r="AI17" s="251"/>
-      <c r="AJ17" s="251"/>
-      <c r="AL17" s="234" t="s">
+      <c r="AB17" s="267"/>
+      <c r="AC17" s="267"/>
+      <c r="AD17" s="267"/>
+      <c r="AE17" s="267"/>
+      <c r="AF17" s="267"/>
+      <c r="AG17" s="267"/>
+      <c r="AH17" s="267"/>
+      <c r="AI17" s="267"/>
+      <c r="AJ17" s="267"/>
+      <c r="AL17" s="245" t="s">
         <v>128</v>
       </c>
-      <c r="AM17" s="234"/>
-      <c r="AN17" s="234"/>
+      <c r="AM17" s="245"/>
+      <c r="AN17" s="245"/>
       <c r="AO17" s="1"/>
     </row>
     <row r="18" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -13423,9 +13487,9 @@
       <c r="C18" s="79" t="s">
         <v>125</v>
       </c>
-      <c r="D18" s="247"/>
-      <c r="E18" s="248"/>
-      <c r="F18" s="248"/>
+      <c r="D18" s="279"/>
+      <c r="E18" s="280"/>
+      <c r="F18" s="280"/>
       <c r="G18" s="64"/>
       <c r="H18" s="83" t="s">
         <v>112</v>
@@ -13433,21 +13497,21 @@
       <c r="I18" s="79" t="s">
         <v>104</v>
       </c>
-      <c r="J18" s="247"/>
-      <c r="K18" s="248"/>
-      <c r="L18" s="248"/>
+      <c r="J18" s="279"/>
+      <c r="K18" s="280"/>
+      <c r="L18" s="280"/>
       <c r="M18" s="73"/>
-      <c r="N18" s="251" t="s">
+      <c r="N18" s="267" t="s">
         <v>143</v>
       </c>
-      <c r="O18" s="251"/>
+      <c r="O18" s="267"/>
       <c r="P18" s="73"/>
-      <c r="Q18" s="252" t="s">
+      <c r="Q18" s="269" t="s">
         <v>144</v>
       </c>
-      <c r="R18" s="252"/>
+      <c r="R18" s="269"/>
       <c r="S18" s="125"/>
-      <c r="T18" s="266"/>
+      <c r="T18" s="264"/>
       <c r="U18" s="105"/>
       <c r="V18" s="88" t="s">
         <v>85</v>
@@ -13457,7 +13521,7 @@
         <v>82</v>
       </c>
       <c r="Y18" s="107"/>
-      <c r="Z18" s="267"/>
+      <c r="Z18" s="265"/>
       <c r="AA18" s="123"/>
       <c r="AB18" s="152" t="s">
         <v>98</v>
@@ -13484,11 +13548,11 @@
       <c r="AJ18" s="146" t="s">
         <v>98</v>
       </c>
-      <c r="AL18" s="234" t="s">
+      <c r="AL18" s="245" t="s">
         <v>129</v>
       </c>
-      <c r="AM18" s="234"/>
-      <c r="AN18" s="234"/>
+      <c r="AM18" s="245"/>
+      <c r="AN18" s="245"/>
       <c r="AO18" s="1"/>
     </row>
     <row r="19" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -13498,9 +13562,9 @@
       <c r="C19" s="82" t="s">
         <v>106</v>
       </c>
-      <c r="D19" s="247"/>
-      <c r="E19" s="248"/>
-      <c r="F19" s="248"/>
+      <c r="D19" s="279"/>
+      <c r="E19" s="280"/>
+      <c r="F19" s="280"/>
       <c r="G19" s="64"/>
       <c r="H19" s="78" t="s">
         <v>108</v>
@@ -13508,9 +13572,9 @@
       <c r="I19" s="82" t="s">
         <v>115</v>
       </c>
-      <c r="J19" s="247"/>
-      <c r="K19" s="248"/>
-      <c r="L19" s="248"/>
+      <c r="J19" s="279"/>
+      <c r="K19" s="280"/>
+      <c r="L19" s="280"/>
       <c r="M19" s="21"/>
       <c r="N19" s="157" t="s">
         <v>71</v>
@@ -13526,7 +13590,7 @@
         <v>72</v>
       </c>
       <c r="S19" s="125"/>
-      <c r="T19" s="266"/>
+      <c r="T19" s="264"/>
       <c r="U19" s="105"/>
       <c r="V19" s="65" t="s">
         <v>92</v>
@@ -13536,7 +13600,7 @@
         <v>103</v>
       </c>
       <c r="Y19" s="107"/>
-      <c r="Z19" s="267"/>
+      <c r="Z19" s="265"/>
       <c r="AA19" s="123"/>
       <c r="AB19" s="214" t="s">
         <v>192</v>
@@ -13563,11 +13627,11 @@
       <c r="AJ19" s="217" t="s">
         <v>193</v>
       </c>
-      <c r="AL19" s="234" t="s">
+      <c r="AL19" s="245" t="s">
         <v>133</v>
       </c>
-      <c r="AM19" s="234"/>
-      <c r="AN19" s="234"/>
+      <c r="AM19" s="245"/>
+      <c r="AN19" s="245"/>
       <c r="AO19" s="1"/>
     </row>
     <row r="20" spans="2:41" ht="14" customHeight="1" x14ac:dyDescent="0.35">
@@ -13577,9 +13641,9 @@
       <c r="C20" s="79" t="s">
         <v>80</v>
       </c>
-      <c r="D20" s="247"/>
-      <c r="E20" s="248"/>
-      <c r="F20" s="248"/>
+      <c r="D20" s="279"/>
+      <c r="E20" s="280"/>
+      <c r="F20" s="280"/>
       <c r="G20" s="64"/>
       <c r="H20" s="83" t="s">
         <v>118</v>
@@ -13587,9 +13651,9 @@
       <c r="I20" s="79" t="s">
         <v>113</v>
       </c>
-      <c r="J20" s="247"/>
-      <c r="K20" s="248"/>
-      <c r="L20" s="248"/>
+      <c r="J20" s="279"/>
+      <c r="K20" s="280"/>
+      <c r="L20" s="280"/>
       <c r="M20" s="21"/>
       <c r="N20" s="95" t="s">
         <v>77</v>
@@ -13605,7 +13669,7 @@
         <v>79</v>
       </c>
       <c r="S20" s="125"/>
-      <c r="T20" s="266"/>
+      <c r="T20" s="264"/>
       <c r="U20" s="105"/>
       <c r="V20" s="88" t="s">
         <v>95</v>
@@ -13615,7 +13679,7 @@
         <v>93</v>
       </c>
       <c r="Y20" s="107"/>
-      <c r="Z20" s="267"/>
+      <c r="Z20" s="265"/>
       <c r="AA20" s="123"/>
       <c r="AB20" s="147" t="s">
         <v>192</v>
@@ -13646,9 +13710,9 @@
       <c r="C21" s="82" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="247"/>
-      <c r="E21" s="248"/>
-      <c r="F21" s="248"/>
+      <c r="D21" s="279"/>
+      <c r="E21" s="280"/>
+      <c r="F21" s="280"/>
       <c r="G21" s="64"/>
       <c r="H21" s="78" t="s">
         <v>116</v>
@@ -13656,9 +13720,9 @@
       <c r="I21" s="82" t="s">
         <v>89</v>
       </c>
-      <c r="J21" s="247"/>
-      <c r="K21" s="248"/>
-      <c r="L21" s="248"/>
+      <c r="J21" s="279"/>
+      <c r="K21" s="280"/>
+      <c r="L21" s="280"/>
       <c r="N21" s="68" t="s">
         <v>86</v>
       </c>
@@ -13672,7 +13736,7 @@
         <v>96</v>
       </c>
       <c r="S21" s="125"/>
-      <c r="T21" s="266"/>
+      <c r="T21" s="264"/>
       <c r="U21" s="105"/>
       <c r="V21" s="65" t="s">
         <v>104</v>
@@ -13682,7 +13746,7 @@
         <v>112</v>
       </c>
       <c r="Y21" s="107"/>
-      <c r="Z21" s="267"/>
+      <c r="Z21" s="265"/>
       <c r="AA21" s="123"/>
       <c r="AB21" s="148" t="s">
         <v>81</v>
@@ -13721,9 +13785,9 @@
       <c r="C22" s="79" t="s">
         <v>127</v>
       </c>
-      <c r="D22" s="247"/>
-      <c r="E22" s="248"/>
-      <c r="F22" s="248"/>
+      <c r="D22" s="279"/>
+      <c r="E22" s="280"/>
+      <c r="F22" s="280"/>
       <c r="G22" s="64"/>
       <c r="H22" s="83" t="s">
         <v>122</v>
@@ -13731,9 +13795,9 @@
       <c r="I22" s="79" t="s">
         <v>119</v>
       </c>
-      <c r="J22" s="247"/>
-      <c r="K22" s="248"/>
-      <c r="L22" s="248"/>
+      <c r="J22" s="279"/>
+      <c r="K22" s="280"/>
+      <c r="L22" s="280"/>
       <c r="N22" s="89" t="s">
         <v>88</v>
       </c>
@@ -13747,7 +13811,7 @@
         <v>90</v>
       </c>
       <c r="S22" s="60"/>
-      <c r="T22" s="266"/>
+      <c r="T22" s="264"/>
       <c r="U22" s="105"/>
       <c r="V22" s="88" t="s">
         <v>106</v>
@@ -13757,7 +13821,7 @@
         <v>105</v>
       </c>
       <c r="Y22" s="107"/>
-      <c r="Z22" s="267"/>
+      <c r="Z22" s="265"/>
       <c r="AA22" s="123"/>
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
@@ -13780,9 +13844,9 @@
       <c r="C23" s="84" t="s">
         <v>107</v>
       </c>
-      <c r="D23" s="247"/>
-      <c r="E23" s="248"/>
-      <c r="F23" s="248"/>
+      <c r="D23" s="279"/>
+      <c r="E23" s="280"/>
+      <c r="F23" s="280"/>
       <c r="G23" s="64"/>
       <c r="H23" s="80" t="s">
         <v>121</v>
@@ -13790,9 +13854,9 @@
       <c r="I23" s="84" t="s">
         <v>123</v>
       </c>
-      <c r="J23" s="247"/>
-      <c r="K23" s="248"/>
-      <c r="L23" s="248"/>
+      <c r="J23" s="279"/>
+      <c r="K23" s="280"/>
+      <c r="L23" s="280"/>
       <c r="N23" s="68" t="s">
         <v>97</v>
       </c>
@@ -13805,7 +13869,7 @@
       <c r="R23" s="86" t="s">
         <v>107</v>
       </c>
-      <c r="T23" s="266"/>
+      <c r="T23" s="264"/>
       <c r="U23" s="105"/>
       <c r="V23" s="65" t="s">
         <v>113</v>
@@ -13815,7 +13879,7 @@
         <v>118</v>
       </c>
       <c r="Y23" s="107"/>
-      <c r="Z23" s="267"/>
+      <c r="Z23" s="265"/>
       <c r="AA23" s="123"/>
       <c r="AB23" s="152" t="s">
         <v>98</v>
@@ -13861,7 +13925,7 @@
         <v>125</v>
       </c>
       <c r="S24" s="1"/>
-      <c r="T24" s="266"/>
+      <c r="T24" s="264"/>
       <c r="U24" s="105"/>
       <c r="V24" s="88" t="s">
         <v>110</v>
@@ -13871,7 +13935,7 @@
         <v>114</v>
       </c>
       <c r="Y24" s="107"/>
-      <c r="Z24" s="267"/>
+      <c r="Z24" s="265"/>
       <c r="AA24" s="123"/>
       <c r="AB24" s="214" t="s">
         <v>192</v>
@@ -13897,13 +13961,13 @@
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
-      <c r="H25" s="264" t="s">
+      <c r="H25" s="266" t="s">
         <v>152</v>
       </c>
-      <c r="I25" s="264"/>
-      <c r="J25" s="264"/>
-      <c r="K25" s="264"/>
-      <c r="L25" s="264"/>
+      <c r="I25" s="266"/>
+      <c r="J25" s="266"/>
+      <c r="K25" s="266"/>
+      <c r="L25" s="266"/>
       <c r="N25" s="68" t="s">
         <v>108</v>
       </c>
@@ -13917,7 +13981,7 @@
         <v>115</v>
       </c>
       <c r="S25" s="1"/>
-      <c r="T25" s="266"/>
+      <c r="T25" s="264"/>
       <c r="U25" s="105"/>
       <c r="V25" s="65" t="s">
         <v>119</v>
@@ -13927,7 +13991,7 @@
         <v>122</v>
       </c>
       <c r="Y25" s="107"/>
-      <c r="Z25" s="267"/>
+      <c r="Z25" s="265"/>
       <c r="AA25" s="123"/>
       <c r="AB25" s="147" t="s">
         <v>192</v>
@@ -13959,19 +14023,19 @@
       <c r="B26" s="74" t="s">
         <v>130</v>
       </c>
-      <c r="C26" s="253" t="s">
+      <c r="C26" s="270" t="s">
         <v>131</v>
       </c>
-      <c r="D26" s="254"/>
-      <c r="E26" s="253" t="s">
+      <c r="D26" s="271"/>
+      <c r="E26" s="270" t="s">
         <v>132</v>
       </c>
-      <c r="F26" s="255"/>
-      <c r="H26" s="264"/>
-      <c r="I26" s="264"/>
-      <c r="J26" s="264"/>
-      <c r="K26" s="264"/>
-      <c r="L26" s="264"/>
+      <c r="F26" s="272"/>
+      <c r="H26" s="266"/>
+      <c r="I26" s="266"/>
+      <c r="J26" s="266"/>
+      <c r="K26" s="266"/>
+      <c r="L26" s="266"/>
       <c r="N26" s="89" t="s">
         <v>109</v>
       </c>
@@ -13985,7 +14049,7 @@
         <v>78</v>
       </c>
       <c r="S26" s="1"/>
-      <c r="T26" s="266"/>
+      <c r="T26" s="264"/>
       <c r="U26" s="118"/>
       <c r="V26" s="94" t="s">
         <v>83</v>
@@ -13995,7 +14059,7 @@
         <v>120</v>
       </c>
       <c r="Y26" s="112"/>
-      <c r="Z26" s="267"/>
+      <c r="Z26" s="265"/>
       <c r="AA26" s="123"/>
       <c r="AB26" s="148" t="s">
         <v>81</v>
@@ -14027,19 +14091,19 @@
       <c r="B27" s="75" t="s">
         <v>134</v>
       </c>
-      <c r="C27" s="256">
+      <c r="C27" s="273">
         <v>0.8</v>
       </c>
-      <c r="D27" s="257"/>
-      <c r="E27" s="256">
+      <c r="D27" s="274"/>
+      <c r="E27" s="273">
         <v>100</v>
       </c>
-      <c r="F27" s="258"/>
-      <c r="H27" s="264"/>
-      <c r="I27" s="264"/>
-      <c r="J27" s="264"/>
-      <c r="K27" s="264"/>
-      <c r="L27" s="264"/>
+      <c r="F27" s="275"/>
+      <c r="H27" s="266"/>
+      <c r="I27" s="266"/>
+      <c r="J27" s="266"/>
+      <c r="K27" s="266"/>
+      <c r="L27" s="266"/>
       <c r="N27" s="68" t="s">
         <v>116</v>
       </c>
@@ -14063,19 +14127,19 @@
       <c r="B28" s="76" t="s">
         <v>135</v>
       </c>
-      <c r="C28" s="259">
+      <c r="C28" s="276">
         <v>1</v>
       </c>
-      <c r="D28" s="260"/>
-      <c r="E28" s="259">
+      <c r="D28" s="277"/>
+      <c r="E28" s="276">
         <v>180</v>
       </c>
-      <c r="F28" s="261"/>
-      <c r="H28" s="264"/>
-      <c r="I28" s="264"/>
-      <c r="J28" s="264"/>
-      <c r="K28" s="264"/>
-      <c r="L28" s="264"/>
+      <c r="F28" s="278"/>
+      <c r="H28" s="266"/>
+      <c r="I28" s="266"/>
+      <c r="J28" s="266"/>
+      <c r="K28" s="266"/>
+      <c r="L28" s="266"/>
       <c r="N28" s="89" t="s">
         <v>117</v>
       </c>
@@ -14088,36 +14152,36 @@
       <c r="R28" s="90" t="s">
         <v>100</v>
       </c>
-      <c r="V28" s="270" t="s">
+      <c r="V28" s="260" t="s">
         <v>76</v>
       </c>
-      <c r="W28" s="270"/>
-      <c r="X28" s="270"/>
-      <c r="AB28" s="268" t="s">
+      <c r="W28" s="260"/>
+      <c r="X28" s="260"/>
+      <c r="AB28" s="258" t="s">
         <v>197</v>
       </c>
-      <c r="AC28" s="268"/>
-      <c r="AD28" s="268"/>
-      <c r="AE28" s="268"/>
-      <c r="AF28" s="268"/>
-      <c r="AG28" s="268"/>
-      <c r="AH28" s="268"/>
-      <c r="AI28" s="268"/>
-      <c r="AJ28" s="268"/>
+      <c r="AC28" s="258"/>
+      <c r="AD28" s="258"/>
+      <c r="AE28" s="258"/>
+      <c r="AF28" s="258"/>
+      <c r="AG28" s="258"/>
+      <c r="AH28" s="258"/>
+      <c r="AI28" s="258"/>
+      <c r="AJ28" s="258"/>
     </row>
     <row r="29" spans="2:41" ht="14" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="250" t="s">
+      <c r="B29" s="268" t="s">
         <v>136</v>
       </c>
-      <c r="C29" s="250"/>
-      <c r="D29" s="250"/>
-      <c r="E29" s="250"/>
-      <c r="F29" s="250"/>
-      <c r="H29" s="264"/>
-      <c r="I29" s="264"/>
-      <c r="J29" s="264"/>
-      <c r="K29" s="264"/>
-      <c r="L29" s="264"/>
+      <c r="C29" s="268"/>
+      <c r="D29" s="268"/>
+      <c r="E29" s="268"/>
+      <c r="F29" s="268"/>
+      <c r="H29" s="266"/>
+      <c r="I29" s="266"/>
+      <c r="J29" s="266"/>
+      <c r="K29" s="266"/>
+      <c r="L29" s="266"/>
       <c r="N29" s="70" t="s">
         <v>121</v>
       </c>
@@ -14131,20 +14195,20 @@
         <v>123</v>
       </c>
       <c r="S29" s="60"/>
-      <c r="V29" s="249"/>
-      <c r="W29" s="249"/>
-      <c r="X29" s="249"/>
-      <c r="AB29" s="268" t="s">
+      <c r="V29" s="261"/>
+      <c r="W29" s="261"/>
+      <c r="X29" s="261"/>
+      <c r="AB29" s="258" t="s">
         <v>196</v>
       </c>
-      <c r="AC29" s="268"/>
-      <c r="AD29" s="268"/>
-      <c r="AE29" s="268"/>
-      <c r="AF29" s="268"/>
-      <c r="AG29" s="268"/>
-      <c r="AH29" s="268"/>
-      <c r="AI29" s="268"/>
-      <c r="AJ29" s="268"/>
+      <c r="AC29" s="258"/>
+      <c r="AD29" s="258"/>
+      <c r="AE29" s="258"/>
+      <c r="AF29" s="258"/>
+      <c r="AG29" s="258"/>
+      <c r="AH29" s="258"/>
+      <c r="AI29" s="258"/>
+      <c r="AJ29" s="258"/>
     </row>
     <row r="30" spans="2:41" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="S30" s="1"/>
@@ -14182,21 +14246,11 @@
     <row r="41" spans="19:19" ht="14" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="AB28:AJ28"/>
-    <mergeCell ref="AB29:AJ29"/>
-    <mergeCell ref="AL3:AN3"/>
-    <mergeCell ref="AB3:AJ3"/>
-    <mergeCell ref="V28:X29"/>
-    <mergeCell ref="V2:X3"/>
-    <mergeCell ref="T5:T26"/>
-    <mergeCell ref="Z5:Z26"/>
-    <mergeCell ref="AL15:AN15"/>
-    <mergeCell ref="AL4:AN12"/>
-    <mergeCell ref="AL17:AN17"/>
-    <mergeCell ref="AL18:AN18"/>
-    <mergeCell ref="AB4:AJ5"/>
-    <mergeCell ref="AB16:AJ17"/>
-    <mergeCell ref="AL19:AN19"/>
+    <mergeCell ref="D3:F4"/>
+    <mergeCell ref="J3:L7"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="D5:F5"/>
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="N18:O18"/>
     <mergeCell ref="Q18:R18"/>
@@ -14210,25 +14264,35 @@
     <mergeCell ref="J8:L8"/>
     <mergeCell ref="J10:L23"/>
     <mergeCell ref="H25:L29"/>
-    <mergeCell ref="D3:F4"/>
-    <mergeCell ref="J3:L7"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="T5:T26"/>
+    <mergeCell ref="Z5:Z26"/>
+    <mergeCell ref="AL15:AN15"/>
+    <mergeCell ref="AL4:AN12"/>
+    <mergeCell ref="AL17:AN17"/>
+    <mergeCell ref="AL18:AN18"/>
+    <mergeCell ref="AB4:AJ5"/>
+    <mergeCell ref="AB16:AJ17"/>
+    <mergeCell ref="AL19:AN19"/>
+    <mergeCell ref="AB28:AJ28"/>
+    <mergeCell ref="AB29:AJ29"/>
+    <mergeCell ref="AL3:AN3"/>
+    <mergeCell ref="AB3:AJ3"/>
+    <mergeCell ref="V28:X29"/>
+    <mergeCell ref="V2:X3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="44" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE3DEC1-8A52-4F6E-BFF3-45BA2A41D962}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:AC43"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="G1" zoomScale="84" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="84" workbookViewId="0">
       <selection activeCell="O45" sqref="O45"/>
     </sheetView>
   </sheetViews>
@@ -14245,27 +14309,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:29" ht="16" x14ac:dyDescent="0.35">
-      <c r="B2" s="276" t="s">
+      <c r="B2" s="296" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="276"/>
-      <c r="D2" s="276"/>
-      <c r="E2" s="276"/>
-      <c r="F2" s="276"/>
-      <c r="N2" s="249" t="s">
+      <c r="C2" s="296"/>
+      <c r="D2" s="296"/>
+      <c r="E2" s="296"/>
+      <c r="F2" s="296"/>
+      <c r="N2" s="261" t="s">
         <v>173</v>
       </c>
-      <c r="O2" s="249"/>
-      <c r="P2" s="249"/>
-      <c r="Q2" s="249"/>
-      <c r="R2" s="249"/>
-      <c r="T2" s="249" t="s">
+      <c r="O2" s="261"/>
+      <c r="P2" s="261"/>
+      <c r="Q2" s="261"/>
+      <c r="R2" s="261"/>
+      <c r="T2" s="261" t="s">
         <v>172</v>
       </c>
-      <c r="U2" s="249"/>
-      <c r="V2" s="249"/>
-      <c r="W2" s="249"/>
-      <c r="X2" s="249"/>
+      <c r="U2" s="261"/>
+      <c r="V2" s="261"/>
+      <c r="W2" s="261"/>
+      <c r="X2" s="261"/>
     </row>
     <row r="3" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="H3" s="24" t="s">
@@ -14274,34 +14338,34 @@
       <c r="I3" s="1">
         <v>20</v>
       </c>
-      <c r="N3" s="278" t="s">
+      <c r="N3" s="298" t="s">
         <v>176</v>
       </c>
-      <c r="O3" s="278"/>
-      <c r="P3" s="278"/>
-      <c r="Q3" s="278"/>
-      <c r="R3" s="278"/>
-      <c r="T3" s="278" t="s">
+      <c r="O3" s="298"/>
+      <c r="P3" s="298"/>
+      <c r="Q3" s="298"/>
+      <c r="R3" s="298"/>
+      <c r="T3" s="298" t="s">
         <v>177</v>
       </c>
-      <c r="U3" s="278"/>
-      <c r="V3" s="278"/>
-      <c r="W3" s="278"/>
-      <c r="X3" s="278"/>
-      <c r="Z3" s="248" t="s">
+      <c r="U3" s="298"/>
+      <c r="V3" s="298"/>
+      <c r="W3" s="298"/>
+      <c r="X3" s="298"/>
+      <c r="Z3" s="280" t="s">
         <v>34</v>
       </c>
-      <c r="AA3" s="248"/>
-      <c r="AB3" s="248"/>
+      <c r="AA3" s="280"/>
+      <c r="AB3" s="280"/>
     </row>
     <row r="4" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="26"/>
-      <c r="C4" s="277" t="s">
+      <c r="C4" s="297" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="275"/>
-      <c r="E4" s="275"/>
-      <c r="F4" s="275"/>
+      <c r="D4" s="291"/>
+      <c r="E4" s="291"/>
+      <c r="F4" s="291"/>
       <c r="H4" s="1" t="s">
         <v>4</v>
       </c>
@@ -14318,9 +14382,9 @@
       <c r="V4" s="20"/>
       <c r="W4" s="20"/>
       <c r="X4" s="22"/>
-      <c r="Z4" s="248"/>
-      <c r="AA4" s="248"/>
-      <c r="AB4" s="248"/>
+      <c r="Z4" s="280"/>
+      <c r="AA4" s="280"/>
+      <c r="AB4" s="280"/>
     </row>
     <row r="5" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="H5" s="1" t="s">
@@ -14329,44 +14393,44 @@
       <c r="I5" s="1">
         <v>20</v>
       </c>
-      <c r="Z5" s="248"/>
-      <c r="AA5" s="248"/>
-      <c r="AB5" s="248"/>
+      <c r="Z5" s="280"/>
+      <c r="AA5" s="280"/>
+      <c r="AB5" s="280"/>
       <c r="AC5" s="21"/>
     </row>
     <row r="6" spans="1:29" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="275" t="s">
+      <c r="C6" s="291" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="275"/>
-      <c r="E6" s="275"/>
-      <c r="F6" s="275"/>
+      <c r="D6" s="291"/>
+      <c r="E6" s="291"/>
+      <c r="F6" s="291"/>
       <c r="H6" s="1" t="s">
         <v>37</v>
       </c>
       <c r="I6" s="1">
         <v>20</v>
       </c>
-      <c r="N6" s="273" t="s">
+      <c r="N6" s="292" t="s">
         <v>199</v>
       </c>
-      <c r="O6" s="274"/>
-      <c r="Q6" s="273" t="s">
+      <c r="O6" s="293"/>
+      <c r="Q6" s="292" t="s">
         <v>199</v>
       </c>
-      <c r="R6" s="274"/>
-      <c r="T6" s="273" t="s">
+      <c r="R6" s="293"/>
+      <c r="T6" s="292" t="s">
         <v>203</v>
       </c>
-      <c r="U6" s="274"/>
+      <c r="U6" s="293"/>
       <c r="V6" s="27"/>
-      <c r="W6" s="273" t="s">
+      <c r="W6" s="292" t="s">
         <v>203</v>
       </c>
-      <c r="X6" s="274"/>
+      <c r="X6" s="293"/>
       <c r="Z6" s="21"/>
       <c r="AA6" s="21"/>
       <c r="AB6" s="21"/>
@@ -14374,22 +14438,22 @@
     </row>
     <row r="7" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="M7" s="29"/>
-      <c r="Z7" s="248" t="s">
+      <c r="Z7" s="280" t="s">
         <v>42</v>
       </c>
-      <c r="AA7" s="248"/>
-      <c r="AB7" s="248"/>
+      <c r="AA7" s="280"/>
+      <c r="AB7" s="280"/>
     </row>
     <row r="8" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="275" t="s">
+      <c r="C8" s="291" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="275"/>
-      <c r="E8" s="275"/>
-      <c r="F8" s="275"/>
+      <c r="D8" s="291"/>
+      <c r="E8" s="291"/>
+      <c r="F8" s="291"/>
       <c r="N8" s="30" t="s">
         <v>41</v>
       </c>
@@ -14414,25 +14478,25 @@
       <c r="X8" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="Z8" s="248"/>
-      <c r="AA8" s="248"/>
-      <c r="AB8" s="248"/>
+      <c r="Z8" s="280"/>
+      <c r="AA8" s="280"/>
+      <c r="AB8" s="280"/>
     </row>
     <row r="9" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="Z9" s="248"/>
-      <c r="AA9" s="248"/>
-      <c r="AB9" s="248"/>
+      <c r="Z9" s="280"/>
+      <c r="AA9" s="280"/>
+      <c r="AB9" s="280"/>
     </row>
     <row r="10" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="275" t="s">
+      <c r="C10" s="291" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="275"/>
-      <c r="E10" s="275"/>
-      <c r="F10" s="275"/>
+      <c r="D10" s="291"/>
+      <c r="E10" s="291"/>
+      <c r="F10" s="291"/>
       <c r="N10" s="34" t="s">
         <v>44</v>
       </c>
@@ -14462,36 +14526,36 @@
       <c r="AB10" s="38"/>
     </row>
     <row r="11" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N11" s="275" t="s">
+      <c r="N11" s="291" t="s">
         <v>58</v>
       </c>
-      <c r="O11" s="275"/>
-      <c r="Q11" s="275" t="s">
+      <c r="O11" s="291"/>
+      <c r="Q11" s="291" t="s">
         <v>58</v>
       </c>
-      <c r="R11" s="275"/>
-      <c r="T11" s="272" t="s">
+      <c r="R11" s="291"/>
+      <c r="T11" s="295" t="s">
         <v>59</v>
       </c>
-      <c r="U11" s="272"/>
-      <c r="W11" s="272" t="s">
+      <c r="U11" s="295"/>
+      <c r="W11" s="295" t="s">
         <v>59</v>
       </c>
-      <c r="X11" s="272"/>
-      <c r="Z11" s="248" t="s">
+      <c r="X11" s="295"/>
+      <c r="Z11" s="280" t="s">
         <v>49</v>
       </c>
-      <c r="AA11" s="248"/>
-      <c r="AB11" s="248"/>
+      <c r="AA11" s="280"/>
+      <c r="AB11" s="280"/>
     </row>
     <row r="12" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="279" t="s">
+      <c r="B12" s="294" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="279"/>
-      <c r="D12" s="279"/>
-      <c r="E12" s="279"/>
-      <c r="F12" s="279"/>
+      <c r="C12" s="294"/>
+      <c r="D12" s="294"/>
+      <c r="E12" s="294"/>
+      <c r="F12" s="294"/>
       <c r="N12" s="40" t="s">
         <v>45</v>
       </c>
@@ -14516,46 +14580,46 @@
       <c r="X12" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="Z12" s="248"/>
-      <c r="AA12" s="248"/>
-      <c r="AB12" s="248"/>
+      <c r="Z12" s="280"/>
+      <c r="AA12" s="280"/>
+      <c r="AB12" s="280"/>
     </row>
     <row r="13" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N13" s="275" t="s">
+      <c r="N13" s="291" t="s">
         <v>61</v>
       </c>
-      <c r="O13" s="275"/>
-      <c r="Q13" s="275" t="s">
+      <c r="O13" s="291"/>
+      <c r="Q13" s="291" t="s">
         <v>61</v>
       </c>
-      <c r="R13" s="275"/>
-      <c r="T13" s="275" t="s">
+      <c r="R13" s="291"/>
+      <c r="T13" s="291" t="s">
         <v>62</v>
       </c>
-      <c r="U13" s="275"/>
-      <c r="W13" s="275" t="s">
+      <c r="U13" s="291"/>
+      <c r="W13" s="291" t="s">
         <v>62</v>
       </c>
-      <c r="X13" s="275"/>
-      <c r="Z13" s="248"/>
-      <c r="AA13" s="248"/>
-      <c r="AB13" s="248"/>
+      <c r="X13" s="291"/>
+      <c r="Z13" s="280"/>
+      <c r="AA13" s="280"/>
+      <c r="AB13" s="280"/>
     </row>
     <row r="14" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="280" t="s">
+      <c r="B14" s="289" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="280"/>
-      <c r="D14" s="280"/>
-      <c r="E14" s="280"/>
-      <c r="F14" s="280"/>
-      <c r="H14" s="281" t="s">
+      <c r="C14" s="289"/>
+      <c r="D14" s="289"/>
+      <c r="E14" s="289"/>
+      <c r="F14" s="289"/>
+      <c r="H14" s="290" t="s">
         <v>5</v>
       </c>
-      <c r="I14" s="281"/>
-      <c r="J14" s="281"/>
-      <c r="K14" s="281"/>
-      <c r="L14" s="281"/>
+      <c r="I14" s="290"/>
+      <c r="J14" s="290"/>
+      <c r="K14" s="290"/>
+      <c r="L14" s="290"/>
       <c r="N14" s="44" t="s">
         <v>175</v>
       </c>
@@ -14582,30 +14646,30 @@
       </c>
     </row>
     <row r="15" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N15" s="275" t="s">
+      <c r="N15" s="291" t="s">
         <v>65</v>
       </c>
-      <c r="O15" s="275"/>
-      <c r="Q15" s="275" t="s">
+      <c r="O15" s="291"/>
+      <c r="Q15" s="291" t="s">
         <v>65</v>
       </c>
-      <c r="R15" s="275"/>
-      <c r="T15" s="275" t="s">
+      <c r="R15" s="291"/>
+      <c r="T15" s="291" t="s">
         <v>64</v>
       </c>
-      <c r="U15" s="275"/>
-      <c r="W15" s="275" t="s">
+      <c r="U15" s="291"/>
+      <c r="W15" s="291" t="s">
         <v>64</v>
       </c>
-      <c r="X15" s="275"/>
-      <c r="Z15" s="248" t="s">
+      <c r="X15" s="291"/>
+      <c r="Z15" s="280" t="s">
         <v>55</v>
       </c>
-      <c r="AA15" s="248"/>
-      <c r="AB15" s="248"/>
+      <c r="AA15" s="280"/>
+      <c r="AB15" s="280"/>
     </row>
     <row r="16" spans="1:29" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="282">
+      <c r="A16" s="283">
         <v>1</v>
       </c>
       <c r="B16" s="45" t="s">
@@ -14614,7 +14678,7 @@
       <c r="C16" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="283">
+      <c r="D16" s="284">
         <v>3</v>
       </c>
       <c r="E16" s="45" t="s">
@@ -14623,7 +14687,7 @@
       <c r="F16" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="282">
+      <c r="G16" s="283">
         <v>1</v>
       </c>
       <c r="H16" s="47" t="s">
@@ -14632,7 +14696,7 @@
       <c r="I16" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="J16" s="283">
+      <c r="J16" s="284">
         <v>3</v>
       </c>
       <c r="K16" s="47" t="s">
@@ -14641,63 +14705,63 @@
       <c r="L16" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="Z16" s="248"/>
-      <c r="AA16" s="248"/>
-      <c r="AB16" s="248"/>
+      <c r="Z16" s="280"/>
+      <c r="AA16" s="280"/>
+      <c r="AB16" s="280"/>
     </row>
     <row r="17" spans="1:28" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="282"/>
+      <c r="A17" s="283"/>
       <c r="B17" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="283"/>
+      <c r="D17" s="284"/>
       <c r="E17" s="49" t="s">
         <v>15</v>
       </c>
       <c r="F17" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="282"/>
+      <c r="G17" s="283"/>
       <c r="H17" s="51" t="s">
         <v>16</v>
       </c>
       <c r="I17" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="283"/>
+      <c r="J17" s="284"/>
       <c r="K17" s="51" t="s">
         <v>15</v>
       </c>
       <c r="L17" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="N17" s="273" t="s">
+      <c r="N17" s="292" t="s">
         <v>200</v>
       </c>
-      <c r="O17" s="274"/>
+      <c r="O17" s="293"/>
       <c r="P17" s="27"/>
-      <c r="Q17" s="273" t="s">
+      <c r="Q17" s="292" t="s">
         <v>200</v>
       </c>
-      <c r="R17" s="274"/>
-      <c r="T17" s="273" t="s">
+      <c r="R17" s="293"/>
+      <c r="T17" s="292" t="s">
         <v>201</v>
       </c>
-      <c r="U17" s="274"/>
-      <c r="W17" s="273" t="s">
+      <c r="U17" s="293"/>
+      <c r="W17" s="292" t="s">
         <v>202</v>
       </c>
-      <c r="X17" s="274"/>
-      <c r="Z17" s="248"/>
-      <c r="AA17" s="248"/>
-      <c r="AB17" s="248"/>
+      <c r="X17" s="293"/>
+      <c r="Z17" s="280"/>
+      <c r="AA17" s="280"/>
+      <c r="AB17" s="280"/>
     </row>
     <row r="18" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="19" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="282">
+      <c r="A19" s="283">
         <v>2</v>
       </c>
       <c r="B19" s="45" t="s">
@@ -14706,7 +14770,7 @@
       <c r="C19" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="283">
+      <c r="D19" s="284">
         <v>4</v>
       </c>
       <c r="E19" s="45" t="s">
@@ -14715,7 +14779,7 @@
       <c r="F19" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="282">
+      <c r="G19" s="283">
         <v>2</v>
       </c>
       <c r="H19" s="47" t="s">
@@ -14724,7 +14788,7 @@
       <c r="I19" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="J19" s="283">
+      <c r="J19" s="284">
         <v>4</v>
       </c>
       <c r="K19" s="47" t="s">
@@ -14757,44 +14821,44 @@
       <c r="X19" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="Z19" s="248" t="s">
+      <c r="Z19" s="280" t="s">
         <v>57</v>
       </c>
-      <c r="AA19" s="248"/>
-      <c r="AB19" s="248"/>
+      <c r="AA19" s="280"/>
+      <c r="AB19" s="280"/>
     </row>
     <row r="20" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="282"/>
+      <c r="A20" s="283"/>
       <c r="B20" s="49" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="283"/>
+      <c r="D20" s="284"/>
       <c r="E20" s="49" t="s">
         <v>15</v>
       </c>
       <c r="F20" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="282"/>
+      <c r="G20" s="283"/>
       <c r="H20" s="51" t="s">
         <v>16</v>
       </c>
       <c r="I20" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="J20" s="283"/>
+      <c r="J20" s="284"/>
       <c r="K20" s="51" t="s">
         <v>15</v>
       </c>
       <c r="L20" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="Z20" s="248"/>
-      <c r="AA20" s="248"/>
-      <c r="AB20" s="248"/>
+      <c r="Z20" s="280"/>
+      <c r="AA20" s="280"/>
+      <c r="AB20" s="280"/>
     </row>
     <row r="21" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
       <c r="N21" s="35" t="s">
@@ -14821,43 +14885,43 @@
       <c r="X21" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="Z21" s="248"/>
-      <c r="AA21" s="248"/>
-      <c r="AB21" s="248"/>
+      <c r="Z21" s="280"/>
+      <c r="AA21" s="280"/>
+      <c r="AB21" s="280"/>
     </row>
     <row r="22" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N22" s="272" t="s">
+      <c r="N22" s="295" t="s">
         <v>47</v>
       </c>
-      <c r="O22" s="272"/>
-      <c r="Q22" s="272" t="s">
+      <c r="O22" s="295"/>
+      <c r="Q22" s="295" t="s">
         <v>47</v>
       </c>
-      <c r="R22" s="272"/>
-      <c r="T22" s="275" t="s">
+      <c r="R22" s="295"/>
+      <c r="T22" s="291" t="s">
         <v>48</v>
       </c>
-      <c r="U22" s="275"/>
-      <c r="W22" s="275" t="s">
+      <c r="U22" s="291"/>
+      <c r="W22" s="291" t="s">
         <v>48</v>
       </c>
-      <c r="X22" s="275"/>
+      <c r="X22" s="291"/>
     </row>
     <row r="23" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="285" t="s">
+      <c r="B23" s="286" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="285"/>
-      <c r="D23" s="285"/>
-      <c r="E23" s="285"/>
-      <c r="F23" s="285"/>
-      <c r="H23" s="248" t="s">
+      <c r="C23" s="286"/>
+      <c r="D23" s="286"/>
+      <c r="E23" s="286"/>
+      <c r="F23" s="286"/>
+      <c r="H23" s="280" t="s">
         <v>60</v>
       </c>
-      <c r="I23" s="248"/>
-      <c r="J23" s="248"/>
-      <c r="K23" s="248"/>
-      <c r="L23" s="248"/>
+      <c r="I23" s="280"/>
+      <c r="J23" s="280"/>
+      <c r="K23" s="280"/>
+      <c r="L23" s="280"/>
       <c r="N23" s="39" t="s">
         <v>46</v>
       </c>
@@ -14882,40 +14946,40 @@
       <c r="X23" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="Z23" s="248" t="s">
+      <c r="Z23" s="280" t="s">
         <v>63</v>
       </c>
-      <c r="AA23" s="248"/>
-      <c r="AB23" s="248"/>
+      <c r="AA23" s="280"/>
+      <c r="AB23" s="280"/>
     </row>
     <row r="24" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H24" s="248"/>
-      <c r="I24" s="248"/>
-      <c r="J24" s="248"/>
-      <c r="K24" s="248"/>
-      <c r="L24" s="248"/>
-      <c r="N24" s="275" t="s">
+      <c r="H24" s="280"/>
+      <c r="I24" s="280"/>
+      <c r="J24" s="280"/>
+      <c r="K24" s="280"/>
+      <c r="L24" s="280"/>
+      <c r="N24" s="291" t="s">
         <v>51</v>
       </c>
-      <c r="O24" s="275"/>
-      <c r="Q24" s="275" t="s">
+      <c r="O24" s="291"/>
+      <c r="Q24" s="291" t="s">
         <v>51</v>
       </c>
-      <c r="R24" s="275"/>
-      <c r="T24" s="275" t="s">
+      <c r="R24" s="291"/>
+      <c r="T24" s="291" t="s">
         <v>52</v>
       </c>
-      <c r="U24" s="275"/>
-      <c r="W24" s="275" t="s">
+      <c r="U24" s="291"/>
+      <c r="W24" s="291" t="s">
         <v>52</v>
       </c>
-      <c r="X24" s="275"/>
-      <c r="Z24" s="248"/>
-      <c r="AA24" s="248"/>
-      <c r="AB24" s="248"/>
+      <c r="X24" s="291"/>
+      <c r="Z24" s="280"/>
+      <c r="AA24" s="280"/>
+      <c r="AB24" s="280"/>
     </row>
     <row r="25" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="282">
+      <c r="A25" s="283">
         <v>1</v>
       </c>
       <c r="B25" s="53" t="s">
@@ -14924,7 +14988,7 @@
       <c r="C25" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="283">
+      <c r="D25" s="284">
         <v>3</v>
       </c>
       <c r="E25" s="53" t="s">
@@ -14933,11 +14997,11 @@
       <c r="F25" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="248"/>
-      <c r="I25" s="248"/>
-      <c r="J25" s="248"/>
-      <c r="K25" s="248"/>
-      <c r="L25" s="248"/>
+      <c r="H25" s="280"/>
+      <c r="I25" s="280"/>
+      <c r="J25" s="280"/>
+      <c r="K25" s="280"/>
+      <c r="L25" s="280"/>
       <c r="N25" s="42" t="s">
         <v>45</v>
       </c>
@@ -14962,53 +15026,53 @@
       <c r="X25" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="Z25" s="248"/>
-      <c r="AA25" s="248"/>
-      <c r="AB25" s="248"/>
+      <c r="Z25" s="280"/>
+      <c r="AA25" s="280"/>
+      <c r="AB25" s="280"/>
     </row>
     <row r="26" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="282"/>
+      <c r="A26" s="283"/>
       <c r="B26" s="55" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="283"/>
+      <c r="D26" s="284"/>
       <c r="E26" s="55" t="s">
         <v>15</v>
       </c>
       <c r="F26" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="H26" s="248"/>
-      <c r="I26" s="248"/>
-      <c r="J26" s="248"/>
-      <c r="K26" s="248"/>
-      <c r="L26" s="248"/>
-      <c r="N26" s="275" t="s">
+      <c r="H26" s="280"/>
+      <c r="I26" s="280"/>
+      <c r="J26" s="280"/>
+      <c r="K26" s="280"/>
+      <c r="L26" s="280"/>
+      <c r="N26" s="291" t="s">
         <v>54</v>
       </c>
-      <c r="O26" s="275"/>
-      <c r="Q26" s="275" t="s">
+      <c r="O26" s="291"/>
+      <c r="Q26" s="291" t="s">
         <v>54</v>
       </c>
-      <c r="R26" s="275"/>
-      <c r="T26" s="275" t="s">
+      <c r="R26" s="291"/>
+      <c r="T26" s="291" t="s">
         <v>53</v>
       </c>
-      <c r="U26" s="275"/>
-      <c r="W26" s="275" t="s">
+      <c r="U26" s="291"/>
+      <c r="W26" s="291" t="s">
         <v>53</v>
       </c>
-      <c r="X26" s="275"/>
+      <c r="X26" s="291"/>
     </row>
     <row r="27" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H27" s="248"/>
-      <c r="I27" s="248"/>
-      <c r="J27" s="248"/>
-      <c r="K27" s="248"/>
-      <c r="L27" s="248"/>
+      <c r="H27" s="280"/>
+      <c r="I27" s="280"/>
+      <c r="J27" s="280"/>
+      <c r="K27" s="280"/>
+      <c r="L27" s="280"/>
       <c r="N27" s="57"/>
       <c r="O27" s="210"/>
       <c r="P27" s="210"/>
@@ -15021,7 +15085,7 @@
       <c r="X27" s="23"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A28" s="282">
+      <c r="A28" s="283">
         <v>2</v>
       </c>
       <c r="B28" s="53" t="s">
@@ -15030,7 +15094,7 @@
       <c r="C28" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="D28" s="283">
+      <c r="D28" s="284">
         <v>4</v>
       </c>
       <c r="E28" s="53" t="s">
@@ -15039,49 +15103,49 @@
       <c r="F28" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="H28" s="248"/>
-      <c r="I28" s="248"/>
-      <c r="J28" s="248"/>
-      <c r="K28" s="248"/>
-      <c r="L28" s="248"/>
-      <c r="N28" s="286" t="s">
+      <c r="H28" s="280"/>
+      <c r="I28" s="280"/>
+      <c r="J28" s="280"/>
+      <c r="K28" s="280"/>
+      <c r="L28" s="280"/>
+      <c r="N28" s="287" t="s">
         <v>179</v>
       </c>
-      <c r="O28" s="286"/>
-      <c r="P28" s="286"/>
-      <c r="Q28" s="286"/>
-      <c r="R28" s="286"/>
+      <c r="O28" s="287"/>
+      <c r="P28" s="287"/>
+      <c r="Q28" s="287"/>
+      <c r="R28" s="287"/>
       <c r="S28" s="58"/>
-      <c r="T28" s="287" t="s">
+      <c r="T28" s="288" t="s">
         <v>178</v>
       </c>
-      <c r="U28" s="287"/>
-      <c r="V28" s="287"/>
-      <c r="W28" s="287"/>
-      <c r="X28" s="287"/>
+      <c r="U28" s="288"/>
+      <c r="V28" s="288"/>
+      <c r="W28" s="288"/>
+      <c r="X28" s="288"/>
     </row>
     <row r="29" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="282"/>
+      <c r="A29" s="283"/>
       <c r="B29" s="55" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="283"/>
+      <c r="D29" s="284"/>
       <c r="E29" s="55" t="s">
         <v>15</v>
       </c>
       <c r="F29" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="284" t="s">
+      <c r="H29" s="285" t="s">
         <v>66</v>
       </c>
-      <c r="I29" s="284"/>
-      <c r="J29" s="284"/>
-      <c r="K29" s="284"/>
-      <c r="L29" s="284"/>
+      <c r="I29" s="285"/>
+      <c r="J29" s="285"/>
+      <c r="K29" s="285"/>
+      <c r="L29" s="285"/>
       <c r="N29" s="59"/>
       <c r="O29" s="59"/>
       <c r="P29" s="58"/>
@@ -15234,11 +15298,11 @@
       <c r="E39" s="220" t="s">
         <v>9</v>
       </c>
-      <c r="G39" s="248" t="s">
+      <c r="G39" s="280" t="s">
         <v>189</v>
       </c>
-      <c r="H39" s="248"/>
-      <c r="I39" s="248"/>
+      <c r="H39" s="280"/>
+      <c r="I39" s="280"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B40" s="223"/>
@@ -15251,9 +15315,9 @@
       <c r="E40" s="220" t="s">
         <v>8</v>
       </c>
-      <c r="G40" s="248"/>
-      <c r="H40" s="248"/>
-      <c r="I40" s="248"/>
+      <c r="G40" s="280"/>
+      <c r="H40" s="280"/>
+      <c r="I40" s="280"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B41" s="225"/>
@@ -15298,36 +15362,28 @@
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="G39:I40"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="H29:L29"/>
-    <mergeCell ref="Z23:AB25"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="H23:L28"/>
-    <mergeCell ref="N28:R28"/>
-    <mergeCell ref="T28:X28"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="Z19:AB21"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="H14:L14"/>
-    <mergeCell ref="W13:X13"/>
-    <mergeCell ref="Z15:AB17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="W15:X15"/>
-    <mergeCell ref="T17:U17"/>
-    <mergeCell ref="W17:X17"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="T15:U15"/>
+    <mergeCell ref="W11:X11"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="T22:U22"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="T26:U26"/>
+    <mergeCell ref="W22:X22"/>
+    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="T2:X2"/>
+    <mergeCell ref="Z3:AB5"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="N3:R3"/>
+    <mergeCell ref="T3:X3"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="Z7:AB9"/>
     <mergeCell ref="C8:F8"/>
@@ -15344,28 +15400,36 @@
     <mergeCell ref="Q11:R11"/>
     <mergeCell ref="T11:U11"/>
     <mergeCell ref="T13:U13"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="T2:X2"/>
-    <mergeCell ref="Z3:AB5"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="N3:R3"/>
-    <mergeCell ref="T3:X3"/>
-    <mergeCell ref="W11:X11"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="N17:O17"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="Q22:R22"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="T22:U22"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="T26:U26"/>
-    <mergeCell ref="W22:X22"/>
-    <mergeCell ref="W24:X24"/>
-    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="H14:L14"/>
+    <mergeCell ref="W13:X13"/>
+    <mergeCell ref="Z15:AB17"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="W15:X15"/>
+    <mergeCell ref="T17:U17"/>
+    <mergeCell ref="W17:X17"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="T15:U15"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="Z19:AB21"/>
+    <mergeCell ref="G39:I40"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="Z23:AB25"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="H23:L28"/>
+    <mergeCell ref="N28:R28"/>
+    <mergeCell ref="T28:X28"/>
   </mergeCells>
   <pageMargins left="2.56" right="2.15" top="0.75" bottom="0.75" header="0.61" footer="0.3"/>
   <pageSetup scale="32" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -15373,14 +15437,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B56F31A9-A5D7-41B5-92A8-08C9990FECCF}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B2:S38"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D2" zoomScale="77" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="77" workbookViewId="0">
       <selection activeCell="B7" sqref="B7:M11"/>
     </sheetView>
   </sheetViews>
@@ -15394,10 +15458,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B2" s="289" t="s">
+      <c r="B2" s="300" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="289"/>
+      <c r="C2" s="300"/>
       <c r="D2" s="60"/>
       <c r="E2" s="60"/>
       <c r="F2" s="60"/>
@@ -15411,28 +15475,28 @@
       <c r="N2" s="60"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B3" s="263" t="s">
+      <c r="B3" s="282" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="263"/>
-      <c r="D3" s="263"/>
-      <c r="E3" s="263"/>
-      <c r="F3" s="263"/>
-      <c r="G3" s="263"/>
-      <c r="H3" s="263"/>
-      <c r="I3" s="263"/>
-      <c r="J3" s="263"/>
-      <c r="K3" s="263"/>
-      <c r="L3" s="263"/>
-      <c r="M3" s="263"/>
+      <c r="C3" s="282"/>
+      <c r="D3" s="282"/>
+      <c r="E3" s="282"/>
+      <c r="F3" s="282"/>
+      <c r="G3" s="282"/>
+      <c r="H3" s="282"/>
+      <c r="I3" s="282"/>
+      <c r="J3" s="282"/>
+      <c r="K3" s="282"/>
+      <c r="L3" s="282"/>
+      <c r="M3" s="282"/>
       <c r="N3" s="60"/>
-      <c r="O3" s="268" t="s">
+      <c r="O3" s="258" t="s">
         <v>147</v>
       </c>
-      <c r="P3" s="268"/>
-      <c r="Q3" s="268"/>
-      <c r="R3" s="268"/>
-      <c r="S3" s="263"/>
+      <c r="P3" s="258"/>
+      <c r="Q3" s="258"/>
+      <c r="R3" s="258"/>
+      <c r="S3" s="282"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B4" s="62">
@@ -15472,164 +15536,164 @@
         <v>12</v>
       </c>
       <c r="N4" s="127"/>
-      <c r="O4" s="268"/>
-      <c r="P4" s="268"/>
-      <c r="Q4" s="268"/>
-      <c r="R4" s="268"/>
-      <c r="S4" s="263"/>
+      <c r="O4" s="258"/>
+      <c r="P4" s="258"/>
+      <c r="Q4" s="258"/>
+      <c r="R4" s="258"/>
+      <c r="S4" s="282"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B5" s="290" t="s">
+      <c r="B5" s="301" t="s">
         <v>69</v>
       </c>
-      <c r="C5" s="291"/>
-      <c r="D5" s="290" t="s">
+      <c r="C5" s="302"/>
+      <c r="D5" s="301" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="291"/>
-      <c r="F5" s="290" t="s">
+      <c r="E5" s="302"/>
+      <c r="F5" s="301" t="s">
         <v>69</v>
       </c>
-      <c r="G5" s="291"/>
-      <c r="H5" s="290" t="s">
+      <c r="G5" s="302"/>
+      <c r="H5" s="301" t="s">
         <v>70</v>
       </c>
-      <c r="I5" s="291"/>
-      <c r="J5" s="290" t="s">
+      <c r="I5" s="302"/>
+      <c r="J5" s="301" t="s">
         <v>69</v>
       </c>
-      <c r="K5" s="292"/>
-      <c r="L5" s="290" t="s">
+      <c r="K5" s="303"/>
+      <c r="L5" s="301" t="s">
         <v>70</v>
       </c>
-      <c r="M5" s="292"/>
+      <c r="M5" s="303"/>
       <c r="N5" s="60"/>
-      <c r="S5" s="263"/>
+      <c r="S5" s="282"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B6" s="63"/>
-      <c r="O6" s="248" t="s">
+      <c r="O6" s="280" t="s">
         <v>149</v>
       </c>
-      <c r="P6" s="248"/>
-      <c r="Q6" s="248"/>
-      <c r="R6" s="248"/>
-      <c r="S6" s="263"/>
+      <c r="P6" s="280"/>
+      <c r="Q6" s="280"/>
+      <c r="R6" s="280"/>
+      <c r="S6" s="282"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B7" s="248" t="s">
+      <c r="B7" s="280" t="s">
         <v>190</v>
       </c>
-      <c r="C7" s="248"/>
-      <c r="D7" s="248"/>
-      <c r="E7" s="248"/>
-      <c r="F7" s="248"/>
-      <c r="G7" s="248"/>
-      <c r="H7" s="248"/>
-      <c r="I7" s="248"/>
-      <c r="J7" s="248"/>
-      <c r="K7" s="248"/>
-      <c r="L7" s="248"/>
-      <c r="M7" s="248"/>
+      <c r="C7" s="280"/>
+      <c r="D7" s="280"/>
+      <c r="E7" s="280"/>
+      <c r="F7" s="280"/>
+      <c r="G7" s="280"/>
+      <c r="H7" s="280"/>
+      <c r="I7" s="280"/>
+      <c r="J7" s="280"/>
+      <c r="K7" s="280"/>
+      <c r="L7" s="280"/>
+      <c r="M7" s="280"/>
       <c r="N7" s="141"/>
-      <c r="O7" s="248"/>
-      <c r="P7" s="248"/>
-      <c r="Q7" s="248"/>
-      <c r="R7" s="248"/>
-      <c r="S7" s="263"/>
+      <c r="O7" s="280"/>
+      <c r="P7" s="280"/>
+      <c r="Q7" s="280"/>
+      <c r="R7" s="280"/>
+      <c r="S7" s="282"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B8" s="248"/>
-      <c r="C8" s="248"/>
-      <c r="D8" s="248"/>
-      <c r="E8" s="248"/>
-      <c r="F8" s="248"/>
-      <c r="G8" s="248"/>
-      <c r="H8" s="248"/>
-      <c r="I8" s="248"/>
-      <c r="J8" s="248"/>
-      <c r="K8" s="248"/>
-      <c r="L8" s="248"/>
-      <c r="M8" s="248"/>
+      <c r="B8" s="280"/>
+      <c r="C8" s="280"/>
+      <c r="D8" s="280"/>
+      <c r="E8" s="280"/>
+      <c r="F8" s="280"/>
+      <c r="G8" s="280"/>
+      <c r="H8" s="280"/>
+      <c r="I8" s="280"/>
+      <c r="J8" s="280"/>
+      <c r="K8" s="280"/>
+      <c r="L8" s="280"/>
+      <c r="M8" s="280"/>
       <c r="N8" s="141"/>
-      <c r="O8" s="248"/>
-      <c r="P8" s="248"/>
-      <c r="Q8" s="248"/>
-      <c r="R8" s="248"/>
-      <c r="S8" s="263"/>
+      <c r="O8" s="280"/>
+      <c r="P8" s="280"/>
+      <c r="Q8" s="280"/>
+      <c r="R8" s="280"/>
+      <c r="S8" s="282"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B9" s="248"/>
-      <c r="C9" s="248"/>
-      <c r="D9" s="248"/>
-      <c r="E9" s="248"/>
-      <c r="F9" s="248"/>
-      <c r="G9" s="248"/>
-      <c r="H9" s="248"/>
-      <c r="I9" s="248"/>
-      <c r="J9" s="248"/>
-      <c r="K9" s="248"/>
-      <c r="L9" s="248"/>
-      <c r="M9" s="248"/>
+      <c r="B9" s="280"/>
+      <c r="C9" s="280"/>
+      <c r="D9" s="280"/>
+      <c r="E9" s="280"/>
+      <c r="F9" s="280"/>
+      <c r="G9" s="280"/>
+      <c r="H9" s="280"/>
+      <c r="I9" s="280"/>
+      <c r="J9" s="280"/>
+      <c r="K9" s="280"/>
+      <c r="L9" s="280"/>
+      <c r="M9" s="280"/>
       <c r="N9" s="141"/>
-      <c r="O9" s="248"/>
-      <c r="P9" s="248"/>
-      <c r="Q9" s="248"/>
-      <c r="R9" s="248"/>
-      <c r="S9" s="263"/>
+      <c r="O9" s="280"/>
+      <c r="P9" s="280"/>
+      <c r="Q9" s="280"/>
+      <c r="R9" s="280"/>
+      <c r="S9" s="282"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B10" s="248"/>
-      <c r="C10" s="248"/>
-      <c r="D10" s="248"/>
-      <c r="E10" s="248"/>
-      <c r="F10" s="248"/>
-      <c r="G10" s="248"/>
-      <c r="H10" s="248"/>
-      <c r="I10" s="248"/>
-      <c r="J10" s="248"/>
-      <c r="K10" s="248"/>
-      <c r="L10" s="248"/>
-      <c r="M10" s="248"/>
+      <c r="B10" s="280"/>
+      <c r="C10" s="280"/>
+      <c r="D10" s="280"/>
+      <c r="E10" s="280"/>
+      <c r="F10" s="280"/>
+      <c r="G10" s="280"/>
+      <c r="H10" s="280"/>
+      <c r="I10" s="280"/>
+      <c r="J10" s="280"/>
+      <c r="K10" s="280"/>
+      <c r="L10" s="280"/>
+      <c r="M10" s="280"/>
       <c r="N10" s="141"/>
-      <c r="O10" s="248"/>
-      <c r="P10" s="248"/>
-      <c r="Q10" s="248"/>
-      <c r="R10" s="248"/>
-      <c r="S10" s="263"/>
+      <c r="O10" s="280"/>
+      <c r="P10" s="280"/>
+      <c r="Q10" s="280"/>
+      <c r="R10" s="280"/>
+      <c r="S10" s="282"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B11" s="248"/>
-      <c r="C11" s="248"/>
-      <c r="D11" s="248"/>
-      <c r="E11" s="248"/>
-      <c r="F11" s="248"/>
-      <c r="G11" s="248"/>
-      <c r="H11" s="248"/>
-      <c r="I11" s="248"/>
-      <c r="J11" s="248"/>
-      <c r="K11" s="248"/>
-      <c r="L11" s="248"/>
-      <c r="M11" s="248"/>
+      <c r="B11" s="280"/>
+      <c r="C11" s="280"/>
+      <c r="D11" s="280"/>
+      <c r="E11" s="280"/>
+      <c r="F11" s="280"/>
+      <c r="G11" s="280"/>
+      <c r="H11" s="280"/>
+      <c r="I11" s="280"/>
+      <c r="J11" s="280"/>
+      <c r="K11" s="280"/>
+      <c r="L11" s="280"/>
+      <c r="M11" s="280"/>
       <c r="N11" s="141"/>
-      <c r="O11" s="248"/>
-      <c r="P11" s="248"/>
-      <c r="Q11" s="248"/>
-      <c r="R11" s="248"/>
-      <c r="S11" s="263"/>
+      <c r="O11" s="280"/>
+      <c r="P11" s="280"/>
+      <c r="Q11" s="280"/>
+      <c r="R11" s="280"/>
+      <c r="S11" s="282"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="O12" s="248"/>
-      <c r="P12" s="248"/>
-      <c r="Q12" s="248"/>
-      <c r="R12" s="248"/>
-      <c r="S12" s="263"/>
+      <c r="O12" s="280"/>
+      <c r="P12" s="280"/>
+      <c r="Q12" s="280"/>
+      <c r="R12" s="280"/>
+      <c r="S12" s="282"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B13" s="288" t="s">
+      <c r="B13" s="299" t="s">
         <v>153</v>
       </c>
-      <c r="C13" s="288"/>
+      <c r="C13" s="299"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B14" s="60">
@@ -15646,12 +15710,12 @@
       <c r="C15" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="O15" s="248" t="s">
+      <c r="O15" s="280" t="s">
         <v>148</v>
       </c>
-      <c r="P15" s="248"/>
-      <c r="Q15" s="248"/>
-      <c r="R15" s="248"/>
+      <c r="P15" s="280"/>
+      <c r="Q15" s="280"/>
+      <c r="R15" s="280"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B16" s="60">
@@ -15660,10 +15724,10 @@
       <c r="C16" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="O16" s="248"/>
-      <c r="P16" s="248"/>
-      <c r="Q16" s="248"/>
-      <c r="R16" s="248"/>
+      <c r="O16" s="280"/>
+      <c r="P16" s="280"/>
+      <c r="Q16" s="280"/>
+      <c r="R16" s="280"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B17" s="60">
@@ -15680,12 +15744,12 @@
       <c r="C18" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="O18" s="248" t="s">
+      <c r="O18" s="280" t="s">
         <v>150</v>
       </c>
-      <c r="P18" s="248"/>
-      <c r="Q18" s="248"/>
-      <c r="R18" s="248"/>
+      <c r="P18" s="280"/>
+      <c r="Q18" s="280"/>
+      <c r="R18" s="280"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B19" s="60">
@@ -15694,97 +15758,97 @@
       <c r="C19" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="O19" s="248"/>
-      <c r="P19" s="248"/>
-      <c r="Q19" s="248"/>
-      <c r="R19" s="248"/>
+      <c r="O19" s="280"/>
+      <c r="P19" s="280"/>
+      <c r="Q19" s="280"/>
+      <c r="R19" s="280"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O20" s="248"/>
-      <c r="P20" s="248"/>
-      <c r="Q20" s="248"/>
-      <c r="R20" s="248"/>
+      <c r="O20" s="280"/>
+      <c r="P20" s="280"/>
+      <c r="Q20" s="280"/>
+      <c r="R20" s="280"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O21" s="248"/>
-      <c r="P21" s="248"/>
-      <c r="Q21" s="248"/>
-      <c r="R21" s="248"/>
+      <c r="O21" s="280"/>
+      <c r="P21" s="280"/>
+      <c r="Q21" s="280"/>
+      <c r="R21" s="280"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O22" s="248"/>
-      <c r="P22" s="248"/>
-      <c r="Q22" s="248"/>
-      <c r="R22" s="248"/>
+      <c r="O22" s="280"/>
+      <c r="P22" s="280"/>
+      <c r="Q22" s="280"/>
+      <c r="R22" s="280"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O23" s="248"/>
-      <c r="P23" s="248"/>
-      <c r="Q23" s="248"/>
-      <c r="R23" s="248"/>
+      <c r="O23" s="280"/>
+      <c r="P23" s="280"/>
+      <c r="Q23" s="280"/>
+      <c r="R23" s="280"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O27" s="268" t="s">
+      <c r="O27" s="258" t="s">
         <v>146</v>
       </c>
-      <c r="P27" s="268"/>
-      <c r="Q27" s="268"/>
-      <c r="R27" s="268"/>
+      <c r="P27" s="258"/>
+      <c r="Q27" s="258"/>
+      <c r="R27" s="258"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O28" s="268"/>
-      <c r="P28" s="268"/>
-      <c r="Q28" s="268"/>
-      <c r="R28" s="268"/>
+      <c r="O28" s="258"/>
+      <c r="P28" s="258"/>
+      <c r="Q28" s="258"/>
+      <c r="R28" s="258"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O30" s="248" t="s">
+      <c r="O30" s="280" t="s">
         <v>145</v>
       </c>
-      <c r="P30" s="248"/>
-      <c r="Q30" s="248"/>
-      <c r="R30" s="248"/>
+      <c r="P30" s="280"/>
+      <c r="Q30" s="280"/>
+      <c r="R30" s="280"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.35">
-      <c r="O31" s="248"/>
-      <c r="P31" s="248"/>
-      <c r="Q31" s="248"/>
-      <c r="R31" s="248"/>
+      <c r="O31" s="280"/>
+      <c r="P31" s="280"/>
+      <c r="Q31" s="280"/>
+      <c r="R31" s="280"/>
     </row>
     <row r="32" spans="2:18" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="M32" s="73"/>
       <c r="N32" s="73"/>
-      <c r="O32" s="248"/>
-      <c r="P32" s="248"/>
-      <c r="Q32" s="248"/>
-      <c r="R32" s="248"/>
+      <c r="O32" s="280"/>
+      <c r="P32" s="280"/>
+      <c r="Q32" s="280"/>
+      <c r="R32" s="280"/>
     </row>
     <row r="33" spans="12:18" x14ac:dyDescent="0.35">
       <c r="L33" s="73"/>
       <c r="M33" s="73"/>
       <c r="N33" s="73"/>
-      <c r="O33" s="248"/>
-      <c r="P33" s="248"/>
-      <c r="Q33" s="248"/>
-      <c r="R33" s="248"/>
+      <c r="O33" s="280"/>
+      <c r="P33" s="280"/>
+      <c r="Q33" s="280"/>
+      <c r="R33" s="280"/>
     </row>
     <row r="34" spans="12:18" x14ac:dyDescent="0.35">
       <c r="L34" s="73"/>
       <c r="M34" s="73"/>
       <c r="N34" s="73"/>
-      <c r="O34" s="248"/>
-      <c r="P34" s="248"/>
-      <c r="Q34" s="248"/>
-      <c r="R34" s="248"/>
+      <c r="O34" s="280"/>
+      <c r="P34" s="280"/>
+      <c r="Q34" s="280"/>
+      <c r="R34" s="280"/>
     </row>
     <row r="35" spans="12:18" x14ac:dyDescent="0.35">
       <c r="L35" s="73"/>
       <c r="M35" s="73"/>
       <c r="N35" s="73"/>
-      <c r="O35" s="248"/>
-      <c r="P35" s="248"/>
-      <c r="Q35" s="248"/>
-      <c r="R35" s="248"/>
+      <c r="O35" s="280"/>
+      <c r="P35" s="280"/>
+      <c r="Q35" s="280"/>
+      <c r="R35" s="280"/>
     </row>
     <row r="36" spans="12:18" x14ac:dyDescent="0.35">
       <c r="L36" s="73"/>
@@ -15812,11 +15876,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="O30:R35"/>
-    <mergeCell ref="O15:R16"/>
-    <mergeCell ref="O3:R4"/>
-    <mergeCell ref="O18:R23"/>
-    <mergeCell ref="O6:R12"/>
     <mergeCell ref="B7:M11"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="S3:S12"/>
@@ -15829,6 +15888,11 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="L5:M5"/>
+    <mergeCell ref="O30:R35"/>
+    <mergeCell ref="O15:R16"/>
+    <mergeCell ref="O3:R4"/>
+    <mergeCell ref="O18:R23"/>
+    <mergeCell ref="O6:R12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="55" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -15836,14 +15900,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36839812-F352-426E-BC42-FB52ACE5CD7F}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B3:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
+    <sheetView zoomScale="82" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -15856,57 +15920,57 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:18" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="B3" s="295" t="s">
+      <c r="B3" s="311" t="s">
         <v>154</v>
       </c>
-      <c r="C3" s="269"/>
-      <c r="D3" s="269"/>
-      <c r="E3" s="269"/>
-      <c r="F3" s="295" t="s">
+      <c r="C3" s="259"/>
+      <c r="D3" s="259"/>
+      <c r="E3" s="259"/>
+      <c r="F3" s="311" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="295"/>
-      <c r="H3" s="295"/>
-      <c r="I3" s="295"/>
-      <c r="J3" s="295"/>
-      <c r="K3" s="295"/>
-      <c r="L3" s="295"/>
-      <c r="M3" s="295"/>
-      <c r="N3" s="295"/>
-      <c r="O3" s="295"/>
-      <c r="P3" s="295"/>
-      <c r="Q3" s="295"/>
+      <c r="G3" s="311"/>
+      <c r="H3" s="311"/>
+      <c r="I3" s="311"/>
+      <c r="J3" s="311"/>
+      <c r="K3" s="311"/>
+      <c r="L3" s="311"/>
+      <c r="M3" s="311"/>
+      <c r="N3" s="311"/>
+      <c r="O3" s="311"/>
+      <c r="P3" s="311"/>
+      <c r="Q3" s="311"/>
     </row>
     <row r="4" spans="2:18" ht="19" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B4" s="299" t="s">
+      <c r="B4" s="315" t="s">
         <v>204</v>
       </c>
-      <c r="C4" s="299"/>
-      <c r="D4" s="299"/>
-      <c r="E4" s="299"/>
-      <c r="F4" s="299" t="s">
+      <c r="C4" s="315"/>
+      <c r="D4" s="315"/>
+      <c r="E4" s="315"/>
+      <c r="F4" s="315" t="s">
         <v>162</v>
       </c>
-      <c r="G4" s="299"/>
-      <c r="H4" s="299"/>
-      <c r="I4" s="299"/>
-      <c r="J4" s="299"/>
-      <c r="K4" s="299"/>
-      <c r="L4" s="299"/>
-      <c r="M4" s="299"/>
-      <c r="N4" s="299"/>
-      <c r="O4" s="299"/>
-      <c r="P4" s="299"/>
-      <c r="Q4" s="299"/>
+      <c r="G4" s="315"/>
+      <c r="H4" s="315"/>
+      <c r="I4" s="315"/>
+      <c r="J4" s="315"/>
+      <c r="K4" s="315"/>
+      <c r="L4" s="315"/>
+      <c r="M4" s="315"/>
+      <c r="N4" s="315"/>
+      <c r="O4" s="315"/>
+      <c r="P4" s="315"/>
+      <c r="Q4" s="315"/>
       <c r="R4" s="172"/>
     </row>
     <row r="5" spans="2:18" ht="14" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="318">
+      <c r="B5" s="242">
         <v>80</v>
       </c>
-      <c r="C5" s="319"/>
-      <c r="D5" s="319"/>
-      <c r="E5" s="320"/>
+      <c r="C5" s="243"/>
+      <c r="D5" s="243"/>
+      <c r="E5" s="244"/>
       <c r="F5" s="171">
         <v>6</v>
       </c>
@@ -15984,29 +16048,29 @@
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B8" s="173"/>
-      <c r="C8" s="298" t="s">
+      <c r="C8" s="314" t="s">
         <v>157</v>
       </c>
-      <c r="D8" s="298"/>
+      <c r="D8" s="314"/>
       <c r="E8" s="163"/>
       <c r="F8" s="178"/>
       <c r="G8" s="179"/>
-      <c r="H8" s="293" t="s">
+      <c r="H8" s="309" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="294"/>
+      <c r="I8" s="310"/>
       <c r="J8" s="178"/>
       <c r="K8" s="179"/>
-      <c r="L8" s="293" t="s">
+      <c r="L8" s="309" t="s">
         <v>70</v>
       </c>
-      <c r="M8" s="294"/>
+      <c r="M8" s="310"/>
       <c r="N8" s="178"/>
       <c r="O8" s="179"/>
-      <c r="P8" s="296" t="s">
+      <c r="P8" s="312" t="s">
         <v>70</v>
       </c>
-      <c r="Q8" s="297"/>
+      <c r="Q8" s="313"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B9" s="207"/>
@@ -16017,22 +16081,22 @@
         <v>20</v>
       </c>
       <c r="E9" s="165"/>
-      <c r="F9" s="302" t="s">
+      <c r="F9" s="305" t="s">
         <v>69</v>
       </c>
-      <c r="G9" s="302"/>
+      <c r="G9" s="305"/>
       <c r="H9" s="181"/>
       <c r="I9" s="182"/>
-      <c r="J9" s="302" t="s">
+      <c r="J9" s="305" t="s">
         <v>69</v>
       </c>
-      <c r="K9" s="302"/>
+      <c r="K9" s="305"/>
       <c r="L9" s="183"/>
       <c r="M9" s="183"/>
-      <c r="N9" s="302" t="s">
+      <c r="N9" s="305" t="s">
         <v>69</v>
       </c>
-      <c r="O9" s="302"/>
+      <c r="O9" s="305"/>
       <c r="P9" s="183"/>
       <c r="Q9" s="183"/>
     </row>
@@ -16063,27 +16127,27 @@
       <c r="C11" s="167"/>
       <c r="D11" s="167"/>
       <c r="E11" s="167"/>
-      <c r="F11" s="300" t="s">
+      <c r="F11" s="316" t="s">
         <v>165</v>
       </c>
-      <c r="G11" s="300"/>
-      <c r="H11" s="300"/>
-      <c r="I11" s="300"/>
-      <c r="J11" s="300"/>
-      <c r="K11" s="300"/>
-      <c r="L11" s="300"/>
-      <c r="M11" s="300"/>
-      <c r="N11" s="300"/>
-      <c r="O11" s="300"/>
-      <c r="P11" s="300"/>
-      <c r="Q11" s="300"/>
+      <c r="G11" s="316"/>
+      <c r="H11" s="316"/>
+      <c r="I11" s="316"/>
+      <c r="J11" s="316"/>
+      <c r="K11" s="316"/>
+      <c r="L11" s="316"/>
+      <c r="M11" s="316"/>
+      <c r="N11" s="316"/>
+      <c r="O11" s="316"/>
+      <c r="P11" s="316"/>
+      <c r="Q11" s="316"/>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.35">
       <c r="B12" s="168"/>
-      <c r="C12" s="298" t="s">
+      <c r="C12" s="314" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="298"/>
+      <c r="D12" s="314"/>
       <c r="E12" s="168"/>
       <c r="F12" s="191"/>
       <c r="G12" s="191"/>
@@ -16110,15 +16174,15 @@
       <c r="F13" s="191"/>
       <c r="G13" s="191"/>
       <c r="H13" s="191"/>
-      <c r="I13" s="301" t="s">
+      <c r="I13" s="304" t="s">
         <v>167</v>
       </c>
-      <c r="J13" s="301"/>
-      <c r="K13" s="301"/>
-      <c r="L13" s="301"/>
-      <c r="M13" s="301"/>
-      <c r="N13" s="301"/>
-      <c r="O13" s="301"/>
+      <c r="J13" s="304"/>
+      <c r="K13" s="304"/>
+      <c r="L13" s="304"/>
+      <c r="M13" s="304"/>
+      <c r="N13" s="304"/>
+      <c r="O13" s="304"/>
       <c r="P13" s="192"/>
       <c r="Q13" s="192"/>
     </row>
@@ -16138,9 +16202,9 @@
       <c r="J14" s="206" t="s">
         <v>168</v>
       </c>
-      <c r="K14" s="305"/>
-      <c r="L14" s="305"/>
-      <c r="M14" s="305"/>
+      <c r="K14" s="308"/>
+      <c r="L14" s="308"/>
+      <c r="M14" s="308"/>
       <c r="N14" s="206" t="s">
         <v>169</v>
       </c>
@@ -16217,13 +16281,13 @@
       <c r="G17" s="191"/>
       <c r="H17" s="191"/>
       <c r="I17" s="199"/>
-      <c r="J17" s="304" t="s">
+      <c r="J17" s="307" t="s">
         <v>166</v>
       </c>
-      <c r="K17" s="304"/>
-      <c r="L17" s="304"/>
-      <c r="M17" s="304"/>
-      <c r="N17" s="304"/>
+      <c r="K17" s="307"/>
+      <c r="L17" s="307"/>
+      <c r="M17" s="307"/>
+      <c r="N17" s="307"/>
       <c r="O17" s="200"/>
       <c r="P17" s="191"/>
       <c r="Q17" s="191"/>
@@ -16261,70 +16325,63 @@
       <c r="Q19" s="191"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B21" s="303" t="s">
+      <c r="B21" s="306" t="s">
         <v>180</v>
       </c>
-      <c r="C21" s="303"/>
-      <c r="D21" s="303"/>
-      <c r="E21" s="303"/>
-      <c r="F21" s="303"/>
-      <c r="G21" s="303"/>
-      <c r="H21" s="303"/>
-      <c r="I21" s="303"/>
-      <c r="J21" s="303"/>
-      <c r="K21" s="303"/>
-      <c r="L21" s="303"/>
-      <c r="M21" s="303"/>
-      <c r="N21" s="303"/>
-      <c r="O21" s="303"/>
-      <c r="P21" s="303"/>
-      <c r="Q21" s="303"/>
+      <c r="C21" s="306"/>
+      <c r="D21" s="306"/>
+      <c r="E21" s="306"/>
+      <c r="F21" s="306"/>
+      <c r="G21" s="306"/>
+      <c r="H21" s="306"/>
+      <c r="I21" s="306"/>
+      <c r="J21" s="306"/>
+      <c r="K21" s="306"/>
+      <c r="L21" s="306"/>
+      <c r="M21" s="306"/>
+      <c r="N21" s="306"/>
+      <c r="O21" s="306"/>
+      <c r="P21" s="306"/>
+      <c r="Q21" s="306"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B22" s="303"/>
-      <c r="C22" s="303"/>
-      <c r="D22" s="303"/>
-      <c r="E22" s="303"/>
-      <c r="F22" s="303"/>
-      <c r="G22" s="303"/>
-      <c r="H22" s="303"/>
-      <c r="I22" s="303"/>
-      <c r="J22" s="303"/>
-      <c r="K22" s="303"/>
-      <c r="L22" s="303"/>
-      <c r="M22" s="303"/>
-      <c r="N22" s="303"/>
-      <c r="O22" s="303"/>
-      <c r="P22" s="303"/>
-      <c r="Q22" s="303"/>
+      <c r="B22" s="306"/>
+      <c r="C22" s="306"/>
+      <c r="D22" s="306"/>
+      <c r="E22" s="306"/>
+      <c r="F22" s="306"/>
+      <c r="G22" s="306"/>
+      <c r="H22" s="306"/>
+      <c r="I22" s="306"/>
+      <c r="J22" s="306"/>
+      <c r="K22" s="306"/>
+      <c r="L22" s="306"/>
+      <c r="M22" s="306"/>
+      <c r="N22" s="306"/>
+      <c r="O22" s="306"/>
+      <c r="P22" s="306"/>
+      <c r="Q22" s="306"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.35">
-      <c r="B23" s="303"/>
-      <c r="C23" s="303"/>
-      <c r="D23" s="303"/>
-      <c r="E23" s="303"/>
-      <c r="F23" s="303"/>
-      <c r="G23" s="303"/>
-      <c r="H23" s="303"/>
-      <c r="I23" s="303"/>
-      <c r="J23" s="303"/>
-      <c r="K23" s="303"/>
-      <c r="L23" s="303"/>
-      <c r="M23" s="303"/>
-      <c r="N23" s="303"/>
-      <c r="O23" s="303"/>
-      <c r="P23" s="303"/>
-      <c r="Q23" s="303"/>
+      <c r="B23" s="306"/>
+      <c r="C23" s="306"/>
+      <c r="D23" s="306"/>
+      <c r="E23" s="306"/>
+      <c r="F23" s="306"/>
+      <c r="G23" s="306"/>
+      <c r="H23" s="306"/>
+      <c r="I23" s="306"/>
+      <c r="J23" s="306"/>
+      <c r="K23" s="306"/>
+      <c r="L23" s="306"/>
+      <c r="M23" s="306"/>
+      <c r="N23" s="306"/>
+      <c r="O23" s="306"/>
+      <c r="P23" s="306"/>
+      <c r="Q23" s="306"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="I13:O13"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="B21:Q23"/>
-    <mergeCell ref="J17:N17"/>
-    <mergeCell ref="K14:M14"/>
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="F3:Q3"/>
     <mergeCell ref="H8:I8"/>
@@ -16335,13 +16392,20 @@
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="F4:Q4"/>
     <mergeCell ref="F11:Q11"/>
+    <mergeCell ref="I13:O13"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="B21:Q23"/>
+    <mergeCell ref="J17:N17"/>
+    <mergeCell ref="K14:M14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8FBCA58-0396-46E3-8F1B-89C0F6C32117}">
   <dimension ref="B2:X20"/>
   <sheetViews>
@@ -16351,290 +16415,290 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="8.7265625" style="313"/>
-    <col min="3" max="12" width="5.6328125" style="313" customWidth="1"/>
-    <col min="13" max="24" width="4.6328125" style="313" customWidth="1"/>
-    <col min="25" max="16384" width="8.7265625" style="313"/>
+    <col min="1" max="2" width="8.7265625" style="241"/>
+    <col min="3" max="12" width="5.6328125" style="241" customWidth="1"/>
+    <col min="13" max="24" width="4.6328125" style="241" customWidth="1"/>
+    <col min="25" max="16384" width="8.7265625" style="241"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C2" s="315" t="s">
+      <c r="C2" s="317" t="s">
         <v>206</v>
       </c>
-      <c r="D2" s="315"/>
-      <c r="E2" s="315"/>
-      <c r="F2" s="315"/>
-      <c r="G2" s="315"/>
-      <c r="H2" s="315"/>
-      <c r="I2" s="315"/>
-      <c r="J2" s="315"/>
-      <c r="K2" s="315"/>
-      <c r="L2" s="315"/>
-      <c r="M2" s="315" t="s">
+      <c r="D2" s="317"/>
+      <c r="E2" s="317"/>
+      <c r="F2" s="317"/>
+      <c r="G2" s="317"/>
+      <c r="H2" s="317"/>
+      <c r="I2" s="317"/>
+      <c r="J2" s="317"/>
+      <c r="K2" s="317"/>
+      <c r="L2" s="317"/>
+      <c r="M2" s="317" t="s">
         <v>207</v>
       </c>
-      <c r="N2" s="315"/>
-      <c r="O2" s="315"/>
-      <c r="P2" s="315"/>
-      <c r="Q2" s="315"/>
-      <c r="R2" s="315"/>
-      <c r="S2" s="315"/>
-      <c r="T2" s="315"/>
-      <c r="U2" s="315"/>
-      <c r="V2" s="315"/>
-      <c r="W2" s="315"/>
-      <c r="X2" s="315"/>
+      <c r="N2" s="317"/>
+      <c r="O2" s="317"/>
+      <c r="P2" s="317"/>
+      <c r="Q2" s="317"/>
+      <c r="R2" s="317"/>
+      <c r="S2" s="317"/>
+      <c r="T2" s="317"/>
+      <c r="U2" s="317"/>
+      <c r="V2" s="317"/>
+      <c r="W2" s="317"/>
+      <c r="X2" s="317"/>
     </row>
     <row r="3" spans="2:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="313" t="s">
+      <c r="B3" s="241" t="s">
         <v>205</v>
       </c>
-      <c r="C3" s="306">
+      <c r="C3" s="234">
         <v>1</v>
       </c>
-      <c r="D3" s="307">
+      <c r="D3" s="235">
         <v>2</v>
       </c>
-      <c r="E3" s="307">
+      <c r="E3" s="235">
         <v>3</v>
       </c>
-      <c r="F3" s="307">
+      <c r="F3" s="235">
         <v>4</v>
       </c>
-      <c r="G3" s="307">
+      <c r="G3" s="235">
         <v>5</v>
       </c>
-      <c r="H3" s="307">
+      <c r="H3" s="235">
         <v>6</v>
       </c>
-      <c r="I3" s="307">
+      <c r="I3" s="235">
         <v>7</v>
       </c>
-      <c r="J3" s="307">
+      <c r="J3" s="235">
         <v>8</v>
       </c>
-      <c r="K3" s="307">
+      <c r="K3" s="235">
         <v>9</v>
       </c>
-      <c r="L3" s="308">
+      <c r="L3" s="236">
         <v>10</v>
       </c>
-      <c r="M3" s="309">
+      <c r="M3" s="237">
         <v>11</v>
       </c>
-      <c r="N3" s="310">
+      <c r="N3" s="238">
         <v>12</v>
       </c>
-      <c r="O3" s="311">
+      <c r="O3" s="239">
         <v>13</v>
       </c>
-      <c r="P3" s="312">
+      <c r="P3" s="240">
         <v>14</v>
       </c>
-      <c r="Q3" s="309">
+      <c r="Q3" s="237">
         <v>15</v>
       </c>
-      <c r="R3" s="310">
+      <c r="R3" s="238">
         <v>16</v>
       </c>
-      <c r="S3" s="311">
+      <c r="S3" s="239">
         <v>17</v>
       </c>
-      <c r="T3" s="312">
+      <c r="T3" s="240">
         <v>18</v>
       </c>
-      <c r="U3" s="309">
+      <c r="U3" s="237">
         <v>19</v>
       </c>
-      <c r="V3" s="310">
+      <c r="V3" s="238">
         <v>20</v>
       </c>
-      <c r="W3" s="311">
+      <c r="W3" s="239">
         <v>21</v>
       </c>
-      <c r="X3" s="310">
+      <c r="X3" s="238">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="C4" s="316" t="s">
+      <c r="C4" s="319" t="s">
         <v>221</v>
       </c>
-      <c r="D4" s="316"/>
-      <c r="E4" s="316"/>
-      <c r="F4" s="316"/>
-      <c r="G4" s="316"/>
-      <c r="H4" s="316"/>
-      <c r="I4" s="316"/>
-      <c r="J4" s="316"/>
-      <c r="K4" s="316"/>
-      <c r="L4" s="316"/>
-      <c r="M4" s="317" t="s">
+      <c r="D4" s="319"/>
+      <c r="E4" s="319"/>
+      <c r="F4" s="319"/>
+      <c r="G4" s="319"/>
+      <c r="H4" s="319"/>
+      <c r="I4" s="319"/>
+      <c r="J4" s="319"/>
+      <c r="K4" s="319"/>
+      <c r="L4" s="319"/>
+      <c r="M4" s="320" t="s">
         <v>222</v>
       </c>
-      <c r="N4" s="317"/>
-      <c r="O4" s="317"/>
-      <c r="P4" s="317"/>
-      <c r="Q4" s="317"/>
-      <c r="R4" s="317"/>
-      <c r="S4" s="317"/>
-      <c r="T4" s="317"/>
-      <c r="U4" s="317"/>
-      <c r="V4" s="317"/>
-      <c r="W4" s="317"/>
-      <c r="X4" s="317"/>
+      <c r="N4" s="320"/>
+      <c r="O4" s="320"/>
+      <c r="P4" s="320"/>
+      <c r="Q4" s="320"/>
+      <c r="R4" s="320"/>
+      <c r="S4" s="320"/>
+      <c r="T4" s="320"/>
+      <c r="U4" s="320"/>
+      <c r="V4" s="320"/>
+      <c r="W4" s="320"/>
+      <c r="X4" s="320"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="D5" s="313" t="s">
+      <c r="D5" s="241" t="s">
         <v>211</v>
       </c>
-      <c r="M5" s="313" t="s">
+      <c r="M5" s="241" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="E6" s="313" t="s">
+      <c r="E6" s="241" t="s">
         <v>209</v>
       </c>
-      <c r="N6" s="313" t="s">
+      <c r="N6" s="241" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="F7" s="313" t="s">
+      <c r="F7" s="241" t="s">
         <v>210</v>
       </c>
-      <c r="P7" s="313" t="s">
+      <c r="P7" s="241" t="s">
         <v>226</v>
       </c>
-      <c r="R7" s="313">
+      <c r="R7" s="241">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="G8" s="313" t="s">
+      <c r="G8" s="241" t="s">
         <v>216</v>
       </c>
-      <c r="I8" s="313" t="s">
+      <c r="I8" s="241" t="s">
         <v>218</v>
       </c>
-      <c r="P8" s="313" t="s">
+      <c r="P8" s="241" t="s">
         <v>226</v>
       </c>
-      <c r="R8" s="313">
+      <c r="R8" s="241">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="F9" s="313" t="s">
+      <c r="F9" s="241" t="s">
         <v>220</v>
       </c>
-      <c r="P9" s="313" t="s">
+      <c r="P9" s="241" t="s">
         <v>226</v>
       </c>
-      <c r="R9" s="313">
+      <c r="R9" s="241">
         <v>40</v>
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="G10" s="313" t="s">
+      <c r="G10" s="241" t="s">
         <v>216</v>
       </c>
-      <c r="I10" s="313" t="s">
+      <c r="I10" s="241" t="s">
         <v>218</v>
       </c>
-      <c r="P10" s="313" t="s">
+      <c r="P10" s="241" t="s">
         <v>226</v>
       </c>
-      <c r="R10" s="313">
+      <c r="R10" s="241">
         <v>45</v>
       </c>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="E11" s="313" t="s">
+      <c r="E11" s="241" t="s">
         <v>212</v>
       </c>
-      <c r="P11" s="313" t="s">
+      <c r="P11" s="241" t="s">
         <v>226</v>
       </c>
-      <c r="R11" s="313">
+      <c r="R11" s="241">
         <v>55</v>
       </c>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="F12" s="313" t="s">
+      <c r="F12" s="241" t="s">
         <v>215</v>
       </c>
-      <c r="P12" s="313" t="s">
+      <c r="P12" s="241" t="s">
         <v>226</v>
       </c>
-      <c r="R12" s="313">
+      <c r="R12" s="241">
         <v>70</v>
       </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="G13" s="314" t="s">
+      <c r="G13" s="318" t="s">
         <v>216</v>
       </c>
-      <c r="H13" s="314"/>
-      <c r="I13" s="313" t="s">
+      <c r="H13" s="318"/>
+      <c r="I13" s="241" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="G14" s="314" t="s">
+      <c r="G14" s="318" t="s">
         <v>216</v>
       </c>
-      <c r="H14" s="314"/>
-      <c r="I14" s="313" t="s">
+      <c r="H14" s="318"/>
+      <c r="I14" s="241" t="s">
         <v>219</v>
       </c>
-      <c r="O14" s="313" t="s">
+      <c r="O14" s="241" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="F15" s="313" t="s">
+      <c r="F15" s="241" t="s">
         <v>214</v>
       </c>
-      <c r="P15" s="313" t="s">
+      <c r="P15" s="241" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.35">
-      <c r="G16" s="313" t="s">
+      <c r="G16" s="241" t="s">
         <v>217</v>
       </c>
-      <c r="I16" s="313" t="s">
+      <c r="I16" s="241" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="17" spans="6:9" x14ac:dyDescent="0.35">
-      <c r="G17" s="313" t="s">
+      <c r="G17" s="241" t="s">
         <v>217</v>
       </c>
-      <c r="I17" s="313" t="s">
+      <c r="I17" s="241" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="18" spans="6:9" x14ac:dyDescent="0.35">
-      <c r="F18" s="313" t="s">
+      <c r="F18" s="241" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="19" spans="6:9" x14ac:dyDescent="0.35">
-      <c r="G19" s="313" t="s">
+      <c r="G19" s="241" t="s">
         <v>217</v>
       </c>
-      <c r="I19" s="313" t="s">
+      <c r="I19" s="241" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="20" spans="6:9" x14ac:dyDescent="0.35">
-      <c r="G20" s="313" t="s">
+      <c r="G20" s="241" t="s">
         <v>217</v>
       </c>
-      <c r="I20" s="313" t="s">
+      <c r="I20" s="241" t="s">
         <v>219</v>
       </c>
     </row>

</xml_diff>